<commit_message>
fix percentage in xlsx
</commit_message>
<xml_diff>
--- a/data/climate-data.xlsx
+++ b/data/climate-data.xlsx
@@ -42,7 +42,7 @@
     <t>Län</t>
   </si>
   <si>
-    <t>KPI1: Förändringstakt andel laddbara bilar</t>
+    <t>KPI1: Förändringstakt andel laddbara bilar (%)</t>
   </si>
   <si>
     <t>KPI2: Klimatplan länk</t>
@@ -1761,7 +1761,7 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>0.04848084661477944</v>
+        <v>4.8</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>0.07043528444297543</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -1795,7 +1795,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>0.06084937111254478</v>
+        <v>6.1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
@@ -1812,7 +1812,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>0.05164583397223511</v>
+        <v>5.2</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1829,7 +1829,7 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>0.06815959442215519</v>
+        <v>6.8</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -1880,7 +1880,7 @@
         <v>141</v>
       </c>
       <c r="C2">
-        <v>0.03093897466485612</v>
+        <v>3.1</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -1897,7 +1897,7 @@
         <v>141</v>
       </c>
       <c r="C3">
-        <v>0.06399848551346246</v>
+        <v>6.4</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -1914,7 +1914,7 @@
         <v>141</v>
       </c>
       <c r="C4">
-        <v>0.05515919356681476</v>
+        <v>5.5</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -1931,7 +1931,7 @@
         <v>141</v>
       </c>
       <c r="C5">
-        <v>0.0377335161585747</v>
+        <v>3.8</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1948,7 +1948,7 @@
         <v>141</v>
       </c>
       <c r="C6">
-        <v>0.06042340263846041</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -1965,7 +1965,7 @@
         <v>141</v>
       </c>
       <c r="C7">
-        <v>0.06810241001823615</v>
+        <v>6.8</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -1982,7 +1982,7 @@
         <v>141</v>
       </c>
       <c r="C8">
-        <v>0.04653639904835516</v>
+        <v>4.7</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -1999,7 +1999,7 @@
         <v>141</v>
       </c>
       <c r="C9">
-        <v>0.05977188843177565</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -2016,7 +2016,7 @@
         <v>141</v>
       </c>
       <c r="C10">
-        <v>0.05512807341840541</v>
+        <v>5.5</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>142</v>
@@ -2033,7 +2033,7 @@
         <v>141</v>
       </c>
       <c r="C11">
-        <v>0.07563750342085944</v>
+        <v>7.6</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -2050,7 +2050,7 @@
         <v>141</v>
       </c>
       <c r="C12">
-        <v>0.08428524112409641</v>
+        <v>8.4</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -2067,7 +2067,7 @@
         <v>141</v>
       </c>
       <c r="C13">
-        <v>0.06055208372530786</v>
+        <v>6.1</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>143</v>
@@ -2084,7 +2084,7 @@
         <v>141</v>
       </c>
       <c r="C14">
-        <v>0.03895314311746793</v>
+        <v>3.9</v>
       </c>
       <c r="D14" t="s">
         <v>144</v>
@@ -2101,7 +2101,7 @@
         <v>141</v>
       </c>
       <c r="C15">
-        <v>0.03892288872701098</v>
+        <v>3.9</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>145</v>
@@ -2153,7 +2153,7 @@
         <v>179</v>
       </c>
       <c r="C2">
-        <v>0.06736436245177074</v>
+        <v>6.7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>180</v>
@@ -2170,7 +2170,7 @@
         <v>179</v>
       </c>
       <c r="C3">
-        <v>0.08181108702724145</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>181</v>
@@ -2187,7 +2187,7 @@
         <v>179</v>
       </c>
       <c r="C4">
-        <v>0.04753188216316283</v>
+        <v>4.8</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -2204,7 +2204,7 @@
         <v>179</v>
       </c>
       <c r="C5">
-        <v>0.08439202799046437</v>
+        <v>8.4</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>182</v>
@@ -2221,7 +2221,7 @@
         <v>179</v>
       </c>
       <c r="C6">
-        <v>0.07524982951593966</v>
+        <v>7.5</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -2238,7 +2238,7 @@
         <v>179</v>
       </c>
       <c r="C7">
-        <v>0.03301981588753814</v>
+        <v>3.3</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -2255,7 +2255,7 @@
         <v>179</v>
       </c>
       <c r="C8">
-        <v>0.04610376188397754</v>
+        <v>4.6</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -2272,7 +2272,7 @@
         <v>179</v>
       </c>
       <c r="C9">
-        <v>0.09283559648488335</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -2289,7 +2289,7 @@
         <v>179</v>
       </c>
       <c r="C10">
-        <v>0.08962152539618798</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>183</v>
@@ -2306,7 +2306,7 @@
         <v>179</v>
       </c>
       <c r="C11">
-        <v>0.07491986404593716</v>
+        <v>7.5</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>184</v>
@@ -2323,7 +2323,7 @@
         <v>179</v>
       </c>
       <c r="C12">
-        <v>0.0663886080143808</v>
+        <v>6.6</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -2340,7 +2340,7 @@
         <v>179</v>
       </c>
       <c r="C13">
-        <v>0.06578047080306838</v>
+        <v>6.6</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>185</v>
@@ -2357,7 +2357,7 @@
         <v>179</v>
       </c>
       <c r="C14">
-        <v>0.07039356467764031</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
@@ -2374,7 +2374,7 @@
         <v>179</v>
       </c>
       <c r="C15">
-        <v>0.06332638122639997</v>
+        <v>6.3</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -2391,7 +2391,7 @@
         <v>179</v>
       </c>
       <c r="C16">
-        <v>0.02923280316780341</v>
+        <v>2.9</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>186</v>
@@ -2408,7 +2408,7 @@
         <v>179</v>
       </c>
       <c r="C17">
-        <v>0.07115187962866446</v>
+        <v>7.1</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
@@ -2425,7 +2425,7 @@
         <v>179</v>
       </c>
       <c r="C18">
-        <v>0.05433778381448846</v>
+        <v>5.4</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>187</v>
@@ -2442,7 +2442,7 @@
         <v>179</v>
       </c>
       <c r="C19">
-        <v>0.06374565186486536</v>
+        <v>6.4</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -2459,7 +2459,7 @@
         <v>179</v>
       </c>
       <c r="C20">
-        <v>0.06431778429002259</v>
+        <v>6.4</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>188</v>
@@ -2476,7 +2476,7 @@
         <v>179</v>
       </c>
       <c r="C21">
-        <v>0.07218936624257806</v>
+        <v>7.2</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>189</v>
@@ -2493,7 +2493,7 @@
         <v>179</v>
       </c>
       <c r="C22">
-        <v>0.08030708204415621</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -2510,7 +2510,7 @@
         <v>179</v>
       </c>
       <c r="C23">
-        <v>0.06443229869056234</v>
+        <v>6.4</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
@@ -2527,7 +2527,7 @@
         <v>179</v>
       </c>
       <c r="C24">
-        <v>0.1035858311647119</v>
+        <v>10.4</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>190</v>
@@ -2544,7 +2544,7 @@
         <v>179</v>
       </c>
       <c r="C25">
-        <v>0.07376566900343701</v>
+        <v>7.4</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -2561,7 +2561,7 @@
         <v>179</v>
       </c>
       <c r="C26">
-        <v>0.06302096256173736</v>
+        <v>6.3</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>191</v>
@@ -2578,7 +2578,7 @@
         <v>179</v>
       </c>
       <c r="C27">
-        <v>0.07286294683214967</v>
+        <v>7.3</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>192</v>
@@ -2595,7 +2595,7 @@
         <v>179</v>
       </c>
       <c r="C28">
-        <v>0.05901942847303372</v>
+        <v>5.9</v>
       </c>
       <c r="D28" t="s">
         <v>14</v>
@@ -2612,7 +2612,7 @@
         <v>179</v>
       </c>
       <c r="C29">
-        <v>0.05677580065707093</v>
+        <v>5.7</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>193</v>
@@ -2629,7 +2629,7 @@
         <v>179</v>
       </c>
       <c r="C30">
-        <v>0.07304337752578609</v>
+        <v>7.3</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -2646,7 +2646,7 @@
         <v>179</v>
       </c>
       <c r="C31">
-        <v>0.07535474375627423</v>
+        <v>7.5</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>194</v>
@@ -2663,7 +2663,7 @@
         <v>179</v>
       </c>
       <c r="C32">
-        <v>0.06034983087158206</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
         <v>14</v>
@@ -2680,7 +2680,7 @@
         <v>179</v>
       </c>
       <c r="C33">
-        <v>0.06255937990183585</v>
+        <v>6.3</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
@@ -2697,7 +2697,7 @@
         <v>179</v>
       </c>
       <c r="C34">
-        <v>0.05603986261884942</v>
+        <v>5.6</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
@@ -2761,7 +2761,7 @@
         <v>221</v>
       </c>
       <c r="C2">
-        <v>0.0765374063331129</v>
+        <v>7.7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>222</v>
@@ -2778,7 +2778,7 @@
         <v>221</v>
       </c>
       <c r="C3">
-        <v>0.08854171329681397</v>
+        <v>8.9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>223</v>
@@ -2795,7 +2795,7 @@
         <v>221</v>
       </c>
       <c r="C4">
-        <v>0.07938435305447579</v>
+        <v>7.9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>224</v>
@@ -2812,7 +2812,7 @@
         <v>221</v>
       </c>
       <c r="C5">
-        <v>0.09712375610874407</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>225</v>
@@ -2829,7 +2829,7 @@
         <v>221</v>
       </c>
       <c r="C6">
-        <v>0.08209290709034771</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>226</v>
@@ -2846,7 +2846,7 @@
         <v>221</v>
       </c>
       <c r="C7">
-        <v>0.09099684043102808</v>
+        <v>9.1</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>227</v>
@@ -2863,7 +2863,7 @@
         <v>221</v>
       </c>
       <c r="C8">
-        <v>0.06869420554248744</v>
+        <v>6.9</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>228</v>
@@ -2880,7 +2880,7 @@
         <v>221</v>
       </c>
       <c r="C9">
-        <v>0.06410773867813389</v>
+        <v>6.4</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>229</v>
@@ -2897,7 +2897,7 @@
         <v>221</v>
       </c>
       <c r="C10">
-        <v>0.0714780271065529</v>
+        <v>7.1</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -2914,7 +2914,7 @@
         <v>221</v>
       </c>
       <c r="C11">
-        <v>0.06666338594504451</v>
+        <v>6.7</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>230</v>
@@ -2931,7 +2931,7 @@
         <v>221</v>
       </c>
       <c r="C12">
-        <v>0.08346914882009587</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>231</v>
@@ -2948,7 +2948,7 @@
         <v>221</v>
       </c>
       <c r="C13">
-        <v>0.08185558879772066</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>232</v>
@@ -2965,7 +2965,7 @@
         <v>221</v>
       </c>
       <c r="C14">
-        <v>0.06462434911498847</v>
+        <v>6.5</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
@@ -2982,7 +2982,7 @@
         <v>221</v>
       </c>
       <c r="C15">
-        <v>0.08723877258687399</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -2999,7 +2999,7 @@
         <v>221</v>
       </c>
       <c r="C16">
-        <v>0.104575205822188</v>
+        <v>10.5</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>233</v>
@@ -3016,7 +3016,7 @@
         <v>221</v>
       </c>
       <c r="C17">
-        <v>0.09384386828142256</v>
+        <v>9.4</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>234</v>
@@ -3033,7 +3033,7 @@
         <v>221</v>
       </c>
       <c r="C18">
-        <v>0.09141670840433368</v>
+        <v>9.1</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>235</v>
@@ -3050,7 +3050,7 @@
         <v>221</v>
       </c>
       <c r="C19">
-        <v>0.07725999060272203</v>
+        <v>7.7</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -3067,7 +3067,7 @@
         <v>221</v>
       </c>
       <c r="C20">
-        <v>0.0938950133601959</v>
+        <v>9.4</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -3084,7 +3084,7 @@
         <v>221</v>
       </c>
       <c r="C21">
-        <v>0.1128371249859808</v>
+        <v>11.3</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -3101,7 +3101,7 @@
         <v>221</v>
       </c>
       <c r="C22">
-        <v>0.09063096588168804</v>
+        <v>9.1</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>236</v>
@@ -3118,7 +3118,7 @@
         <v>221</v>
       </c>
       <c r="C23">
-        <v>0.08638179745773583</v>
+        <v>8.6</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>237</v>
@@ -3135,7 +3135,7 @@
         <v>221</v>
       </c>
       <c r="C24">
-        <v>0.0854422793529529</v>
+        <v>8.5</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>238</v>
@@ -3152,7 +3152,7 @@
         <v>221</v>
       </c>
       <c r="C25">
-        <v>0.06271267374618099</v>
+        <v>6.3</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>239</v>
@@ -3169,7 +3169,7 @@
         <v>221</v>
       </c>
       <c r="C26">
-        <v>0.08230968541458143</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>240</v>
@@ -3186,7 +3186,7 @@
         <v>221</v>
       </c>
       <c r="C27">
-        <v>0.07270911712824234</v>
+        <v>7.3</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>241</v>
@@ -3255,7 +3255,7 @@
         <v>251</v>
       </c>
       <c r="C2">
-        <v>0.06369487159665729</v>
+        <v>6.4</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -3272,7 +3272,7 @@
         <v>251</v>
       </c>
       <c r="C3">
-        <v>0.07878057228987029</v>
+        <v>7.9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>252</v>
@@ -3289,7 +3289,7 @@
         <v>251</v>
       </c>
       <c r="C4">
-        <v>0.0666231467111337</v>
+        <v>6.7</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>253</v>
@@ -3306,7 +3306,7 @@
         <v>251</v>
       </c>
       <c r="C5">
-        <v>0.06918068895426813</v>
+        <v>6.9</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -3323,7 +3323,7 @@
         <v>251</v>
       </c>
       <c r="C6">
-        <v>0.06586217303091861</v>
+        <v>6.6</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>254</v>
@@ -3340,7 +3340,7 @@
         <v>251</v>
       </c>
       <c r="C7">
-        <v>0.06806819251218851</v>
+        <v>6.8</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -3357,7 +3357,7 @@
         <v>251</v>
       </c>
       <c r="C8">
-        <v>0.07440516778597488</v>
+        <v>7.4</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>255</v>
@@ -3374,7 +3374,7 @@
         <v>251</v>
       </c>
       <c r="C9">
-        <v>0.06106344520813337</v>
+        <v>6.1</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>256</v>
@@ -3391,7 +3391,7 @@
         <v>251</v>
       </c>
       <c r="C10">
-        <v>0.07994518335545023</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -3445,7 +3445,7 @@
         <v>265</v>
       </c>
       <c r="C2">
-        <v>0.06332352673472733</v>
+        <v>6.3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>266</v>
@@ -3462,7 +3462,7 @@
         <v>265</v>
       </c>
       <c r="C3">
-        <v>0.08039150618547321</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -3479,7 +3479,7 @@
         <v>265</v>
       </c>
       <c r="C4">
-        <v>0.09554434701457269</v>
+        <v>9.6</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -3496,7 +3496,7 @@
         <v>265</v>
       </c>
       <c r="C5">
-        <v>0.07250361450039211</v>
+        <v>7.3</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -3513,7 +3513,7 @@
         <v>265</v>
       </c>
       <c r="C6">
-        <v>0.08058750519372183</v>
+        <v>8.1</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>267</v>
@@ -3530,7 +3530,7 @@
         <v>265</v>
       </c>
       <c r="C7">
-        <v>0.07604799399367819</v>
+        <v>7.6</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>268</v>
@@ -3547,7 +3547,7 @@
         <v>265</v>
       </c>
       <c r="C8">
-        <v>0.07283663159432276</v>
+        <v>7.3</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>269</v>
@@ -3564,7 +3564,7 @@
         <v>265</v>
       </c>
       <c r="C9">
-        <v>0.05800046961784733</v>
+        <v>5.8</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -3617,7 +3617,7 @@
         <v>286</v>
       </c>
       <c r="C2">
-        <v>0.06355871073210718</v>
+        <v>6.4</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -3634,7 +3634,7 @@
         <v>286</v>
       </c>
       <c r="C3">
-        <v>0.04019340700337465</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>287</v>
@@ -3651,7 +3651,7 @@
         <v>286</v>
       </c>
       <c r="C4">
-        <v>0.04892038514354501</v>
+        <v>4.9</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -3668,7 +3668,7 @@
         <v>286</v>
       </c>
       <c r="C5">
-        <v>0.06211116863729343</v>
+        <v>6.2</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -3685,7 +3685,7 @@
         <v>286</v>
       </c>
       <c r="C6">
-        <v>0.0712436857988574</v>
+        <v>7.1</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -3702,7 +3702,7 @@
         <v>286</v>
       </c>
       <c r="C7">
-        <v>0.05845845875138749</v>
+        <v>5.8</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -3719,7 +3719,7 @@
         <v>286</v>
       </c>
       <c r="C8">
-        <v>0.07085106106291314</v>
+        <v>7.1</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>288</v>
@@ -3736,7 +3736,7 @@
         <v>286</v>
       </c>
       <c r="C9">
-        <v>0.07597880990069575</v>
+        <v>7.6</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -3753,7 +3753,7 @@
         <v>286</v>
       </c>
       <c r="C10">
-        <v>0.04682916517497189</v>
+        <v>4.7</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -3770,7 +3770,7 @@
         <v>286</v>
       </c>
       <c r="C11">
-        <v>0.05265839985775768</v>
+        <v>5.3</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>289</v>
@@ -3787,7 +3787,7 @@
         <v>286</v>
       </c>
       <c r="C12">
-        <v>0.04989308453351107</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -3804,7 +3804,7 @@
         <v>286</v>
       </c>
       <c r="C13">
-        <v>0.05632201864964928</v>
+        <v>5.6</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -3821,7 +3821,7 @@
         <v>286</v>
       </c>
       <c r="C14">
-        <v>0.04838530752286105</v>
+        <v>4.8</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
@@ -3838,7 +3838,7 @@
         <v>286</v>
       </c>
       <c r="C15">
-        <v>0.02410397443604743</v>
+        <v>2.4</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>290</v>
@@ -3855,7 +3855,7 @@
         <v>286</v>
       </c>
       <c r="C16">
-        <v>0.06325904988850772</v>
+        <v>6.3</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -3872,7 +3872,7 @@
         <v>286</v>
       </c>
       <c r="C17">
-        <v>0.06686873815265758</v>
+        <v>6.7</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>291</v>
@@ -3926,7 +3926,7 @@
         <v>307</v>
       </c>
       <c r="C2">
-        <v>0.08463110138607759</v>
+        <v>8.5</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -3943,7 +3943,7 @@
         <v>307</v>
       </c>
       <c r="C3">
-        <v>0.06209325396825398</v>
+        <v>6.2</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>308</v>
@@ -3960,7 +3960,7 @@
         <v>307</v>
       </c>
       <c r="C4">
-        <v>0.08172730299016158</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -3977,7 +3977,7 @@
         <v>307</v>
       </c>
       <c r="C5">
-        <v>0.100632611114207</v>
+        <v>10.1</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -3994,7 +3994,7 @@
         <v>307</v>
       </c>
       <c r="C6">
-        <v>0.1022547543607607</v>
+        <v>10.2</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -4011,7 +4011,7 @@
         <v>307</v>
       </c>
       <c r="C7">
-        <v>0.03897844908714474</v>
+        <v>3.9</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -4028,7 +4028,7 @@
         <v>307</v>
       </c>
       <c r="C8">
-        <v>0.05899824729406899</v>
+        <v>5.9</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>309</v>
@@ -4045,7 +4045,7 @@
         <v>307</v>
       </c>
       <c r="C9">
-        <v>0.01785714285714285</v>
+        <v>1.8</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -4062,7 +4062,7 @@
         <v>307</v>
       </c>
       <c r="C10">
-        <v>0.03745039682539682</v>
+        <v>3.7</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -4079,7 +4079,7 @@
         <v>307</v>
       </c>
       <c r="C11">
-        <v>0.08293148872104252</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -4096,7 +4096,7 @@
         <v>307</v>
       </c>
       <c r="C12">
-        <v>0.05728046158686402</v>
+        <v>5.7</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -4113,7 +4113,7 @@
         <v>307</v>
       </c>
       <c r="C13">
-        <v>0.07965942787371361</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -4130,7 +4130,7 @@
         <v>307</v>
       </c>
       <c r="C14">
-        <v>0.07299210060480074</v>
+        <v>7.3</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>310</v>
@@ -4147,7 +4147,7 @@
         <v>307</v>
       </c>
       <c r="C15">
-        <v>0.06312012057143704</v>
+        <v>6.3</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -4164,7 +4164,7 @@
         <v>307</v>
       </c>
       <c r="C16">
-        <v>0.08220670884696615</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>311</v>
@@ -4217,7 +4217,7 @@
         <v>319</v>
       </c>
       <c r="C2">
-        <v>0.05920741158752741</v>
+        <v>5.9</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -4234,7 +4234,7 @@
         <v>319</v>
       </c>
       <c r="C3">
-        <v>0.07530256376717442</v>
+        <v>7.5</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -4251,7 +4251,7 @@
         <v>319</v>
       </c>
       <c r="C4">
-        <v>0.07240952545804048</v>
+        <v>7.2</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -4268,7 +4268,7 @@
         <v>319</v>
       </c>
       <c r="C5">
-        <v>0.06560283314932576</v>
+        <v>6.6</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>320</v>
@@ -4285,7 +4285,7 @@
         <v>319</v>
       </c>
       <c r="C6">
-        <v>0.08132507376740258</v>
+        <v>8.1</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>321</v>
@@ -4302,7 +4302,7 @@
         <v>319</v>
       </c>
       <c r="C7">
-        <v>0.06229187253517578</v>
+        <v>6.2</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -4319,7 +4319,7 @@
         <v>319</v>
       </c>
       <c r="C8">
-        <v>0.06104495238337404</v>
+        <v>6.1</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -4370,7 +4370,7 @@
         <v>332</v>
       </c>
       <c r="C2">
-        <v>0.08467082063406652</v>
+        <v>8.5</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -4387,7 +4387,7 @@
         <v>332</v>
       </c>
       <c r="C3">
-        <v>0.08341704594444087</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -4404,7 +4404,7 @@
         <v>332</v>
       </c>
       <c r="C4">
-        <v>0.07679359962426027</v>
+        <v>7.7</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -4421,7 +4421,7 @@
         <v>332</v>
       </c>
       <c r="C5">
-        <v>0.08123456469983636</v>
+        <v>8.1</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -4438,7 +4438,7 @@
         <v>332</v>
       </c>
       <c r="C6">
-        <v>0.08162202620088913</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>333</v>
@@ -4455,7 +4455,7 @@
         <v>332</v>
       </c>
       <c r="C7">
-        <v>0.07642102938412798</v>
+        <v>7.6</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>334</v>
@@ -4472,7 +4472,7 @@
         <v>332</v>
       </c>
       <c r="C8">
-        <v>0.06924026936717274</v>
+        <v>6.9</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>335</v>
@@ -4489,7 +4489,7 @@
         <v>332</v>
       </c>
       <c r="C9">
-        <v>0.05952735943117683</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -4506,7 +4506,7 @@
         <v>332</v>
       </c>
       <c r="C10">
-        <v>0.0670495271242888</v>
+        <v>6.7</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -4523,7 +4523,7 @@
         <v>332</v>
       </c>
       <c r="C11">
-        <v>0.07658767428480581</v>
+        <v>7.7</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -4575,7 +4575,7 @@
         <v>385</v>
       </c>
       <c r="C2">
-        <v>0.08968315530502405</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>386</v>
@@ -4592,7 +4592,7 @@
         <v>385</v>
       </c>
       <c r="C3">
-        <v>0.07797206459456414</v>
+        <v>7.8</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -4609,7 +4609,7 @@
         <v>385</v>
       </c>
       <c r="C4">
-        <v>0.07675163702380684</v>
+        <v>7.7</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -4626,7 +4626,7 @@
         <v>385</v>
       </c>
       <c r="C5">
-        <v>0.08220843541623976</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -4643,7 +4643,7 @@
         <v>385</v>
       </c>
       <c r="C6">
-        <v>0.0817404698595658</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -4660,7 +4660,7 @@
         <v>385</v>
       </c>
       <c r="C7">
-        <v>0.07628487606585559</v>
+        <v>7.6</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -4677,7 +4677,7 @@
         <v>385</v>
       </c>
       <c r="C8">
-        <v>0.08320347022902196</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>387</v>
@@ -4694,7 +4694,7 @@
         <v>385</v>
       </c>
       <c r="C9">
-        <v>0.07614390539753603</v>
+        <v>7.6</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -4711,7 +4711,7 @@
         <v>385</v>
       </c>
       <c r="C10">
-        <v>0.07740142887033657</v>
+        <v>7.7</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>388</v>
@@ -4728,7 +4728,7 @@
         <v>385</v>
       </c>
       <c r="C11">
-        <v>0.07013240027920878</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>389</v>
@@ -4745,7 +4745,7 @@
         <v>385</v>
       </c>
       <c r="C12">
-        <v>0.05543863728702094</v>
+        <v>5.5</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -4762,7 +4762,7 @@
         <v>385</v>
       </c>
       <c r="C13">
-        <v>0.07763704818023739</v>
+        <v>7.8</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>390</v>
@@ -4779,7 +4779,7 @@
         <v>385</v>
       </c>
       <c r="C14">
-        <v>0.08931430314467403</v>
+        <v>8.9</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
@@ -4796,7 +4796,7 @@
         <v>385</v>
       </c>
       <c r="C15">
-        <v>0.07425641056499373</v>
+        <v>7.4</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -4813,7 +4813,7 @@
         <v>385</v>
       </c>
       <c r="C16">
-        <v>0.0749761798547102</v>
+        <v>7.5</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -4830,7 +4830,7 @@
         <v>385</v>
       </c>
       <c r="C17">
-        <v>0.06330140371433526</v>
+        <v>6.3</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
@@ -4847,7 +4847,7 @@
         <v>385</v>
       </c>
       <c r="C18">
-        <v>0.05532045814186719</v>
+        <v>5.5</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -4864,7 +4864,7 @@
         <v>385</v>
       </c>
       <c r="C19">
-        <v>0.06578073314142187</v>
+        <v>6.6</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -4881,7 +4881,7 @@
         <v>385</v>
       </c>
       <c r="C20">
-        <v>0.0465946550369637</v>
+        <v>4.7</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -4898,7 +4898,7 @@
         <v>385</v>
       </c>
       <c r="C21">
-        <v>0.0701876136565409</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -4915,7 +4915,7 @@
         <v>385</v>
       </c>
       <c r="C22">
-        <v>0.05503121325281628</v>
+        <v>5.5</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
@@ -4932,7 +4932,7 @@
         <v>385</v>
       </c>
       <c r="C23">
-        <v>0.05547856641444567</v>
+        <v>5.5</v>
       </c>
       <c r="D23" t="s">
         <v>14</v>
@@ -4949,7 +4949,7 @@
         <v>385</v>
       </c>
       <c r="C24">
-        <v>0.07145206664468494</v>
+        <v>7.1</v>
       </c>
       <c r="D24" t="s">
         <v>14</v>
@@ -4966,7 +4966,7 @@
         <v>385</v>
       </c>
       <c r="C25">
-        <v>0.05887189376903463</v>
+        <v>5.9</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -4983,7 +4983,7 @@
         <v>385</v>
       </c>
       <c r="C26">
-        <v>0.07129087547601946</v>
+        <v>7.1</v>
       </c>
       <c r="D26" t="s">
         <v>14</v>
@@ -5000,7 +5000,7 @@
         <v>385</v>
       </c>
       <c r="C27">
-        <v>0.07421594247781289</v>
+        <v>7.4</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>391</v>
@@ -5017,7 +5017,7 @@
         <v>385</v>
       </c>
       <c r="C28">
-        <v>0.08063160922382689</v>
+        <v>8.1</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>392</v>
@@ -5034,7 +5034,7 @@
         <v>385</v>
       </c>
       <c r="C29">
-        <v>0.05796873288707401</v>
+        <v>5.8</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>393</v>
@@ -5051,7 +5051,7 @@
         <v>385</v>
       </c>
       <c r="C30">
-        <v>0.07900324612193288</v>
+        <v>7.9</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -5068,7 +5068,7 @@
         <v>385</v>
       </c>
       <c r="C31">
-        <v>0.05767007673304146</v>
+        <v>5.8</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>394</v>
@@ -5085,7 +5085,7 @@
         <v>385</v>
       </c>
       <c r="C32">
-        <v>0.08139978209978142</v>
+        <v>8.1</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>395</v>
@@ -5102,7 +5102,7 @@
         <v>385</v>
       </c>
       <c r="C33">
-        <v>0.08264060483353733</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>396</v>
@@ -5119,7 +5119,7 @@
         <v>385</v>
       </c>
       <c r="C34">
-        <v>0.06459040640158112</v>
+        <v>6.5</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
@@ -5136,7 +5136,7 @@
         <v>385</v>
       </c>
       <c r="C35">
-        <v>0.06799621860120332</v>
+        <v>6.8</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
@@ -5153,7 +5153,7 @@
         <v>385</v>
       </c>
       <c r="C36">
-        <v>0.08432083248236984</v>
+        <v>8.4</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>397</v>
@@ -5170,7 +5170,7 @@
         <v>385</v>
       </c>
       <c r="C37">
-        <v>0.07956377478869936</v>
+        <v>8</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>398</v>
@@ -5187,7 +5187,7 @@
         <v>385</v>
       </c>
       <c r="C38">
-        <v>0.06902258111591543</v>
+        <v>6.9</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>399</v>
@@ -5204,7 +5204,7 @@
         <v>385</v>
       </c>
       <c r="C39">
-        <v>0.07693129067052229</v>
+        <v>7.7</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -5221,7 +5221,7 @@
         <v>385</v>
       </c>
       <c r="C40">
-        <v>0.05692912903302751</v>
+        <v>5.7</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>400</v>
@@ -5238,7 +5238,7 @@
         <v>385</v>
       </c>
       <c r="C41">
-        <v>0.0688514886498573</v>
+        <v>6.9</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>401</v>
@@ -5255,7 +5255,7 @@
         <v>385</v>
       </c>
       <c r="C42">
-        <v>0.05423459046932939</v>
+        <v>5.4</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
@@ -5272,7 +5272,7 @@
         <v>385</v>
       </c>
       <c r="C43">
-        <v>0.04722049692122803</v>
+        <v>4.7</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>402</v>
@@ -5289,7 +5289,7 @@
         <v>385</v>
       </c>
       <c r="C44">
-        <v>0.05800223919314745</v>
+        <v>5.8</v>
       </c>
       <c r="D44" t="s">
         <v>14</v>
@@ -5306,7 +5306,7 @@
         <v>385</v>
       </c>
       <c r="C45">
-        <v>0.06323238491530066</v>
+        <v>6.3</v>
       </c>
       <c r="D45" t="s">
         <v>14</v>
@@ -5323,7 +5323,7 @@
         <v>385</v>
       </c>
       <c r="C46">
-        <v>0.06307028341146065</v>
+        <v>6.3</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>403</v>
@@ -5340,7 +5340,7 @@
         <v>385</v>
       </c>
       <c r="C47">
-        <v>0.06008614401892933</v>
+        <v>6</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>404</v>
@@ -5357,7 +5357,7 @@
         <v>385</v>
       </c>
       <c r="C48">
-        <v>0.0739392676549078</v>
+        <v>7.4</v>
       </c>
       <c r="D48" t="s">
         <v>14</v>
@@ -5374,7 +5374,7 @@
         <v>385</v>
       </c>
       <c r="C49">
-        <v>0.06286312320785492</v>
+        <v>6.3</v>
       </c>
       <c r="D49" t="s">
         <v>14</v>
@@ -5391,7 +5391,7 @@
         <v>385</v>
       </c>
       <c r="C50">
-        <v>0.06034227676939238</v>
+        <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>405</v>
@@ -5460,7 +5460,7 @@
         <v>30</v>
       </c>
       <c r="C2">
-        <v>0.06892917836138833</v>
+        <v>6.9</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -5477,7 +5477,7 @@
         <v>30</v>
       </c>
       <c r="C3">
-        <v>0.06841056261265648</v>
+        <v>6.8</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -5494,7 +5494,7 @@
         <v>30</v>
       </c>
       <c r="C4">
-        <v>0.07890026754016323</v>
+        <v>7.9</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -5511,7 +5511,7 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>0.07429398622338473</v>
+        <v>7.4</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -5528,7 +5528,7 @@
         <v>30</v>
       </c>
       <c r="C6">
-        <v>0.06738883066063339</v>
+        <v>6.7</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -5545,7 +5545,7 @@
         <v>30</v>
       </c>
       <c r="C7">
-        <v>0.06616169766656933</v>
+        <v>6.6</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -5562,7 +5562,7 @@
         <v>30</v>
       </c>
       <c r="C8">
-        <v>0.05055099741651649</v>
+        <v>5.1</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -5579,7 +5579,7 @@
         <v>30</v>
       </c>
       <c r="C9">
-        <v>0.07060793700347996</v>
+        <v>7.1</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -5596,7 +5596,7 @@
         <v>30</v>
       </c>
       <c r="C10">
-        <v>0.07610466370177843</v>
+        <v>7.6</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -5613,7 +5613,7 @@
         <v>30</v>
       </c>
       <c r="C11">
-        <v>0.07338052290831522</v>
+        <v>7.3</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>32</v>
@@ -5630,7 +5630,7 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>0.06932502973026199</v>
+        <v>6.9</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>33</v>
@@ -5647,7 +5647,7 @@
         <v>30</v>
       </c>
       <c r="C13">
-        <v>0.0856519990705167</v>
+        <v>8.6</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -5664,7 +5664,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>0.07311584698923557</v>
+        <v>7.3</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>34</v>
@@ -5681,7 +5681,7 @@
         <v>30</v>
       </c>
       <c r="C15">
-        <v>0.0635646911666385</v>
+        <v>6.4</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>35</v>
@@ -5698,7 +5698,7 @@
         <v>30</v>
       </c>
       <c r="C16">
-        <v>0.06305293399226239</v>
+        <v>6.3</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -5751,7 +5751,7 @@
         <v>418</v>
       </c>
       <c r="C2">
-        <v>0.08794698058806111</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>419</v>
@@ -5768,7 +5768,7 @@
         <v>418</v>
       </c>
       <c r="C3">
-        <v>0.07003482854357825</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -5785,7 +5785,7 @@
         <v>418</v>
       </c>
       <c r="C4">
-        <v>0.06981823238845705</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -5802,7 +5802,7 @@
         <v>418</v>
       </c>
       <c r="C5">
-        <v>0.05963444012440951</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>420</v>
@@ -5819,7 +5819,7 @@
         <v>418</v>
       </c>
       <c r="C6">
-        <v>0.02273222109920967</v>
+        <v>2.3</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -5836,7 +5836,7 @@
         <v>418</v>
       </c>
       <c r="C7">
-        <v>0.06161332505413199</v>
+        <v>6.2</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -5853,7 +5853,7 @@
         <v>418</v>
       </c>
       <c r="C8">
-        <v>0.06838985391189982</v>
+        <v>6.8</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>421</v>
@@ -5870,7 +5870,7 @@
         <v>418</v>
       </c>
       <c r="C9">
-        <v>0.07362269170409613</v>
+        <v>7.4</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -5887,7 +5887,7 @@
         <v>418</v>
       </c>
       <c r="C10">
-        <v>0.08155194210851513</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>422</v>
@@ -5904,7 +5904,7 @@
         <v>418</v>
       </c>
       <c r="C11">
-        <v>0.06741071126861059</v>
+        <v>6.7</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>423</v>
@@ -5921,7 +5921,7 @@
         <v>418</v>
       </c>
       <c r="C12">
-        <v>0.07832037383929294</v>
+        <v>7.8</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -5938,7 +5938,7 @@
         <v>418</v>
       </c>
       <c r="C13">
-        <v>0.06278204096372671</v>
+        <v>6.3</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -5992,7 +5992,7 @@
         <v>437</v>
       </c>
       <c r="C2">
-        <v>0.07059067095543468</v>
+        <v>7.1</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -6009,7 +6009,7 @@
         <v>437</v>
       </c>
       <c r="C3">
-        <v>0.06084149828047423</v>
+        <v>6.1</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -6026,7 +6026,7 @@
         <v>437</v>
       </c>
       <c r="C4">
-        <v>0.07656595537898003</v>
+        <v>7.7</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -6043,7 +6043,7 @@
         <v>437</v>
       </c>
       <c r="C5">
-        <v>0.06825478883054295</v>
+        <v>6.8</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -6060,7 +6060,7 @@
         <v>437</v>
       </c>
       <c r="C6">
-        <v>0.07781171707064609</v>
+        <v>7.8</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>438</v>
@@ -6077,7 +6077,7 @@
         <v>437</v>
       </c>
       <c r="C7">
-        <v>0.06605029780674963</v>
+        <v>6.6</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -6094,7 +6094,7 @@
         <v>437</v>
       </c>
       <c r="C8">
-        <v>0.06314947707714712</v>
+        <v>6.3</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -6111,7 +6111,7 @@
         <v>437</v>
       </c>
       <c r="C9">
-        <v>0.07817576996138308</v>
+        <v>7.8</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>439</v>
@@ -6128,7 +6128,7 @@
         <v>437</v>
       </c>
       <c r="C10">
-        <v>0.06870100704679302</v>
+        <v>6.9</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -6145,7 +6145,7 @@
         <v>437</v>
       </c>
       <c r="C11">
-        <v>0.07926457547430098</v>
+        <v>7.9</v>
       </c>
       <c r="D11" t="s">
         <v>440</v>
@@ -6162,7 +6162,7 @@
         <v>437</v>
       </c>
       <c r="C12">
-        <v>0.06052378665984954</v>
+        <v>6.1</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -6179,7 +6179,7 @@
         <v>437</v>
       </c>
       <c r="C13">
-        <v>0.08264479516777649</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -6196,7 +6196,7 @@
         <v>437</v>
       </c>
       <c r="C14">
-        <v>0.08345160061637033</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>441</v>
@@ -6248,7 +6248,7 @@
         <v>37</v>
       </c>
       <c r="C2">
-        <v>0.06565393185052729</v>
+        <v>6.6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>38</v>
@@ -6298,7 +6298,7 @@
         <v>49</v>
       </c>
       <c r="C2">
-        <v>0.06545456857956859</v>
+        <v>6.5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>50</v>
@@ -6315,7 +6315,7 @@
         <v>49</v>
       </c>
       <c r="C3">
-        <v>0.05644063397675594</v>
+        <v>5.6</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -6332,7 +6332,7 @@
         <v>49</v>
       </c>
       <c r="C4">
-        <v>0.06444507425844531</v>
+        <v>6.4</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -6349,7 +6349,7 @@
         <v>49</v>
       </c>
       <c r="C5">
-        <v>0.07440985234652259</v>
+        <v>7.4</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -6366,7 +6366,7 @@
         <v>49</v>
       </c>
       <c r="C6">
-        <v>0.03798298146198286</v>
+        <v>3.8</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -6383,7 +6383,7 @@
         <v>49</v>
       </c>
       <c r="C7">
-        <v>0.06100513406216745</v>
+        <v>6.1</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>51</v>
@@ -6400,7 +6400,7 @@
         <v>49</v>
       </c>
       <c r="C8">
-        <v>0.04678196704923624</v>
+        <v>4.7</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -6417,7 +6417,7 @@
         <v>49</v>
       </c>
       <c r="C9">
-        <v>0.06065326724571211</v>
+        <v>6.1</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -6434,7 +6434,7 @@
         <v>49</v>
       </c>
       <c r="C10">
-        <v>0.0455480925238178</v>
+        <v>4.6</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>52</v>
@@ -6451,7 +6451,7 @@
         <v>49</v>
       </c>
       <c r="C11">
-        <v>0.0678566222826768</v>
+        <v>6.8</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>53</v>
@@ -6504,7 +6504,7 @@
         <v>60</v>
       </c>
       <c r="C2">
-        <v>0.07418984128266769</v>
+        <v>7.4</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -6521,7 +6521,7 @@
         <v>60</v>
       </c>
       <c r="C3">
-        <v>0.06722475368112807</v>
+        <v>6.7</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>61</v>
@@ -6538,7 +6538,7 @@
         <v>60</v>
       </c>
       <c r="C4">
-        <v>0.06060519070905029</v>
+        <v>6.1</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -6555,7 +6555,7 @@
         <v>60</v>
       </c>
       <c r="C5">
-        <v>0.06571854867722164</v>
+        <v>6.6</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -6572,7 +6572,7 @@
         <v>60</v>
       </c>
       <c r="C6">
-        <v>0.07092690309096124</v>
+        <v>7.1</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -6589,7 +6589,7 @@
         <v>60</v>
       </c>
       <c r="C7">
-        <v>0.08085876171896782</v>
+        <v>8.1</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -6639,7 +6639,7 @@
         <v>70</v>
       </c>
       <c r="C2">
-        <v>0.05061831836025384</v>
+        <v>5.1</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -6656,7 +6656,7 @@
         <v>70</v>
       </c>
       <c r="C3">
-        <v>0.07074002442836098</v>
+        <v>7.1</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -6673,7 +6673,7 @@
         <v>70</v>
       </c>
       <c r="C4">
-        <v>0.0929713150065911</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -6690,7 +6690,7 @@
         <v>70</v>
       </c>
       <c r="C5">
-        <v>0.02445954370121613</v>
+        <v>2.4</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -6707,7 +6707,7 @@
         <v>70</v>
       </c>
       <c r="C6">
-        <v>0.07488338094349196</v>
+        <v>7.5</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -6724,7 +6724,7 @@
         <v>70</v>
       </c>
       <c r="C7">
-        <v>0.08054448179106087</v>
+        <v>8.1</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>71</v>
@@ -6741,7 +6741,7 @@
         <v>70</v>
       </c>
       <c r="C8">
-        <v>0.04683688671842642</v>
+        <v>4.7</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -6758,7 +6758,7 @@
         <v>70</v>
       </c>
       <c r="C9">
-        <v>0.0601379340337174</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>72</v>
@@ -6809,7 +6809,7 @@
         <v>86</v>
       </c>
       <c r="C2">
-        <v>0.08172603954176877</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>87</v>
@@ -6826,7 +6826,7 @@
         <v>86</v>
       </c>
       <c r="C3">
-        <v>0.08002508252892905</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -6843,7 +6843,7 @@
         <v>86</v>
       </c>
       <c r="C4">
-        <v>0.07766504804834294</v>
+        <v>7.8</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>88</v>
@@ -6860,7 +6860,7 @@
         <v>86</v>
       </c>
       <c r="C5">
-        <v>0.0777714944006703</v>
+        <v>7.8</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>89</v>
@@ -6877,7 +6877,7 @@
         <v>86</v>
       </c>
       <c r="C6">
-        <v>0.07401713658926597</v>
+        <v>7.4</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>90</v>
@@ -6894,7 +6894,7 @@
         <v>86</v>
       </c>
       <c r="C7">
-        <v>0.07424964946747815</v>
+        <v>7.4</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>91</v>
@@ -6911,7 +6911,7 @@
         <v>86</v>
       </c>
       <c r="C8">
-        <v>0.06056694861443521</v>
+        <v>6.1</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>92</v>
@@ -6928,7 +6928,7 @@
         <v>86</v>
       </c>
       <c r="C9">
-        <v>0.06298481115583551</v>
+        <v>6.3</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>93</v>
@@ -6945,7 +6945,7 @@
         <v>86</v>
       </c>
       <c r="C10">
-        <v>0.05898399875619671</v>
+        <v>5.9</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>94</v>
@@ -6962,7 +6962,7 @@
         <v>86</v>
       </c>
       <c r="C11">
-        <v>0.06408601095112333</v>
+        <v>6.4</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
@@ -6979,7 +6979,7 @@
         <v>86</v>
       </c>
       <c r="C12">
-        <v>0.06388548378969891</v>
+        <v>6.4</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -6996,7 +6996,7 @@
         <v>86</v>
       </c>
       <c r="C13">
-        <v>0.05980457047951254</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -7013,7 +7013,7 @@
         <v>86</v>
       </c>
       <c r="C14">
-        <v>0.07134073785204356</v>
+        <v>7.1</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>95</v>
@@ -7071,7 +7071,7 @@
         <v>108</v>
       </c>
       <c r="C2">
-        <v>0.04783248420472141</v>
+        <v>4.8</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -7088,7 +7088,7 @@
         <v>108</v>
       </c>
       <c r="C3">
-        <v>0.06160773789915487</v>
+        <v>6.2</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -7105,7 +7105,7 @@
         <v>108</v>
       </c>
       <c r="C4">
-        <v>0.07017005932384283</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -7122,7 +7122,7 @@
         <v>108</v>
       </c>
       <c r="C5">
-        <v>0.04809009227386411</v>
+        <v>4.8</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -7139,7 +7139,7 @@
         <v>108</v>
       </c>
       <c r="C6">
-        <v>0.06519788486631281</v>
+        <v>6.5</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -7156,7 +7156,7 @@
         <v>108</v>
       </c>
       <c r="C7">
-        <v>0.05328922529549373</v>
+        <v>5.3</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -7173,7 +7173,7 @@
         <v>108</v>
       </c>
       <c r="C8">
-        <v>0.05652943773447291</v>
+        <v>5.7</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>109</v>
@@ -7190,7 +7190,7 @@
         <v>108</v>
       </c>
       <c r="C9">
-        <v>0.06330461512168965</v>
+        <v>6.3</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -7207,7 +7207,7 @@
         <v>108</v>
       </c>
       <c r="C10">
-        <v>0.05955514770451151</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -7224,7 +7224,7 @@
         <v>108</v>
       </c>
       <c r="C11">
-        <v>0.0577145209931009</v>
+        <v>5.8</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>110</v>
@@ -7241,7 +7241,7 @@
         <v>108</v>
       </c>
       <c r="C12">
-        <v>0.05544340720325495</v>
+        <v>5.5</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -7258,7 +7258,7 @@
         <v>108</v>
       </c>
       <c r="C13">
-        <v>0.07454415068255339</v>
+        <v>7.5</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>111</v>
@@ -7310,7 +7310,7 @@
         <v>120</v>
       </c>
       <c r="C2">
-        <v>0.06993258639548683</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>121</v>
@@ -7327,7 +7327,7 @@
         <v>120</v>
       </c>
       <c r="C3">
-        <v>0.07914745524942891</v>
+        <v>7.9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>122</v>
@@ -7344,7 +7344,7 @@
         <v>120</v>
       </c>
       <c r="C4">
-        <v>0.0596922019546265</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>123</v>
@@ -7361,7 +7361,7 @@
         <v>120</v>
       </c>
       <c r="C5">
-        <v>0.08469554797215427</v>
+        <v>8.5</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -7378,7 +7378,7 @@
         <v>120</v>
       </c>
       <c r="C6">
-        <v>0.07081995808507044</v>
+        <v>7.1</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>124</v>
@@ -7395,7 +7395,7 @@
         <v>120</v>
       </c>
       <c r="C7">
-        <v>0.06568561484182897</v>
+        <v>6.6</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -7412,7 +7412,7 @@
         <v>120</v>
       </c>
       <c r="C8">
-        <v>0.06986862307772726</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>125</v>
@@ -7429,7 +7429,7 @@
         <v>120</v>
       </c>
       <c r="C9">
-        <v>0.05866861261891208</v>
+        <v>5.9</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Update climate plan data
</commit_message>
<xml_diff>
--- a/data/climate-data.xlsx
+++ b/data/climate-data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="455">
   <si>
     <t>Kommun</t>
   </si>
@@ -69,7 +69,7 @@
     <t>Blekinge län</t>
   </si>
   <si>
-    <t>/data/climatePlans/Olofström_Handlingsplan för klimat och energi.pdf</t>
+    <t>/data/climatePlans/Olofstr%C3%B6m_Handlingsplan%20f%C3%B6r%20klimat%20och%20energi.pdf</t>
   </si>
   <si>
     <t>https://www.karlskrona.se/globalassets/kommun-och-politik/sa-arbetar-vi-med/hallbarhetsprogram_karlskrona_kommun_210517.pdf</t>
@@ -129,7 +129,7 @@
     <t>Dalarnas län</t>
   </si>
   <si>
-    <t>public/data/climatePlans/Vansbro_Energi- och klimatplan.pdf</t>
+    <t>/data/climatePlans/Vansbro_Energi och klimatplan.pdf</t>
   </si>
   <si>
     <t>https://www.falun.se/download/18.7eb630aa16a59ef02cf6d5b8/1557238559519/energi_och_klimatprogram_2013_webb.pdf</t>
@@ -222,6 +222,9 @@
     <t>https://www.halmstad.se/download/18.1ab5eabc17db948137827c20/1643015898074/Plan-for-energi-och-klimat-anpassad.pdf</t>
   </si>
   <si>
+    <t>https://kungsbacka.se/download/18.5c06deb5186a19d6e5c23920/1678800987979/Klimatstrategi%202022.pdf</t>
+  </si>
+  <si>
     <t>Ragunda</t>
   </si>
   <si>
@@ -411,7 +414,7 @@
     <t>https://www.almhult.se/stadsutvecklingplanering/strategiskplanering/miljoplan2030.1994.html</t>
   </si>
   <si>
-    <t>https://vaxjo.se/download/18.5975292f184b921397ce18b0/1670511806917/V%C3%A4xj%C3%B6%20kommun%20klimatkontrakt%202022.pdf</t>
+    <t>https://vaxjo.se/download/18.58d9f57a16d9ce07d02dd012/1571219603597/H%C3%A5llbarhetsprogrammet%20H%C3%A5llbara%20V%C3%A4xj%C3%B6%202030_antaget%20av%20KF.pdf</t>
   </si>
   <si>
     <t>https://www.ljungby.se/globalassets/dokument-och-innehall/miljo-och-klimat/hallbar-utveckling/klimat--och-energiplan_digital-lasning.pdf</t>
@@ -465,6 +468,9 @@
     <t>http://www3.alvsbyn.se/styrdoc/Styrdok.nsf/Formnytt.xsp?documentId=D921B3CF75BFCEFFC125868C00428F58&amp;action=openDocument</t>
   </si>
   <si>
+    <t>https://www.pitea.se/contentassets/9c4b5902081c401a985a37bee096f992/handlingsplan-miljo-klimat-och-energi.pdf?t=638201013076470932</t>
+  </si>
+  <si>
     <t>https://www.boden.se/kommunen/organisation-och-styrning/viktiga-styrdokument</t>
   </si>
   <si>
@@ -582,6 +588,9 @@
     <t>https://staffanstorp.se/wp-content/uploads/2021/11/6-17-miljoplan.pdf</t>
   </si>
   <si>
+    <t>https://burlov.se/download/18.1c32a37617b4106947ea55dd/1629702323432/Milj%C3%B6program%202030.pdf</t>
+  </si>
+  <si>
     <t>https://vellinge.se/siteassets/boende-miljo-och-trafik/pdf/vellinge_program-for-hallbar-utveckling_2021_slutlig-version.pdf</t>
   </si>
   <si>
@@ -591,6 +600,9 @@
     <t>https://www.svedala.se/contentassets/ff83c3d46b1e464cb1c0a32030db2256/hallbarhetsstrategi-svedala-kommun-2021-tillganglighetsanpassad-webb.pdf</t>
   </si>
   <si>
+    <t>https://www.skurup.se/36987</t>
+  </si>
+  <si>
     <t>https://www.sjobo.se/bygga-bo-och-miljo/hallbarhet-miljo-och-natur/lokala-miljomal.html</t>
   </si>
   <si>
@@ -600,12 +612,18 @@
     <t>https://www.osby.se/bygga-bo--miljo/natur-och-hallbarhet/klimatarbete.html</t>
   </si>
   <si>
+    <t>https://www.perstorp.se/download/18.6ee8abfe17bedf7491a2a38/1643719465669/Klimat-%20och%20energiprogram.pdf</t>
+  </si>
+  <si>
     <t>https://www.klippan.se/download/18.1b71982c18529d736e712692/1673968304934/Ha%CC%8Allbarhetsstrategi.pdf?query=klimat</t>
   </si>
   <si>
     <t>https://medborgarportalen.astorp.se/welcome-sv/namnder-styrelser/bygg-och-miljonamndens-arbetsutskott/bygg-och-miljonamndens-arbetsutskott/agenda/02-verksamhetsplan-for-strategiskt-arbetsmiljoarbete-2022pdf?downloadMode=open</t>
   </si>
   <si>
+    <t>https://static1.squarespace.com/static/5dd54ca29c9179411df12b85/t/6390ab4da16fc858ade542fa/1670425421810/Viable-Cities-Klimatkontrakt-Malmo-FINAL.pdf</t>
+  </si>
+  <si>
     <t>https://lund.se/download/18.2899fac318093d2b72817dd7/1666783006521/Lunds%20kommuns%20program%20f%C3%B6r%20ekologisk%20h%C3%A5llbar%20utveckling%202021-2030.pdf</t>
   </si>
   <si>
@@ -744,6 +762,12 @@
     <t>https://start.stockholm/globalassets/start/om-stockholms-stad/politik-och-demokrati/styrdokument/klimathandlingsplan-2020-2023.pdf</t>
   </si>
   <si>
+    <t>https://www.sodertalje.se/globalassets/styrande-dokument/miljo--och-klimatstrategi-2022-2030_antagen-av-kf.pdf</t>
+  </si>
+  <si>
+    <t>https://static1.squarespace.com/static/5dd54ca29c9179411df12b85/t/6390ab5d7343c933175d7561/1670425438238/Viable-Cities-Klimatkontrakt-Nacka-FINAL.pdf</t>
+  </si>
+  <si>
     <t>https://www.solna.se/download/18.5002ae1016ed574744199bd/1596180205909/Klimatstrategi_2019.pdf</t>
   </si>
   <si>
@@ -906,6 +930,9 @@
     <t>https://sunne.se/globalassets/dokument/7.-kommun-och-politik/kommunfakta/forfattningssamling/bygga-bo-och-miljo/miljostrategi-2018-2030-kf-2018-05-07.pdf</t>
   </si>
   <si>
+    <t>https://static1.squarespace.com/static/5dd54ca29c9179411df12b85/t/6390ab2cd964d14c504ed938/1670425390573/Viable-Cities-Klimatkontrakt-Karlstad-FINAL.pdf</t>
+  </si>
+  <si>
     <t>https://www.hagfors.se/undersidor/miljo-och-energi/miljomal-och-hallbarhetsarbete/miljoverenskommelsen-2022-2025.html</t>
   </si>
   <si>
@@ -969,7 +996,7 @@
     <t>https://www.umea.se/byggaboochmiljo/samhallsutvecklingochhallbarhet/klimatmiljoochhallbarhet/strategisktmiljoarbete/miljomal/programochplanerformiljomalen.4.4c35eecf182e743a9224108.html</t>
   </si>
   <si>
-    <t>https://skelleftea.se/skelleftea-vaxer/skelleftea-vaxer/en-hallbar-plats</t>
+    <t>https://static1.squarespace.com/static/5dd54ca29c9179411df12b85/t/6390ab7bb0c4e669d7aee685/1670425468289/Viable-Cities-Klimatkontrakt-Skelleftea-FINAL.pdf</t>
   </si>
   <si>
     <t>Ånge</t>
@@ -1002,6 +1029,9 @@
     <t>https://www.kramfors.se/download/18.22be0c416e405e2b6c7c6cb/1575389653000/Kramfors-kommun-Program-f%C3%B6r-ekologisk-h%C3%A5llbarhet-2020-2031.pdf</t>
   </si>
   <si>
+    <t>https://www.ornskoldsvik.se/download/18.54f6f67017d0e18071cc1e0b/1645188359669/Klimatstrategi%202021-2026.pdf</t>
+  </si>
+  <si>
     <t>Skinnskatteberg</t>
   </si>
   <si>
@@ -1044,6 +1074,9 @@
     <t>https://www.sala.se/resources/files/_Nystruktur/Styrdokument/06%20Planer/Energi-%20och%20klimatstrategi%20Sala%20kommun%202020-2030%20med%20utblick%20mot%202045.pdf</t>
   </si>
   <si>
+    <t>https://www.arboga.se/download/18.626a0440182c91de14a1a5/1661251036439/Energi-%20och%20klimatstrategi%202009%20kf.pdf</t>
+  </si>
+  <si>
     <t>Härryda</t>
   </si>
   <si>
@@ -1197,6 +1230,9 @@
     <t>https://www.harryda.se/download/18.c0a4fce181800179101eedd/1660123092984/Energi-%20och%20klimatplan.pdf</t>
   </si>
   <si>
+    <t>https://www.orust.se/download/18.1c4985fe183bfdb97a25a9/1665396992481/Energi-%20och%20klimatstrategi%202017-2030%20Orust.pdf</t>
+  </si>
+  <si>
     <t>https://www.sotenas.se/download/18.31f128a417e9f4ede9dc1776/1644237756609/H%C3%A5llbarhetsstrategi%202030%20antagen%20210218%20m%C3%A5l%202022.pdf</t>
   </si>
   <si>
@@ -1209,9 +1245,6 @@
     <t>https://www.ale.se/download/18.2dcf200c178661e144145a5/1617883886384/Energi-%20och%20klimatstrategi%202030.pdf</t>
   </si>
   <si>
-    <t>https://herrljunga.se/kommun-och-politik/kommuninformation/klimat-2030.html</t>
-  </si>
-  <si>
     <t>https://vara.se/innehall/2022/02/Milj%C3%B6strategi-2021-2030-antagen-av-KF-2021-10-04-%C2%A7-89.pdf</t>
   </si>
   <si>
@@ -1245,10 +1278,16 @@
     <t>https://www.amal.se/media/467592/antagen-energi-och-klimatstrategi-20171027.pdf</t>
   </si>
   <si>
+    <t>https://static1.squarespace.com/static/5dd54ca29c9179411df12b85/t/6390ab5329d52f430f6fe71a/1670425427707/Viable-Cities-Klimatkontrakt-Mariestad-FINAL.pdf</t>
+  </si>
+  <si>
     <t>https://skara.se/download/18.a9ae3d177427fab272ada/1611824198185/milj%C3%B6strategi%202017web.pdf</t>
   </si>
   <si>
     <t>https://skovde.se/globalassets/energi--och-klimatplanen_webb.pdf</t>
+  </si>
+  <si>
+    <t>https://hjo.se/globalassets/dokument/styrdokument/ovrigt/hallbarhetsstrategi-for-hjo-kommun.pdf</t>
   </si>
   <si>
     <t>https://www.falkoping.se/download/18.1adde54a17861a73b1e11aae/1626330208751/Klimatstrategi%202021-2030.pdf</t>
@@ -1874,10 +1913,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C2">
         <v>3.1</v>
@@ -1891,10 +1930,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C3">
         <v>6.4</v>
@@ -1908,10 +1947,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C4">
         <v>5.5</v>
@@ -1925,10 +1964,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C5">
         <v>3.8</v>
@@ -1942,10 +1981,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -1959,10 +1998,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C7">
         <v>6.8</v>
@@ -1976,10 +2015,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C8">
         <v>4.7</v>
@@ -1993,10 +2032,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -2010,16 +2049,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C10">
         <v>5.5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E10">
         <v>2021</v>
@@ -2027,10 +2066,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C11">
         <v>7.6</v>
@@ -2044,33 +2083,33 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C12">
         <v>8.4</v>
       </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
+      <c r="D12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12">
+        <v>2019</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C13">
         <v>6.1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E13">
         <v>2018</v>
@@ -2078,16 +2117,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C14">
         <v>3.9</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E14">
         <v>2012</v>
@@ -2095,16 +2134,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C15">
         <v>3.9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E15">
         <v>2015</v>
@@ -2113,8 +2152,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1"/>
-    <hyperlink ref="D13" r:id="rId2"/>
-    <hyperlink ref="D15" r:id="rId3"/>
+    <hyperlink ref="D12" r:id="rId2"/>
+    <hyperlink ref="D13" r:id="rId3"/>
+    <hyperlink ref="D15" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2147,16 +2187,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C2">
         <v>6.7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E2">
         <v>2022</v>
@@ -2164,16 +2204,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C3">
         <v>8.199999999999999</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E3">
         <v>2022</v>
@@ -2181,33 +2221,33 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C4">
         <v>4.8</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+      <c r="D4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4">
+        <v>2020</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C5">
         <v>8.4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E5">
         <v>2021</v>
@@ -2215,10 +2255,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C6">
         <v>7.5</v>
@@ -2232,10 +2272,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C7">
         <v>3.3</v>
@@ -2249,10 +2289,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C8">
         <v>4.6</v>
@@ -2266,10 +2306,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C9">
         <v>9.300000000000001</v>
@@ -2283,16 +2323,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E10">
         <v>2020</v>
@@ -2300,16 +2340,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C11">
         <v>7.5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E11">
         <v>2021</v>
@@ -2317,33 +2357,33 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C12">
         <v>6.6</v>
       </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
+      <c r="D12" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12">
+        <v>2017</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C13">
         <v>6.6</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E13">
         <v>2022</v>
@@ -2351,10 +2391,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B14" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C14">
         <v>7</v>
@@ -2368,10 +2408,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C15">
         <v>6.3</v>
@@ -2385,27 +2425,27 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C16">
         <v>2.9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
+        <v>190</v>
+      </c>
+      <c r="E16">
+        <v>2019</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C17">
         <v>7.1</v>
@@ -2419,16 +2459,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C18">
         <v>5.4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E18">
         <v>2021</v>
@@ -2436,33 +2476,33 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C19">
         <v>6.4</v>
       </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
+      <c r="D19" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E19">
+        <v>2021</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C20">
         <v>6.4</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="E20" t="s">
         <v>14</v>
@@ -2470,16 +2510,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C21">
         <v>7.2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E21">
         <v>2022</v>
@@ -2487,10 +2527,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C22">
         <v>8</v>
@@ -2504,33 +2544,33 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C23">
         <v>6.4</v>
       </c>
-      <c r="D23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" t="s">
-        <v>14</v>
+      <c r="D23" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E23">
+        <v>2022</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C24">
         <v>10.4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E24">
         <v>2021</v>
@@ -2538,10 +2578,10 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C25">
         <v>7.4</v>
@@ -2555,16 +2595,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B26" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C26">
         <v>6.3</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="E26">
         <v>2018</v>
@@ -2572,16 +2612,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B27" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C27">
         <v>7.3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E27">
         <v>2015</v>
@@ -2589,10 +2629,10 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B28" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C28">
         <v>5.9</v>
@@ -2606,16 +2646,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C29">
         <v>5.7</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="E29">
         <v>2020</v>
@@ -2623,10 +2663,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C30">
         <v>7.3</v>
@@ -2640,16 +2680,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C31">
         <v>7.5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E31">
         <v>2023</v>
@@ -2657,10 +2697,10 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B32" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -2674,10 +2714,10 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B33" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C33">
         <v>6.3</v>
@@ -2691,10 +2731,10 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B34" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C34">
         <v>5.6</v>
@@ -2710,19 +2750,23 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D10" r:id="rId4"/>
-    <hyperlink ref="D11" r:id="rId5"/>
-    <hyperlink ref="D13" r:id="rId6"/>
-    <hyperlink ref="D16" r:id="rId7"/>
-    <hyperlink ref="D18" r:id="rId8"/>
-    <hyperlink ref="D20" r:id="rId9"/>
-    <hyperlink ref="D21" r:id="rId10"/>
-    <hyperlink ref="D24" r:id="rId11"/>
-    <hyperlink ref="D26" r:id="rId12"/>
-    <hyperlink ref="D27" r:id="rId13"/>
-    <hyperlink ref="D29" r:id="rId14"/>
-    <hyperlink ref="D31" r:id="rId15"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D12" r:id="rId7"/>
+    <hyperlink ref="D13" r:id="rId8"/>
+    <hyperlink ref="D16" r:id="rId9"/>
+    <hyperlink ref="D18" r:id="rId10"/>
+    <hyperlink ref="D19" r:id="rId11"/>
+    <hyperlink ref="D20" r:id="rId12"/>
+    <hyperlink ref="D21" r:id="rId13"/>
+    <hyperlink ref="D23" r:id="rId14"/>
+    <hyperlink ref="D24" r:id="rId15"/>
+    <hyperlink ref="D26" r:id="rId16"/>
+    <hyperlink ref="D27" r:id="rId17"/>
+    <hyperlink ref="D29" r:id="rId18"/>
+    <hyperlink ref="D31" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2755,16 +2799,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C2">
         <v>7.7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E2">
         <v>2022</v>
@@ -2772,16 +2816,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C3">
         <v>8.9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="E3">
         <v>2019</v>
@@ -2789,16 +2833,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C4">
         <v>7.9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="E4">
         <v>2022</v>
@@ -2806,16 +2850,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C5">
         <v>9.699999999999999</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="E5">
         <v>2020</v>
@@ -2823,16 +2867,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C6">
         <v>8.199999999999999</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E6">
         <v>2023</v>
@@ -2840,16 +2884,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C7">
         <v>9.1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="E7">
         <v>2020</v>
@@ -2857,16 +2901,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C8">
         <v>6.9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E8">
         <v>2022</v>
@@ -2874,16 +2918,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C9">
         <v>6.4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E9">
         <v>2018</v>
@@ -2891,10 +2935,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C10">
         <v>7.1</v>
@@ -2908,16 +2952,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B11" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C11">
         <v>6.7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E11">
         <v>2017</v>
@@ -2925,16 +2969,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C12">
         <v>8.300000000000001</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="E12">
         <v>2019</v>
@@ -2942,16 +2986,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B13" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C13">
         <v>8.199999999999999</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E13">
         <v>2023</v>
@@ -2959,10 +3003,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B14" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C14">
         <v>6.5</v>
@@ -2976,10 +3020,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B15" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C15">
         <v>8.699999999999999</v>
@@ -2993,16 +3037,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C16">
         <v>10.5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="E16">
         <v>2020</v>
@@ -3010,16 +3054,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B17" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C17">
         <v>9.4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="E17">
         <v>2021</v>
@@ -3027,16 +3071,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C18">
         <v>9.1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E18">
         <v>2020</v>
@@ -3044,44 +3088,44 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C19">
         <v>7.7</v>
       </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
+      <c r="D19" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E19">
+        <v>2022</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B20" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C20">
         <v>9.4</v>
       </c>
-      <c r="D20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
+      <c r="D20" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20">
+        <v>2022</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B21" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C21">
         <v>11.3</v>
@@ -3095,16 +3139,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B22" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C22">
         <v>9.1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="E22">
         <v>2019</v>
@@ -3112,16 +3156,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="B23" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C23">
         <v>8.6</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="E23">
         <v>2021</v>
@@ -3129,33 +3173,33 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B24" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C24">
         <v>8.5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
+        <v>246</v>
+      </c>
+      <c r="E24">
+        <v>2021</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B25" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C25">
         <v>6.3</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="E25">
         <v>2020</v>
@@ -3163,16 +3207,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B26" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C26">
         <v>8.199999999999999</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="E26">
         <v>2018</v>
@@ -3180,16 +3224,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B27" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C27">
         <v>7.3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E27">
         <v>2022</v>
@@ -3211,12 +3255,14 @@
     <hyperlink ref="D16" r:id="rId12"/>
     <hyperlink ref="D17" r:id="rId13"/>
     <hyperlink ref="D18" r:id="rId14"/>
-    <hyperlink ref="D22" r:id="rId15"/>
-    <hyperlink ref="D23" r:id="rId16"/>
-    <hyperlink ref="D24" r:id="rId17"/>
-    <hyperlink ref="D25" r:id="rId18"/>
-    <hyperlink ref="D26" r:id="rId19"/>
-    <hyperlink ref="D27" r:id="rId20"/>
+    <hyperlink ref="D19" r:id="rId15"/>
+    <hyperlink ref="D20" r:id="rId16"/>
+    <hyperlink ref="D22" r:id="rId17"/>
+    <hyperlink ref="D23" r:id="rId18"/>
+    <hyperlink ref="D24" r:id="rId19"/>
+    <hyperlink ref="D25" r:id="rId20"/>
+    <hyperlink ref="D26" r:id="rId21"/>
+    <hyperlink ref="D27" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3249,10 +3295,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C2">
         <v>6.4</v>
@@ -3266,16 +3312,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C3">
         <v>7.9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="E3">
         <v>2013</v>
@@ -3283,16 +3329,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C4">
         <v>6.7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="E4">
         <v>2022</v>
@@ -3300,10 +3346,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="B5" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C5">
         <v>6.9</v>
@@ -3317,16 +3363,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C6">
         <v>6.6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="E6">
         <v>2019</v>
@@ -3334,10 +3380,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C7">
         <v>6.8</v>
@@ -3351,16 +3397,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C8">
         <v>7.4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="E8">
         <v>2022</v>
@@ -3368,16 +3414,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C9">
         <v>6.1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="E9">
         <v>2021</v>
@@ -3385,10 +3431,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="B10" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -3439,16 +3485,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C2">
         <v>6.3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E2">
         <v>2021</v>
@@ -3456,10 +3502,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -3473,10 +3519,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="B4" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C4">
         <v>9.6</v>
@@ -3490,10 +3536,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C5">
         <v>7.3</v>
@@ -3507,16 +3553,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B6" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C6">
         <v>8.1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E6">
         <v>2020</v>
@@ -3524,16 +3570,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C7">
         <v>7.6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="E7">
         <v>2022</v>
@@ -3541,16 +3587,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C8">
         <v>7.3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="E8">
         <v>2022</v>
@@ -3558,10 +3604,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="B9" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C9">
         <v>5.8</v>
@@ -3611,10 +3657,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C2">
         <v>6.4</v>
@@ -3628,16 +3674,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="E3">
         <v>2020</v>
@@ -3645,10 +3691,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C4">
         <v>4.9</v>
@@ -3662,10 +3708,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C5">
         <v>6.2</v>
@@ -3679,10 +3725,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C6">
         <v>7.1</v>
@@ -3696,10 +3742,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C7">
         <v>5.8</v>
@@ -3713,16 +3759,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="B8" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C8">
         <v>7.1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="E8">
         <v>2021</v>
@@ -3730,10 +3776,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C9">
         <v>7.6</v>
@@ -3747,10 +3793,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B10" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C10">
         <v>4.7</v>
@@ -3764,16 +3810,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="B11" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C11">
         <v>5.3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="E11">
         <v>2018</v>
@@ -3781,27 +3827,27 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
+      <c r="D12" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E12">
+        <v>2022</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B13" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C13">
         <v>5.6</v>
@@ -3815,10 +3861,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C14">
         <v>4.8</v>
@@ -3832,16 +3878,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B15" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C15">
         <v>2.4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="E15">
         <v>2022</v>
@@ -3849,10 +3895,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="B16" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C16">
         <v>6.3</v>
@@ -3866,16 +3912,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B17" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C17">
         <v>6.7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="E17">
         <v>2018</v>
@@ -3886,8 +3932,9 @@
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D8" r:id="rId2"/>
     <hyperlink ref="D11" r:id="rId3"/>
-    <hyperlink ref="D15" r:id="rId4"/>
-    <hyperlink ref="D17" r:id="rId5"/>
+    <hyperlink ref="D12" r:id="rId4"/>
+    <hyperlink ref="D15" r:id="rId5"/>
+    <hyperlink ref="D17" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3920,10 +3967,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C2">
         <v>8.5</v>
@@ -3937,16 +3984,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="B3" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C3">
         <v>6.2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E3">
         <v>2021</v>
@@ -3954,10 +4001,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C4">
         <v>8.199999999999999</v>
@@ -3971,10 +4018,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="B5" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C5">
         <v>10.1</v>
@@ -3988,10 +4035,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="B6" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C6">
         <v>10.2</v>
@@ -4005,10 +4052,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C7">
         <v>3.9</v>
@@ -4022,16 +4069,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="B8" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C8">
         <v>5.9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="E8">
         <v>2020</v>
@@ -4039,10 +4086,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="B9" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C9">
         <v>1.8</v>
@@ -4056,10 +4103,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="B10" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C10">
         <v>3.7</v>
@@ -4073,10 +4120,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="B11" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C11">
         <v>8.300000000000001</v>
@@ -4090,10 +4137,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="B12" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C12">
         <v>5.7</v>
@@ -4107,10 +4154,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="B13" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C13">
         <v>8</v>
@@ -4124,16 +4171,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="B14" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C14">
         <v>7.3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="E14">
         <v>2022</v>
@@ -4141,10 +4188,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="B15" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C15">
         <v>6.3</v>
@@ -4158,16 +4205,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="B16" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C16">
         <v>8.199999999999999</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="E16">
         <v>2022</v>
@@ -4211,10 +4258,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C2">
         <v>5.9</v>
@@ -4228,10 +4275,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C3">
         <v>7.5</v>
@@ -4239,16 +4286,16 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
-        <v>2021</v>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C4">
         <v>7.2</v>
@@ -4262,33 +4309,33 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="B5" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C5">
         <v>6.6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
+        <v>329</v>
+      </c>
+      <c r="E5">
+        <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C6">
         <v>8.1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="E6">
         <v>2019</v>
@@ -4296,10 +4343,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="B7" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C7">
         <v>6.2</v>
@@ -4313,25 +4360,26 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="B8" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C8">
         <v>6.1</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
+      <c r="D8" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="E8">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1"/>
     <hyperlink ref="D6" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4364,10 +4412,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C2">
         <v>8.5</v>
@@ -4381,10 +4429,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="B3" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C3">
         <v>8.300000000000001</v>
@@ -4398,10 +4446,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="B4" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C4">
         <v>7.7</v>
@@ -4415,10 +4463,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="B5" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C5">
         <v>8.1</v>
@@ -4432,16 +4480,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="B6" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C6">
         <v>8.199999999999999</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="E6">
         <v>2021</v>
@@ -4449,16 +4497,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="B7" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C7">
         <v>7.6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="E7">
         <v>2017</v>
@@ -4466,16 +4514,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C8">
         <v>6.9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="E8">
         <v>2019</v>
@@ -4483,10 +4531,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="B9" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -4500,10 +4548,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C10">
         <v>6.7</v>
@@ -4517,19 +4565,19 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C11">
         <v>7.7</v>
       </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
+      <c r="D11" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E11">
+        <v>2009</v>
       </c>
     </row>
   </sheetData>
@@ -4537,6 +4585,7 @@
     <hyperlink ref="D6" r:id="rId1"/>
     <hyperlink ref="D7" r:id="rId2"/>
     <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="D11" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4569,16 +4618,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="B2" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C2">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="E2">
         <v>2021</v>
@@ -4586,10 +4635,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C3">
         <v>7.8</v>
@@ -4603,10 +4652,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="B4" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C4">
         <v>7.7</v>
@@ -4620,10 +4669,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="B5" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C5">
         <v>8.199999999999999</v>
@@ -4637,10 +4686,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="B6" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C6">
         <v>8.199999999999999</v>
@@ -4654,33 +4703,33 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="B7" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C7">
         <v>7.6</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
+      <c r="D7" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E7">
+        <v>2018</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="B8" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C8">
         <v>8.300000000000001</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="E8">
         <v>2018</v>
@@ -4688,10 +4737,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
       <c r="B9" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C9">
         <v>7.6</v>
@@ -4705,33 +4754,33 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B10" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C10">
         <v>7.7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
+        <v>400</v>
+      </c>
+      <c r="E10">
+        <v>2020</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
       <c r="B11" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="E11">
         <v>2020</v>
@@ -4739,10 +4788,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="B12" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C12">
         <v>5.5</v>
@@ -4756,16 +4805,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
       <c r="B13" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C13">
         <v>7.8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
       <c r="E13">
         <v>2021</v>
@@ -4773,10 +4822,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="B14" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C14">
         <v>8.9</v>
@@ -4790,10 +4839,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="B15" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C15">
         <v>7.4</v>
@@ -4807,10 +4856,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="B16" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C16">
         <v>7.5</v>
@@ -4824,10 +4873,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="B17" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C17">
         <v>6.3</v>
@@ -4841,10 +4890,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="B18" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C18">
         <v>5.5</v>
@@ -4858,10 +4907,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="B19" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C19">
         <v>6.6</v>
@@ -4875,10 +4924,10 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="B20" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C20">
         <v>4.7</v>
@@ -4892,10 +4941,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="B21" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C21">
         <v>7</v>
@@ -4909,10 +4958,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="B22" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C22">
         <v>5.5</v>
@@ -4926,10 +4975,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="B23" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C23">
         <v>5.5</v>
@@ -4943,10 +4992,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
       <c r="B24" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C24">
         <v>7.1</v>
@@ -4954,16 +5003,16 @@
       <c r="D24" t="s">
         <v>14</v>
       </c>
-      <c r="E24">
-        <v>2022</v>
+      <c r="E24" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
       <c r="B25" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C25">
         <v>5.9</v>
@@ -4977,10 +5026,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="B26" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C26">
         <v>7.1</v>
@@ -4994,33 +5043,33 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
       <c r="B27" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C27">
         <v>7.4</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="E27">
-        <v>2022</v>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="B28" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C28">
         <v>8.1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="E28">
         <v>2021</v>
@@ -5028,16 +5077,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="B29" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C29">
         <v>5.8</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="E29">
         <v>2019</v>
@@ -5045,10 +5094,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="B30" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C30">
         <v>7.9</v>
@@ -5062,16 +5111,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="B31" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C31">
         <v>5.8</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="E31">
         <v>2022</v>
@@ -5079,16 +5128,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="B32" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C32">
         <v>8.1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>395</v>
+        <v>406</v>
       </c>
       <c r="E32">
         <v>2021</v>
@@ -5096,16 +5145,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="B33" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C33">
         <v>8.300000000000001</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="E33">
         <v>2022</v>
@@ -5113,10 +5162,10 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="B34" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C34">
         <v>6.5</v>
@@ -5130,10 +5179,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="B35" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C35">
         <v>6.8</v>
@@ -5141,22 +5190,22 @@
       <c r="D35" t="s">
         <v>14</v>
       </c>
-      <c r="E35">
-        <v>2022</v>
+      <c r="E35" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="B36" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C36">
         <v>8.4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="E36">
         <v>2022</v>
@@ -5164,16 +5213,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="B37" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C37">
         <v>8</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="E37">
         <v>2021</v>
@@ -5181,16 +5230,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="B38" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C38">
         <v>6.9</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="E38">
         <v>2022</v>
@@ -5198,10 +5247,10 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="B39" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C39">
         <v>7.7</v>
@@ -5215,16 +5264,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="B40" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C40">
         <v>5.7</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="E40">
         <v>2022</v>
@@ -5232,16 +5281,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="B41" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C41">
         <v>6.9</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="E41">
         <v>2020</v>
@@ -5249,10 +5298,10 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="B42" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C42">
         <v>5.4</v>
@@ -5266,16 +5315,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="B43" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C43">
         <v>4.7</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="E43">
         <v>2017</v>
@@ -5283,27 +5332,27 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="B44" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C44">
         <v>5.8</v>
       </c>
-      <c r="D44" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44" t="s">
-        <v>14</v>
+      <c r="D44" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E44">
+        <v>2022</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="B45" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C45">
         <v>6.3</v>
@@ -5317,33 +5366,33 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="B46" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C46">
         <v>6.3</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E46" t="s">
-        <v>14</v>
+        <v>415</v>
+      </c>
+      <c r="E46">
+        <v>2017</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="B47" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C47">
         <v>6</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="E47">
         <v>2021</v>
@@ -5351,27 +5400,27 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="B48" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C48">
         <v>7.4</v>
       </c>
-      <c r="D48" t="s">
-        <v>14</v>
-      </c>
-      <c r="E48" t="s">
-        <v>14</v>
+      <c r="D48" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E48">
+        <v>2018</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="B49" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C49">
         <v>6.3</v>
@@ -5385,16 +5434,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="B50" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C50">
         <v>6</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>405</v>
+        <v>418</v>
       </c>
       <c r="E50">
         <v>2021</v>
@@ -5403,11 +5452,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D8" r:id="rId2"/>
-    <hyperlink ref="D10" r:id="rId3"/>
-    <hyperlink ref="D11" r:id="rId4"/>
-    <hyperlink ref="D13" r:id="rId5"/>
-    <hyperlink ref="D27" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="D10" r:id="rId4"/>
+    <hyperlink ref="D11" r:id="rId5"/>
+    <hyperlink ref="D13" r:id="rId6"/>
     <hyperlink ref="D28" r:id="rId7"/>
     <hyperlink ref="D29" r:id="rId8"/>
     <hyperlink ref="D31" r:id="rId9"/>
@@ -5419,9 +5468,11 @@
     <hyperlink ref="D40" r:id="rId15"/>
     <hyperlink ref="D41" r:id="rId16"/>
     <hyperlink ref="D43" r:id="rId17"/>
-    <hyperlink ref="D46" r:id="rId18"/>
-    <hyperlink ref="D47" r:id="rId19"/>
-    <hyperlink ref="D50" r:id="rId20"/>
+    <hyperlink ref="D44" r:id="rId18"/>
+    <hyperlink ref="D46" r:id="rId19"/>
+    <hyperlink ref="D47" r:id="rId20"/>
+    <hyperlink ref="D48" r:id="rId21"/>
+    <hyperlink ref="D50" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5745,16 +5796,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>419</v>
       </c>
       <c r="B2" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C2">
         <v>8.800000000000001</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="E2">
         <v>2022</v>
@@ -5762,10 +5813,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>407</v>
+        <v>420</v>
       </c>
       <c r="B3" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -5779,10 +5830,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="B4" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -5796,16 +5847,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>420</v>
+        <v>433</v>
       </c>
       <c r="E5">
         <v>2021</v>
@@ -5813,10 +5864,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="B6" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C6">
         <v>2.3</v>
@@ -5830,10 +5881,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>411</v>
+        <v>424</v>
       </c>
       <c r="B7" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C7">
         <v>6.2</v>
@@ -5847,16 +5898,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="B8" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C8">
         <v>6.8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="E8">
         <v>2016</v>
@@ -5864,10 +5915,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>413</v>
+        <v>426</v>
       </c>
       <c r="B9" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C9">
         <v>7.4</v>
@@ -5881,16 +5932,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>414</v>
+        <v>427</v>
       </c>
       <c r="B10" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C10">
         <v>8.199999999999999</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>422</v>
+        <v>435</v>
       </c>
       <c r="E10">
         <v>2022</v>
@@ -5898,16 +5949,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>415</v>
+        <v>428</v>
       </c>
       <c r="B11" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C11">
         <v>6.7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="E11">
         <v>2021</v>
@@ -5915,10 +5966,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>416</v>
+        <v>429</v>
       </c>
       <c r="B12" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C12">
         <v>7.8</v>
@@ -5932,10 +5983,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>417</v>
+        <v>430</v>
       </c>
       <c r="B13" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="C13">
         <v>6.3</v>
@@ -5986,10 +6037,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="B2" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C2">
         <v>7.1</v>
@@ -5997,16 +6048,16 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
-        <v>2012</v>
+      <c r="E2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="B3" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C3">
         <v>6.1</v>
@@ -6020,10 +6071,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="B4" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C4">
         <v>7.7</v>
@@ -6037,10 +6088,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="B5" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C5">
         <v>6.8</v>
@@ -6054,16 +6105,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>428</v>
+        <v>441</v>
       </c>
       <c r="B6" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C6">
         <v>7.8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="E6">
         <v>2022</v>
@@ -6071,10 +6122,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>429</v>
+        <v>442</v>
       </c>
       <c r="B7" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C7">
         <v>6.6</v>
@@ -6082,16 +6133,16 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
-        <v>2015</v>
+      <c r="E7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>430</v>
+        <v>443</v>
       </c>
       <c r="B8" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C8">
         <v>6.3</v>
@@ -6105,16 +6156,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="B9" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C9">
         <v>7.8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>439</v>
+        <v>452</v>
       </c>
       <c r="E9">
         <v>2022</v>
@@ -6122,10 +6173,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>432</v>
+        <v>445</v>
       </c>
       <c r="B10" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C10">
         <v>6.9</v>
@@ -6139,16 +6190,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>433</v>
+        <v>446</v>
       </c>
       <c r="B11" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C11">
         <v>7.9</v>
       </c>
       <c r="D11" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="E11">
         <v>2022</v>
@@ -6156,10 +6207,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>434</v>
+        <v>447</v>
       </c>
       <c r="B12" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C12">
         <v>6.1</v>
@@ -6173,10 +6224,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
       <c r="B13" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C13">
         <v>8.300000000000001</v>
@@ -6190,16 +6241,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>436</v>
+        <v>449</v>
       </c>
       <c r="B14" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
       <c r="C14">
         <v>8.300000000000001</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>441</v>
+        <v>454</v>
       </c>
       <c r="E14">
         <v>2020</v>
@@ -6591,16 +6642,17 @@
       <c r="C7">
         <v>8.1</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
+      <c r="D7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7">
+        <v>2022</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6633,10 +6685,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2">
         <v>5.1</v>
@@ -6650,10 +6702,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>7.1</v>
@@ -6667,10 +6719,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C4">
         <v>9.300000000000001</v>
@@ -6684,10 +6736,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C5">
         <v>2.4</v>
@@ -6701,10 +6753,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>7.5</v>
@@ -6718,16 +6770,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7">
         <v>8.1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7">
         <v>2022</v>
@@ -6735,10 +6787,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C8">
         <v>4.7</v>
@@ -6752,16 +6804,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9">
         <v>2019</v>
@@ -6803,16 +6855,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2">
         <v>8.199999999999999</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E2">
         <v>2011</v>
@@ -6820,10 +6872,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -6837,33 +6889,33 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4">
         <v>7.8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <v>89</v>
+      </c>
+      <c r="E4">
+        <v>2021</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5">
         <v>7.8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E5">
         <v>2021</v>
@@ -6871,16 +6923,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C6">
         <v>7.4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E6">
         <v>2021</v>
@@ -6888,16 +6940,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C7">
         <v>7.4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E7">
         <v>2022</v>
@@ -6905,16 +6957,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C8">
         <v>6.1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E8">
         <v>2022</v>
@@ -6922,16 +6974,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C9">
         <v>6.3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E9">
         <v>2016</v>
@@ -6939,16 +6991,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>5.9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E10">
         <v>2023</v>
@@ -6956,10 +7008,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C11">
         <v>6.4</v>
@@ -6973,10 +7025,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C12">
         <v>6.4</v>
@@ -6990,10 +7042,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -7007,16 +7059,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <v>7.1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E14">
         <v>2022</v>
@@ -7065,10 +7117,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C2">
         <v>4.8</v>
@@ -7082,10 +7134,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3">
         <v>6.2</v>
@@ -7099,10 +7151,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -7116,10 +7168,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C5">
         <v>4.8</v>
@@ -7133,10 +7185,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6">
         <v>6.5</v>
@@ -7150,10 +7202,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C7">
         <v>5.3</v>
@@ -7167,16 +7219,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8">
         <v>5.7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E8">
         <v>2019</v>
@@ -7184,10 +7236,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>6.3</v>
@@ -7201,10 +7253,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -7218,16 +7270,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C11">
         <v>5.8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E11">
         <v>2021</v>
@@ -7235,10 +7287,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C12">
         <v>5.5</v>
@@ -7252,16 +7304,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C13">
         <v>7.5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E13">
         <v>2019</v>
@@ -7304,16 +7356,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E2">
         <v>2022</v>
@@ -7321,16 +7373,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C3">
         <v>7.9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E3">
         <v>2019</v>
@@ -7338,16 +7390,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E4">
         <v>2022</v>
@@ -7355,10 +7407,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C5">
         <v>8.5</v>
@@ -7372,16 +7424,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C6">
         <v>7.1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E6">
         <v>2020</v>
@@ -7389,10 +7441,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C7">
         <v>6.6</v>
@@ -7406,33 +7458,33 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
+        <v>126</v>
+      </c>
+      <c r="E8">
+        <v>2019</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C9">
         <v>5.9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E9">
         <v>2020</v>

</xml_diff>

<commit_message>
update smhi data and years
</commit_message>
<xml_diff>
--- a/data/climate-data.xlsx
+++ b/data/climate-data.xlsx
@@ -42,7 +42,7 @@
     <t>Län</t>
   </si>
   <si>
-    <t>Utsläppsförändring 2019-2020 (%)</t>
+    <t>Utsläppsförändring 2020-2021 (%)</t>
   </si>
   <si>
     <t>KPI1: Förändringstakt andel laddbara bilar (%)</t>
@@ -1806,7 +1806,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1.7</v>
+        <v>85.09999999999999</v>
       </c>
       <c r="D2">
         <v>5.2</v>
@@ -1826,7 +1826,7 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>-7.9</v>
+        <v>-1.4</v>
       </c>
       <c r="D3">
         <v>7</v>
@@ -1846,7 +1846,7 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>-14</v>
+        <v>4.8</v>
       </c>
       <c r="D4">
         <v>4.8</v>
@@ -1866,7 +1866,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>-9.6</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>6.1</v>
@@ -1886,7 +1886,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>-19.6</v>
+        <v>5.4</v>
       </c>
       <c r="D6">
         <v>6.8</v>
@@ -1943,7 +1943,7 @@
         <v>143</v>
       </c>
       <c r="C2">
-        <v>-6.7</v>
+        <v>6.5</v>
       </c>
       <c r="D2">
         <v>6.4</v>
@@ -1963,7 +1963,7 @@
         <v>143</v>
       </c>
       <c r="C3">
-        <v>-10.7</v>
+        <v>2.2</v>
       </c>
       <c r="D3">
         <v>3.1</v>
@@ -1983,7 +1983,7 @@
         <v>143</v>
       </c>
       <c r="C4">
-        <v>-5.8</v>
+        <v>5.3</v>
       </c>
       <c r="D4">
         <v>6.1</v>
@@ -2003,7 +2003,7 @@
         <v>143</v>
       </c>
       <c r="C5">
-        <v>-11.1</v>
+        <v>-4.5</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -2023,7 +2023,7 @@
         <v>143</v>
       </c>
       <c r="C6">
-        <v>-4.6</v>
+        <v>-6.2</v>
       </c>
       <c r="D6">
         <v>3.9</v>
@@ -2043,7 +2043,7 @@
         <v>143</v>
       </c>
       <c r="C7">
-        <v>-6.8</v>
+        <v>5.6</v>
       </c>
       <c r="D7">
         <v>5.5</v>
@@ -2063,7 +2063,7 @@
         <v>143</v>
       </c>
       <c r="C8">
-        <v>-11.2</v>
+        <v>10.3</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -2083,7 +2083,7 @@
         <v>143</v>
       </c>
       <c r="C9">
-        <v>-1.4</v>
+        <v>-2.4</v>
       </c>
       <c r="D9">
         <v>3.9</v>
@@ -2103,7 +2103,7 @@
         <v>143</v>
       </c>
       <c r="C10">
-        <v>-3.1</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>7.6</v>
@@ -2123,7 +2123,7 @@
         <v>143</v>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>-1.3</v>
       </c>
       <c r="D11">
         <v>4.7</v>
@@ -2143,7 +2143,7 @@
         <v>143</v>
       </c>
       <c r="C12">
-        <v>-13.6</v>
+        <v>4.6</v>
       </c>
       <c r="D12">
         <v>8.4</v>
@@ -2163,7 +2163,7 @@
         <v>143</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>-8.1</v>
       </c>
       <c r="D13">
         <v>5.5</v>
@@ -2183,7 +2183,7 @@
         <v>143</v>
       </c>
       <c r="C14">
-        <v>-7.2</v>
+        <v>-0.7</v>
       </c>
       <c r="D14">
         <v>3.8</v>
@@ -2203,7 +2203,7 @@
         <v>143</v>
       </c>
       <c r="C15">
-        <v>-7.8</v>
+        <v>-3.2</v>
       </c>
       <c r="D15">
         <v>6.8</v>
@@ -2262,7 +2262,7 @@
         <v>182</v>
       </c>
       <c r="C2">
-        <v>-5.5</v>
+        <v>1.3</v>
       </c>
       <c r="D2">
         <v>4.6</v>
@@ -2282,7 +2282,7 @@
         <v>182</v>
       </c>
       <c r="C3">
-        <v>-23.8</v>
+        <v>6.7</v>
       </c>
       <c r="D3">
         <v>7.1</v>
@@ -2302,7 +2302,7 @@
         <v>182</v>
       </c>
       <c r="C4">
-        <v>-16.1</v>
+        <v>-11.6</v>
       </c>
       <c r="D4">
         <v>4.8</v>
@@ -2322,7 +2322,7 @@
         <v>182</v>
       </c>
       <c r="C5">
-        <v>-8.9</v>
+        <v>0.6</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -2342,7 +2342,7 @@
         <v>182</v>
       </c>
       <c r="C6">
-        <v>31.3</v>
+        <v>-2.4</v>
       </c>
       <c r="D6">
         <v>5.9</v>
@@ -2362,7 +2362,7 @@
         <v>182</v>
       </c>
       <c r="C7">
-        <v>-6.2</v>
+        <v>1.5</v>
       </c>
       <c r="D7">
         <v>6.3</v>
@@ -2382,7 +2382,7 @@
         <v>182</v>
       </c>
       <c r="C8">
-        <v>3.5</v>
+        <v>-11.6</v>
       </c>
       <c r="D8">
         <v>5.6</v>
@@ -2402,7 +2402,7 @@
         <v>182</v>
       </c>
       <c r="C9">
-        <v>-5.4</v>
+        <v>19.2</v>
       </c>
       <c r="D9">
         <v>7.3</v>
@@ -2422,7 +2422,7 @@
         <v>182</v>
       </c>
       <c r="C10">
-        <v>-8.800000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -2442,7 +2442,7 @@
         <v>182</v>
       </c>
       <c r="C11">
-        <v>-8.800000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D11">
         <v>6.3</v>
@@ -2462,7 +2462,7 @@
         <v>182</v>
       </c>
       <c r="C12">
-        <v>-2.9</v>
+        <v>1.1</v>
       </c>
       <c r="D12">
         <v>6.4</v>
@@ -2482,7 +2482,7 @@
         <v>182</v>
       </c>
       <c r="C13">
-        <v>-8.800000000000001</v>
+        <v>-1.7</v>
       </c>
       <c r="D13">
         <v>7.5</v>
@@ -2502,7 +2502,7 @@
         <v>182</v>
       </c>
       <c r="C14">
-        <v>-7.9</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
         <v>9.300000000000001</v>
@@ -2522,7 +2522,7 @@
         <v>182</v>
       </c>
       <c r="C15">
-        <v>-7.5</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>7.4</v>
@@ -2542,7 +2542,7 @@
         <v>182</v>
       </c>
       <c r="C16">
-        <v>-7.5</v>
+        <v>0.3</v>
       </c>
       <c r="D16">
         <v>9</v>
@@ -2562,7 +2562,7 @@
         <v>182</v>
       </c>
       <c r="C17">
-        <v>-9.300000000000001</v>
+        <v>-3.3</v>
       </c>
       <c r="D17">
         <v>10.4</v>
@@ -2582,7 +2582,7 @@
         <v>182</v>
       </c>
       <c r="C18">
-        <v>-16.6</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>6.4</v>
@@ -2602,7 +2602,7 @@
         <v>182</v>
       </c>
       <c r="C19">
-        <v>-11.5</v>
+        <v>-0.9</v>
       </c>
       <c r="D19">
         <v>5.4</v>
@@ -2622,7 +2622,7 @@
         <v>182</v>
       </c>
       <c r="C20">
-        <v>-0.8</v>
+        <v>1.1</v>
       </c>
       <c r="D20">
         <v>6.4</v>
@@ -2642,7 +2642,7 @@
         <v>182</v>
       </c>
       <c r="C21">
-        <v>-10.5</v>
+        <v>0.2</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -2662,7 +2662,7 @@
         <v>182</v>
       </c>
       <c r="C22">
-        <v>-7.8</v>
+        <v>0.4</v>
       </c>
       <c r="D22">
         <v>6.6</v>
@@ -2682,7 +2682,7 @@
         <v>182</v>
       </c>
       <c r="C23">
-        <v>-7.1</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>6.6</v>
@@ -2702,7 +2702,7 @@
         <v>182</v>
       </c>
       <c r="C24">
-        <v>-7.6</v>
+        <v>0.1</v>
       </c>
       <c r="D24">
         <v>8.199999999999999</v>
@@ -2722,7 +2722,7 @@
         <v>182</v>
       </c>
       <c r="C25">
-        <v>-10</v>
+        <v>2.6</v>
       </c>
       <c r="D25">
         <v>6.7</v>
@@ -2742,7 +2742,7 @@
         <v>182</v>
       </c>
       <c r="C26">
-        <v>-9.199999999999999</v>
+        <v>4.6</v>
       </c>
       <c r="D26">
         <v>7.5</v>
@@ -2762,7 +2762,7 @@
         <v>182</v>
       </c>
       <c r="C27">
-        <v>-7.2</v>
+        <v>-5.7</v>
       </c>
       <c r="D27">
         <v>2.9</v>
@@ -2782,7 +2782,7 @@
         <v>182</v>
       </c>
       <c r="C28">
-        <v>-9.800000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="D28">
         <v>7.3</v>
@@ -2802,7 +2802,7 @@
         <v>182</v>
       </c>
       <c r="C29">
-        <v>-6.5</v>
+        <v>-0.5</v>
       </c>
       <c r="D29">
         <v>8.4</v>
@@ -2822,7 +2822,7 @@
         <v>182</v>
       </c>
       <c r="C30">
-        <v>-7.3</v>
+        <v>0.3</v>
       </c>
       <c r="D30">
         <v>5.7</v>
@@ -2842,7 +2842,7 @@
         <v>182</v>
       </c>
       <c r="C31">
-        <v>-7.7</v>
+        <v>-2.3</v>
       </c>
       <c r="D31">
         <v>6.3</v>
@@ -2862,7 +2862,7 @@
         <v>182</v>
       </c>
       <c r="C32">
-        <v>-11</v>
+        <v>1.9</v>
       </c>
       <c r="D32">
         <v>7.2</v>
@@ -2882,7 +2882,7 @@
         <v>182</v>
       </c>
       <c r="C33">
-        <v>-7.8</v>
+        <v>1.1</v>
       </c>
       <c r="D33">
         <v>3.3</v>
@@ -2902,7 +2902,7 @@
         <v>182</v>
       </c>
       <c r="C34">
-        <v>-10</v>
+        <v>-0.8</v>
       </c>
       <c r="D34">
         <v>7.5</v>
@@ -2976,7 +2976,7 @@
         <v>228</v>
       </c>
       <c r="C2">
-        <v>-9.1</v>
+        <v>-0.3</v>
       </c>
       <c r="D2">
         <v>6.4</v>
@@ -2996,7 +2996,7 @@
         <v>228</v>
       </c>
       <c r="C3">
-        <v>-8.5</v>
+        <v>1.3</v>
       </c>
       <c r="D3">
         <v>10.5</v>
@@ -3016,7 +3016,7 @@
         <v>228</v>
       </c>
       <c r="C4">
-        <v>-11.1</v>
+        <v>7.4</v>
       </c>
       <c r="D4">
         <v>9.1</v>
@@ -3036,7 +3036,7 @@
         <v>228</v>
       </c>
       <c r="C5">
-        <v>-7</v>
+        <v>-3.1</v>
       </c>
       <c r="D5">
         <v>6.7</v>
@@ -3056,7 +3056,7 @@
         <v>228</v>
       </c>
       <c r="C6">
-        <v>-8.9</v>
+        <v>0.3</v>
       </c>
       <c r="D6">
         <v>6.9</v>
@@ -3076,7 +3076,7 @@
         <v>228</v>
       </c>
       <c r="C7">
-        <v>-9.4</v>
+        <v>0.3</v>
       </c>
       <c r="D7">
         <v>8.199999999999999</v>
@@ -3096,7 +3096,7 @@
         <v>228</v>
       </c>
       <c r="C8">
-        <v>7.3</v>
+        <v>9.6</v>
       </c>
       <c r="D8">
         <v>8.6</v>
@@ -3116,7 +3116,7 @@
         <v>228</v>
       </c>
       <c r="C9">
-        <v>-8.699999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D9">
         <v>9.4</v>
@@ -3136,7 +3136,7 @@
         <v>228</v>
       </c>
       <c r="C10">
-        <v>-8.9</v>
+        <v>2.7</v>
       </c>
       <c r="D10">
         <v>6.3</v>
@@ -3156,7 +3156,7 @@
         <v>228</v>
       </c>
       <c r="C11">
-        <v>-9.5</v>
+        <v>0.1</v>
       </c>
       <c r="D11">
         <v>6.5</v>
@@ -3176,7 +3176,7 @@
         <v>228</v>
       </c>
       <c r="C12">
-        <v>-8.4</v>
+        <v>-1.6</v>
       </c>
       <c r="D12">
         <v>7.3</v>
@@ -3196,7 +3196,7 @@
         <v>228</v>
       </c>
       <c r="C13">
-        <v>-8.199999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="D13">
         <v>7.1</v>
@@ -3216,7 +3216,7 @@
         <v>228</v>
       </c>
       <c r="C14">
-        <v>-8.800000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="D14">
         <v>8.199999999999999</v>
@@ -3236,7 +3236,7 @@
         <v>228</v>
       </c>
       <c r="C15">
-        <v>-8.6</v>
+        <v>0.5</v>
       </c>
       <c r="D15">
         <v>9.4</v>
@@ -3256,7 +3256,7 @@
         <v>228</v>
       </c>
       <c r="C16">
-        <v>-8.5</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>9.1</v>
@@ -3276,7 +3276,7 @@
         <v>228</v>
       </c>
       <c r="C17">
-        <v>-27.4</v>
+        <v>5.6</v>
       </c>
       <c r="D17">
         <v>9.1</v>
@@ -3296,7 +3296,7 @@
         <v>228</v>
       </c>
       <c r="C18">
-        <v>-8.9</v>
+        <v>-0</v>
       </c>
       <c r="D18">
         <v>11.3</v>
@@ -3316,7 +3316,7 @@
         <v>228</v>
       </c>
       <c r="C19">
-        <v>-41.6</v>
+        <v>-1.7</v>
       </c>
       <c r="D19">
         <v>7.7</v>
@@ -3336,7 +3336,7 @@
         <v>228</v>
       </c>
       <c r="C20">
-        <v>-8.6</v>
+        <v>0.7</v>
       </c>
       <c r="D20">
         <v>8.300000000000001</v>
@@ -3356,7 +3356,7 @@
         <v>228</v>
       </c>
       <c r="C21">
-        <v>-9.199999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="D21">
         <v>8.699999999999999</v>
@@ -3376,7 +3376,7 @@
         <v>228</v>
       </c>
       <c r="C22">
-        <v>-13.4</v>
+        <v>0.6</v>
       </c>
       <c r="D22">
         <v>7.7</v>
@@ -3396,7 +3396,7 @@
         <v>228</v>
       </c>
       <c r="C23">
-        <v>109</v>
+        <v>2.6</v>
       </c>
       <c r="D23">
         <v>8.199999999999999</v>
@@ -3416,7 +3416,7 @@
         <v>228</v>
       </c>
       <c r="C24">
-        <v>-10</v>
+        <v>0.7</v>
       </c>
       <c r="D24">
         <v>8.9</v>
@@ -3436,7 +3436,7 @@
         <v>228</v>
       </c>
       <c r="C25">
-        <v>-4.9</v>
+        <v>12.3</v>
       </c>
       <c r="D25">
         <v>8.5</v>
@@ -3456,7 +3456,7 @@
         <v>228</v>
       </c>
       <c r="C26">
-        <v>-7.8</v>
+        <v>6.8</v>
       </c>
       <c r="D26">
         <v>9.699999999999999</v>
@@ -3476,7 +3476,7 @@
         <v>228</v>
       </c>
       <c r="C27">
-        <v>-9.300000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D27">
         <v>7.9</v>
@@ -3553,7 +3553,7 @@
         <v>260</v>
       </c>
       <c r="C2">
-        <v>-9.300000000000001</v>
+        <v>3.8</v>
       </c>
       <c r="D2">
         <v>7.4</v>
@@ -3573,7 +3573,7 @@
         <v>260</v>
       </c>
       <c r="C3">
-        <v>-9.300000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="D3">
         <v>6.6</v>
@@ -3593,7 +3593,7 @@
         <v>260</v>
       </c>
       <c r="C4">
-        <v>-12.6</v>
+        <v>3.3</v>
       </c>
       <c r="D4">
         <v>7.9</v>
@@ -3613,7 +3613,7 @@
         <v>260</v>
       </c>
       <c r="C5">
-        <v>-8.1</v>
+        <v>3.5</v>
       </c>
       <c r="D5">
         <v>6.8</v>
@@ -3633,7 +3633,7 @@
         <v>260</v>
       </c>
       <c r="C6">
-        <v>-7.9</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>6.7</v>
@@ -3653,7 +3653,7 @@
         <v>260</v>
       </c>
       <c r="C7">
-        <v>-27.4</v>
+        <v>8.9</v>
       </c>
       <c r="D7">
         <v>6.9</v>
@@ -3673,7 +3673,7 @@
         <v>260</v>
       </c>
       <c r="C8">
-        <v>-4</v>
+        <v>2.4</v>
       </c>
       <c r="D8">
         <v>6.1</v>
@@ -3693,7 +3693,7 @@
         <v>260</v>
       </c>
       <c r="C9">
-        <v>-10.3</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -3713,7 +3713,7 @@
         <v>260</v>
       </c>
       <c r="C10">
-        <v>-12.7</v>
+        <v>1.4</v>
       </c>
       <c r="D10">
         <v>6.4</v>
@@ -3773,7 +3773,7 @@
         <v>274</v>
       </c>
       <c r="C2">
-        <v>-9.1</v>
+        <v>-2.1</v>
       </c>
       <c r="D2">
         <v>7.3</v>
@@ -3793,7 +3793,7 @@
         <v>274</v>
       </c>
       <c r="C3">
-        <v>-6.9</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>7.3</v>
@@ -3813,7 +3813,7 @@
         <v>274</v>
       </c>
       <c r="C4">
-        <v>-8.5</v>
+        <v>5.6</v>
       </c>
       <c r="D4">
         <v>6.3</v>
@@ -3833,7 +3833,7 @@
         <v>274</v>
       </c>
       <c r="C5">
-        <v>-12.5</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>9.6</v>
@@ -3853,7 +3853,7 @@
         <v>274</v>
       </c>
       <c r="C6">
-        <v>-10.9</v>
+        <v>-1.3</v>
       </c>
       <c r="D6">
         <v>8.1</v>
@@ -3873,7 +3873,7 @@
         <v>274</v>
       </c>
       <c r="C7">
-        <v>-24.2</v>
+        <v>2.9</v>
       </c>
       <c r="D7">
         <v>7.6</v>
@@ -3893,7 +3893,7 @@
         <v>274</v>
       </c>
       <c r="C8">
-        <v>-8.6</v>
+        <v>1.8</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -3913,7 +3913,7 @@
         <v>274</v>
       </c>
       <c r="C9">
-        <v>-17.8</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>5.8</v>
@@ -3972,7 +3972,7 @@
         <v>295</v>
       </c>
       <c r="C2">
-        <v>-10.2</v>
+        <v>4.6</v>
       </c>
       <c r="D2">
         <v>6.3</v>
@@ -3992,7 +3992,7 @@
         <v>295</v>
       </c>
       <c r="C3">
-        <v>-5</v>
+        <v>7.9</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -4012,7 +4012,7 @@
         <v>295</v>
       </c>
       <c r="C4">
-        <v>-8.6</v>
+        <v>-1.3</v>
       </c>
       <c r="D4">
         <v>4.8</v>
@@ -4032,7 +4032,7 @@
         <v>295</v>
       </c>
       <c r="C5">
-        <v>-7.6</v>
+        <v>4.2</v>
       </c>
       <c r="D5">
         <v>7.1</v>
@@ -4052,7 +4052,7 @@
         <v>295</v>
       </c>
       <c r="C6">
-        <v>-13.7</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="D6">
         <v>7.6</v>
@@ -4072,7 +4072,7 @@
         <v>295</v>
       </c>
       <c r="C7">
-        <v>-7.7</v>
+        <v>16.7</v>
       </c>
       <c r="D7">
         <v>2.4</v>
@@ -4092,7 +4092,7 @@
         <v>295</v>
       </c>
       <c r="C8">
-        <v>-17.1</v>
+        <v>3.8</v>
       </c>
       <c r="D8">
         <v>7.1</v>
@@ -4112,7 +4112,7 @@
         <v>295</v>
       </c>
       <c r="C9">
-        <v>-6.6</v>
+        <v>1.5</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -4132,7 +4132,7 @@
         <v>295</v>
       </c>
       <c r="C10">
-        <v>-6.7</v>
+        <v>5.8</v>
       </c>
       <c r="D10">
         <v>6.4</v>
@@ -4152,7 +4152,7 @@
         <v>295</v>
       </c>
       <c r="C11">
-        <v>-4.1</v>
+        <v>0.3</v>
       </c>
       <c r="D11">
         <v>5.6</v>
@@ -4172,7 +4172,7 @@
         <v>295</v>
       </c>
       <c r="C12">
-        <v>-6.8</v>
+        <v>-2.6</v>
       </c>
       <c r="D12">
         <v>5.8</v>
@@ -4192,7 +4192,7 @@
         <v>295</v>
       </c>
       <c r="C13">
-        <v>-7.4</v>
+        <v>3.6</v>
       </c>
       <c r="D13">
         <v>6.2</v>
@@ -4212,7 +4212,7 @@
         <v>295</v>
       </c>
       <c r="C14">
-        <v>-11.2</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>5.3</v>
@@ -4232,7 +4232,7 @@
         <v>295</v>
       </c>
       <c r="C15">
-        <v>-6.5</v>
+        <v>10.7</v>
       </c>
       <c r="D15">
         <v>6.7</v>
@@ -4252,7 +4252,7 @@
         <v>295</v>
       </c>
       <c r="C16">
-        <v>-7.6</v>
+        <v>3.6</v>
       </c>
       <c r="D16">
         <v>4.9</v>
@@ -4272,7 +4272,7 @@
         <v>295</v>
       </c>
       <c r="C17">
-        <v>-8</v>
+        <v>1.8</v>
       </c>
       <c r="D17">
         <v>4.7</v>
@@ -4333,7 +4333,7 @@
         <v>317</v>
       </c>
       <c r="C2">
-        <v>-12.4</v>
+        <v>-5.4</v>
       </c>
       <c r="D2">
         <v>6.2</v>
@@ -4353,7 +4353,7 @@
         <v>317</v>
       </c>
       <c r="C3">
-        <v>-6.5</v>
+        <v>-4.8</v>
       </c>
       <c r="D3">
         <v>3.7</v>
@@ -4373,7 +4373,7 @@
         <v>317</v>
       </c>
       <c r="C4">
-        <v>-25</v>
+        <v>7.4</v>
       </c>
       <c r="D4">
         <v>6.3</v>
@@ -4393,7 +4393,7 @@
         <v>317</v>
       </c>
       <c r="C5">
-        <v>-8.800000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="D5">
         <v>3.9</v>
@@ -4413,7 +4413,7 @@
         <v>317</v>
       </c>
       <c r="C6">
-        <v>-11.6</v>
+        <v>1.1</v>
       </c>
       <c r="D6">
         <v>8.5</v>
@@ -4433,7 +4433,7 @@
         <v>317</v>
       </c>
       <c r="C7">
-        <v>-11.4</v>
+        <v>0.5</v>
       </c>
       <c r="D7">
         <v>10.2</v>
@@ -4453,7 +4453,7 @@
         <v>317</v>
       </c>
       <c r="C8">
-        <v>-14.3</v>
+        <v>-0.6</v>
       </c>
       <c r="D8">
         <v>10.1</v>
@@ -4473,7 +4473,7 @@
         <v>317</v>
       </c>
       <c r="C9">
-        <v>-4.7</v>
+        <v>3.3</v>
       </c>
       <c r="D9">
         <v>8.199999999999999</v>
@@ -4493,7 +4493,7 @@
         <v>317</v>
       </c>
       <c r="C10">
-        <v>-6.7</v>
+        <v>3.4</v>
       </c>
       <c r="D10">
         <v>1.8</v>
@@ -4513,7 +4513,7 @@
         <v>317</v>
       </c>
       <c r="C11">
-        <v>-8.1</v>
+        <v>0.8</v>
       </c>
       <c r="D11">
         <v>5.9</v>
@@ -4533,7 +4533,7 @@
         <v>317</v>
       </c>
       <c r="C12">
-        <v>-7.4</v>
+        <v>3.9</v>
       </c>
       <c r="D12">
         <v>7.3</v>
@@ -4553,7 +4553,7 @@
         <v>317</v>
       </c>
       <c r="C13">
-        <v>-7</v>
+        <v>-1.5</v>
       </c>
       <c r="D13">
         <v>5.7</v>
@@ -4573,7 +4573,7 @@
         <v>317</v>
       </c>
       <c r="C14">
-        <v>-9.6</v>
+        <v>-0.3</v>
       </c>
       <c r="D14">
         <v>8.199999999999999</v>
@@ -4593,7 +4593,7 @@
         <v>317</v>
       </c>
       <c r="C15">
-        <v>-11.2</v>
+        <v>2.1</v>
       </c>
       <c r="D15">
         <v>8.300000000000001</v>
@@ -4613,7 +4613,7 @@
         <v>317</v>
       </c>
       <c r="C16">
-        <v>-6.7</v>
+        <v>4.2</v>
       </c>
       <c r="D16">
         <v>8</v>
@@ -4672,7 +4672,7 @@
         <v>329</v>
       </c>
       <c r="C2">
-        <v>-11.9</v>
+        <v>0.9</v>
       </c>
       <c r="D2">
         <v>7.2</v>
@@ -4692,7 +4692,7 @@
         <v>329</v>
       </c>
       <c r="C3">
-        <v>-5.3</v>
+        <v>2.2</v>
       </c>
       <c r="D3">
         <v>8.1</v>
@@ -4712,7 +4712,7 @@
         <v>329</v>
       </c>
       <c r="C4">
-        <v>-6.7</v>
+        <v>-3.8</v>
       </c>
       <c r="D4">
         <v>6.2</v>
@@ -4732,7 +4732,7 @@
         <v>329</v>
       </c>
       <c r="C5">
-        <v>-7</v>
+        <v>-1.4</v>
       </c>
       <c r="D5">
         <v>6.6</v>
@@ -4752,7 +4752,7 @@
         <v>329</v>
       </c>
       <c r="C6">
-        <v>-9.699999999999999</v>
+        <v>-16.8</v>
       </c>
       <c r="D6">
         <v>7.5</v>
@@ -4772,7 +4772,7 @@
         <v>329</v>
       </c>
       <c r="C7">
-        <v>-9</v>
+        <v>7.5</v>
       </c>
       <c r="D7">
         <v>5.9</v>
@@ -4792,7 +4792,7 @@
         <v>329</v>
       </c>
       <c r="C8">
-        <v>-12.1</v>
+        <v>29.1</v>
       </c>
       <c r="D8">
         <v>6.1</v>
@@ -4850,7 +4850,7 @@
         <v>343</v>
       </c>
       <c r="C2">
-        <v>-8.6</v>
+        <v>-0.9</v>
       </c>
       <c r="D2">
         <v>7.7</v>
@@ -4870,7 +4870,7 @@
         <v>343</v>
       </c>
       <c r="C3">
-        <v>-10</v>
+        <v>2.6</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -4890,7 +4890,7 @@
         <v>343</v>
       </c>
       <c r="C4">
-        <v>-7.9</v>
+        <v>0.6</v>
       </c>
       <c r="D4">
         <v>8.1</v>
@@ -4910,7 +4910,7 @@
         <v>343</v>
       </c>
       <c r="C5">
-        <v>-9.199999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D5">
         <v>7.7</v>
@@ -4930,7 +4930,7 @@
         <v>343</v>
       </c>
       <c r="C6">
-        <v>-4.5</v>
+        <v>5.7</v>
       </c>
       <c r="D6">
         <v>6.7</v>
@@ -4950,7 +4950,7 @@
         <v>343</v>
       </c>
       <c r="C7">
-        <v>-8.699999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
         <v>8.199999999999999</v>
@@ -4970,7 +4970,7 @@
         <v>343</v>
       </c>
       <c r="C8">
-        <v>-9.300000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="D8">
         <v>6.9</v>
@@ -4990,7 +4990,7 @@
         <v>343</v>
       </c>
       <c r="C9">
-        <v>-7.3</v>
+        <v>-2.1</v>
       </c>
       <c r="D9">
         <v>8.5</v>
@@ -5010,7 +5010,7 @@
         <v>343</v>
       </c>
       <c r="C10">
-        <v>-10.2</v>
+        <v>2.1</v>
       </c>
       <c r="D10">
         <v>8.300000000000001</v>
@@ -5030,7 +5030,7 @@
         <v>343</v>
       </c>
       <c r="C11">
-        <v>-19.6</v>
+        <v>14.6</v>
       </c>
       <c r="D11">
         <v>7.6</v>
@@ -5089,7 +5089,7 @@
         <v>397</v>
       </c>
       <c r="C2">
-        <v>-16.8</v>
+        <v>5.5</v>
       </c>
       <c r="D2">
         <v>7.8</v>
@@ -5109,7 +5109,7 @@
         <v>397</v>
       </c>
       <c r="C3">
-        <v>-11.6</v>
+        <v>-4.9</v>
       </c>
       <c r="D3">
         <v>5.7</v>
@@ -5129,7 +5129,7 @@
         <v>397</v>
       </c>
       <c r="C4">
-        <v>-14</v>
+        <v>0.1</v>
       </c>
       <c r="D4">
         <v>5.5</v>
@@ -5149,7 +5149,7 @@
         <v>397</v>
       </c>
       <c r="C5">
-        <v>-9.300000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
         <v>7.5</v>
@@ -5169,7 +5169,7 @@
         <v>397</v>
       </c>
       <c r="C6">
-        <v>-7.6</v>
+        <v>0.2</v>
       </c>
       <c r="D6">
         <v>6.9</v>
@@ -5189,7 +5189,7 @@
         <v>397</v>
       </c>
       <c r="C7">
-        <v>-8.800000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -5209,7 +5209,7 @@
         <v>397</v>
       </c>
       <c r="C8">
-        <v>-11.8</v>
+        <v>-2.7</v>
       </c>
       <c r="D8">
         <v>5.5</v>
@@ -5229,7 +5229,7 @@
         <v>397</v>
       </c>
       <c r="C9">
-        <v>-11.6</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -5249,7 +5249,7 @@
         <v>397</v>
       </c>
       <c r="C10">
-        <v>-7.5</v>
+        <v>-2</v>
       </c>
       <c r="D10">
         <v>5.5</v>
@@ -5269,7 +5269,7 @@
         <v>397</v>
       </c>
       <c r="C11">
-        <v>-7.4</v>
+        <v>1.5</v>
       </c>
       <c r="D11">
         <v>6.3</v>
@@ -5289,7 +5289,7 @@
         <v>397</v>
       </c>
       <c r="C12">
-        <v>-8.699999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="D12">
         <v>4.7</v>
@@ -5309,7 +5309,7 @@
         <v>397</v>
       </c>
       <c r="C13">
-        <v>-10.6</v>
+        <v>1.7</v>
       </c>
       <c r="D13">
         <v>8.1</v>
@@ -5329,7 +5329,7 @@
         <v>397</v>
       </c>
       <c r="C14">
-        <v>-5.1</v>
+        <v>-1.3</v>
       </c>
       <c r="D14">
         <v>5.8</v>
@@ -5349,7 +5349,7 @@
         <v>397</v>
       </c>
       <c r="C15">
-        <v>-11.7</v>
+        <v>1.7</v>
       </c>
       <c r="D15">
         <v>7.4</v>
@@ -5369,7 +5369,7 @@
         <v>397</v>
       </c>
       <c r="C16">
-        <v>-9.300000000000001</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>7.4</v>
@@ -5389,7 +5389,7 @@
         <v>397</v>
       </c>
       <c r="C17">
-        <v>-8.5</v>
+        <v>0.6</v>
       </c>
       <c r="D17">
         <v>9</v>
@@ -5409,7 +5409,7 @@
         <v>397</v>
       </c>
       <c r="C18">
-        <v>-13.3</v>
+        <v>0.9</v>
       </c>
       <c r="D18">
         <v>6.6</v>
@@ -5429,7 +5429,7 @@
         <v>397</v>
       </c>
       <c r="C19">
-        <v>-7.5</v>
+        <v>-0.1</v>
       </c>
       <c r="D19">
         <v>6.5</v>
@@ -5449,7 +5449,7 @@
         <v>397</v>
       </c>
       <c r="C20">
-        <v>-10.1</v>
+        <v>3.1</v>
       </c>
       <c r="D20">
         <v>8.9</v>
@@ -5469,7 +5469,7 @@
         <v>397</v>
       </c>
       <c r="C21">
-        <v>-4.1</v>
+        <v>-5.9</v>
       </c>
       <c r="D21">
         <v>6.3</v>
@@ -5489,7 +5489,7 @@
         <v>397</v>
       </c>
       <c r="C22">
-        <v>-6.5</v>
+        <v>-0.7</v>
       </c>
       <c r="D22">
         <v>7.1</v>
@@ -5509,7 +5509,7 @@
         <v>397</v>
       </c>
       <c r="C23">
-        <v>-7.8</v>
+        <v>41.6</v>
       </c>
       <c r="D23">
         <v>6.8</v>
@@ -5529,7 +5529,7 @@
         <v>397</v>
       </c>
       <c r="C24">
-        <v>2.3</v>
+        <v>-2.2</v>
       </c>
       <c r="D24">
         <v>5.8</v>
@@ -5549,7 +5549,7 @@
         <v>397</v>
       </c>
       <c r="C25">
-        <v>-9.300000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D25">
         <v>5.9</v>
@@ -5569,7 +5569,7 @@
         <v>397</v>
       </c>
       <c r="C26">
-        <v>-7</v>
+        <v>0.6</v>
       </c>
       <c r="D26">
         <v>5.5</v>
@@ -5589,7 +5589,7 @@
         <v>397</v>
       </c>
       <c r="C27">
-        <v>-26.8</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <v>7.6</v>
@@ -5609,7 +5609,7 @@
         <v>397</v>
       </c>
       <c r="C28">
-        <v>-9.699999999999999</v>
+        <v>2.7</v>
       </c>
       <c r="D28">
         <v>8.300000000000001</v>
@@ -5629,7 +5629,7 @@
         <v>397</v>
       </c>
       <c r="C29">
-        <v>-7.6</v>
+        <v>5.1</v>
       </c>
       <c r="D29">
         <v>7.6</v>
@@ -5649,7 +5649,7 @@
         <v>397</v>
       </c>
       <c r="C30">
-        <v>-9.1</v>
+        <v>-0.2</v>
       </c>
       <c r="D30">
         <v>7.8</v>
@@ -5669,7 +5669,7 @@
         <v>397</v>
       </c>
       <c r="C31">
-        <v>-8.5</v>
+        <v>-0.2</v>
       </c>
       <c r="D31">
         <v>6.3</v>
@@ -5689,7 +5689,7 @@
         <v>397</v>
       </c>
       <c r="C32">
-        <v>-20</v>
+        <v>427.3</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -5709,7 +5709,7 @@
         <v>397</v>
       </c>
       <c r="C33">
-        <v>-11.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D33">
         <v>8.300000000000001</v>
@@ -5729,7 +5729,7 @@
         <v>397</v>
       </c>
       <c r="C34">
-        <v>-32.1</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="D34">
         <v>8.199999999999999</v>
@@ -5749,7 +5749,7 @@
         <v>397</v>
       </c>
       <c r="C35">
-        <v>-11.8</v>
+        <v>7.4</v>
       </c>
       <c r="D35">
         <v>8</v>
@@ -5769,7 +5769,7 @@
         <v>397</v>
       </c>
       <c r="C36">
-        <v>-8.699999999999999</v>
+        <v>10.5</v>
       </c>
       <c r="D36">
         <v>7.1</v>
@@ -5789,7 +5789,7 @@
         <v>397</v>
       </c>
       <c r="C37">
-        <v>-7.9</v>
+        <v>3.3</v>
       </c>
       <c r="D37">
         <v>7.7</v>
@@ -5809,7 +5809,7 @@
         <v>397</v>
       </c>
       <c r="C38">
-        <v>-11.2</v>
+        <v>-0.9</v>
       </c>
       <c r="D38">
         <v>7.9</v>
@@ -5829,7 +5829,7 @@
         <v>397</v>
       </c>
       <c r="C39">
-        <v>10.5</v>
+        <v>13.2</v>
       </c>
       <c r="D39">
         <v>6.3</v>
@@ -5849,7 +5849,7 @@
         <v>397</v>
       </c>
       <c r="C40">
-        <v>-11.6</v>
+        <v>2.1</v>
       </c>
       <c r="D40">
         <v>8.199999999999999</v>
@@ -5869,7 +5869,7 @@
         <v>397</v>
       </c>
       <c r="C41">
-        <v>-4</v>
+        <v>0.7</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -5889,7 +5889,7 @@
         <v>397</v>
       </c>
       <c r="C42">
-        <v>-8.5</v>
+        <v>0.1</v>
       </c>
       <c r="D42">
         <v>7.7</v>
@@ -5909,7 +5909,7 @@
         <v>397</v>
       </c>
       <c r="C43">
-        <v>-11</v>
+        <v>1.4</v>
       </c>
       <c r="D43">
         <v>5.8</v>
@@ -5929,7 +5929,7 @@
         <v>397</v>
       </c>
       <c r="C44">
-        <v>-9.4</v>
+        <v>11.9</v>
       </c>
       <c r="D44">
         <v>8.4</v>
@@ -5949,7 +5949,7 @@
         <v>397</v>
       </c>
       <c r="C45">
-        <v>-8.5</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>5.4</v>
@@ -5969,7 +5969,7 @@
         <v>397</v>
       </c>
       <c r="C46">
-        <v>-10.1</v>
+        <v>0.2</v>
       </c>
       <c r="D46">
         <v>8.1</v>
@@ -5989,7 +5989,7 @@
         <v>397</v>
       </c>
       <c r="C47">
-        <v>-12.6</v>
+        <v>3.8</v>
       </c>
       <c r="D47">
         <v>6.9</v>
@@ -6009,7 +6009,7 @@
         <v>397</v>
       </c>
       <c r="C48">
-        <v>-7.5</v>
+        <v>1.3</v>
       </c>
       <c r="D48">
         <v>7.4</v>
@@ -6029,7 +6029,7 @@
         <v>397</v>
       </c>
       <c r="C49">
-        <v>-8.300000000000001</v>
+        <v>-0.1</v>
       </c>
       <c r="D49">
         <v>4.7</v>
@@ -6049,7 +6049,7 @@
         <v>397</v>
       </c>
       <c r="C50">
-        <v>-5.6</v>
+        <v>-8.1</v>
       </c>
       <c r="D50">
         <v>7.7</v>
@@ -6126,7 +6126,7 @@
         <v>31</v>
       </c>
       <c r="C2">
-        <v>-9.300000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="D2">
         <v>6.4</v>
@@ -6146,7 +6146,7 @@
         <v>31</v>
       </c>
       <c r="C3">
-        <v>-7.6</v>
+        <v>6.1</v>
       </c>
       <c r="D3">
         <v>6.9</v>
@@ -6166,7 +6166,7 @@
         <v>31</v>
       </c>
       <c r="C4">
-        <v>-8.5</v>
+        <v>1.4</v>
       </c>
       <c r="D4">
         <v>7.3</v>
@@ -6186,7 +6186,7 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>-9.699999999999999</v>
+        <v>-2.3</v>
       </c>
       <c r="D5">
         <v>7.9</v>
@@ -6206,7 +6206,7 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>0.6</v>
+        <v>-2.6</v>
       </c>
       <c r="D6">
         <v>7.3</v>
@@ -6226,7 +6226,7 @@
         <v>31</v>
       </c>
       <c r="C7">
-        <v>-8</v>
+        <v>4.8</v>
       </c>
       <c r="D7">
         <v>7.4</v>
@@ -6246,7 +6246,7 @@
         <v>31</v>
       </c>
       <c r="C8">
-        <v>-23.3</v>
+        <v>-0.3</v>
       </c>
       <c r="D8">
         <v>6.3</v>
@@ -6266,7 +6266,7 @@
         <v>31</v>
       </c>
       <c r="C9">
-        <v>-6.4</v>
+        <v>1.8</v>
       </c>
       <c r="D9">
         <v>6.8</v>
@@ -6286,7 +6286,7 @@
         <v>31</v>
       </c>
       <c r="C10">
-        <v>-6.7</v>
+        <v>-2.1</v>
       </c>
       <c r="D10">
         <v>7.6</v>
@@ -6306,7 +6306,7 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>-6.5</v>
+        <v>-0</v>
       </c>
       <c r="D11">
         <v>6.6</v>
@@ -6326,7 +6326,7 @@
         <v>31</v>
       </c>
       <c r="C12">
-        <v>3.3</v>
+        <v>-0.4</v>
       </c>
       <c r="D12">
         <v>6.7</v>
@@ -6346,7 +6346,7 @@
         <v>31</v>
       </c>
       <c r="C13">
-        <v>-15</v>
+        <v>23.5</v>
       </c>
       <c r="D13">
         <v>7.1</v>
@@ -6366,7 +6366,7 @@
         <v>31</v>
       </c>
       <c r="C14">
-        <v>-8.4</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
         <v>8.6</v>
@@ -6386,7 +6386,7 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>-7.8</v>
+        <v>0.3</v>
       </c>
       <c r="D15">
         <v>6.9</v>
@@ -6406,7 +6406,7 @@
         <v>31</v>
       </c>
       <c r="C16">
-        <v>-6.2</v>
+        <v>-1</v>
       </c>
       <c r="D16">
         <v>5.1</v>
@@ -6465,7 +6465,7 @@
         <v>432</v>
       </c>
       <c r="C2">
-        <v>-7</v>
+        <v>13.1</v>
       </c>
       <c r="D2">
         <v>8.199999999999999</v>
@@ -6485,7 +6485,7 @@
         <v>432</v>
       </c>
       <c r="C3">
-        <v>-13.1</v>
+        <v>2.9</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -6505,7 +6505,7 @@
         <v>432</v>
       </c>
       <c r="C4">
-        <v>-9.300000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -6525,7 +6525,7 @@
         <v>432</v>
       </c>
       <c r="C5">
-        <v>-12.4</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>2.3</v>
@@ -6545,7 +6545,7 @@
         <v>432</v>
       </c>
       <c r="C6">
-        <v>-8</v>
+        <v>-1</v>
       </c>
       <c r="D6">
         <v>6.7</v>
@@ -6565,7 +6565,7 @@
         <v>432</v>
       </c>
       <c r="C7">
-        <v>-5.5</v>
+        <v>8.4</v>
       </c>
       <c r="D7">
         <v>7.4</v>
@@ -6585,7 +6585,7 @@
         <v>432</v>
       </c>
       <c r="C8">
-        <v>-5.7</v>
+        <v>-3.1</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -6605,7 +6605,7 @@
         <v>432</v>
       </c>
       <c r="C9">
-        <v>-8</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
         <v>8.800000000000001</v>
@@ -6625,7 +6625,7 @@
         <v>432</v>
       </c>
       <c r="C10">
-        <v>-12.3</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D10">
         <v>6.3</v>
@@ -6645,7 +6645,7 @@
         <v>432</v>
       </c>
       <c r="C11">
-        <v>-0.3</v>
+        <v>-1.4</v>
       </c>
       <c r="D11">
         <v>6.2</v>
@@ -6665,7 +6665,7 @@
         <v>432</v>
       </c>
       <c r="C12">
-        <v>-8.6</v>
+        <v>1.1</v>
       </c>
       <c r="D12">
         <v>7.8</v>
@@ -6685,7 +6685,7 @@
         <v>432</v>
       </c>
       <c r="C13">
-        <v>-18.1</v>
+        <v>19.1</v>
       </c>
       <c r="D13">
         <v>6.8</v>
@@ -6745,7 +6745,7 @@
         <v>451</v>
       </c>
       <c r="C2">
-        <v>-12.2</v>
+        <v>16.2</v>
       </c>
       <c r="D2">
         <v>6.8</v>
@@ -6765,7 +6765,7 @@
         <v>451</v>
       </c>
       <c r="C3">
-        <v>-8.300000000000001</v>
+        <v>-0.4</v>
       </c>
       <c r="D3">
         <v>6.6</v>
@@ -6785,7 +6785,7 @@
         <v>451</v>
       </c>
       <c r="C4">
-        <v>-9.199999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="D4">
         <v>7.7</v>
@@ -6805,7 +6805,7 @@
         <v>451</v>
       </c>
       <c r="C5">
-        <v>-5</v>
+        <v>4.5</v>
       </c>
       <c r="D5">
         <v>7.8</v>
@@ -6825,7 +6825,7 @@
         <v>451</v>
       </c>
       <c r="C6">
-        <v>-9.199999999999999</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>8.300000000000001</v>
@@ -6845,7 +6845,7 @@
         <v>451</v>
       </c>
       <c r="C7">
-        <v>-9.4</v>
+        <v>3.3</v>
       </c>
       <c r="D7">
         <v>6.1</v>
@@ -6865,7 +6865,7 @@
         <v>451</v>
       </c>
       <c r="C8">
-        <v>-8.699999999999999</v>
+        <v>6.2</v>
       </c>
       <c r="D8">
         <v>6.9</v>
@@ -6885,7 +6885,7 @@
         <v>451</v>
       </c>
       <c r="C9">
-        <v>-12.4</v>
+        <v>1.2</v>
       </c>
       <c r="D9">
         <v>7.9</v>
@@ -6905,7 +6905,7 @@
         <v>451</v>
       </c>
       <c r="C10">
-        <v>-8.4</v>
+        <v>0.3</v>
       </c>
       <c r="D10">
         <v>8.300000000000001</v>
@@ -6925,7 +6925,7 @@
         <v>451</v>
       </c>
       <c r="C11">
-        <v>-12.3</v>
+        <v>4.5</v>
       </c>
       <c r="D11">
         <v>6.3</v>
@@ -6945,7 +6945,7 @@
         <v>451</v>
       </c>
       <c r="C12">
-        <v>-12.1</v>
+        <v>-1.1</v>
       </c>
       <c r="D12">
         <v>6.1</v>
@@ -6965,7 +6965,7 @@
         <v>451</v>
       </c>
       <c r="C13">
-        <v>-12.2</v>
+        <v>1.5</v>
       </c>
       <c r="D13">
         <v>7.8</v>
@@ -6985,7 +6985,7 @@
         <v>451</v>
       </c>
       <c r="C14">
-        <v>-10.9</v>
+        <v>0.1</v>
       </c>
       <c r="D14">
         <v>7.1</v>
@@ -7043,7 +7043,7 @@
         <v>38</v>
       </c>
       <c r="C2">
-        <v>-62.2</v>
+        <v>790.1</v>
       </c>
       <c r="D2">
         <v>6.6</v>
@@ -7099,7 +7099,7 @@
         <v>50</v>
       </c>
       <c r="C2">
-        <v>-3.8</v>
+        <v>4.1</v>
       </c>
       <c r="D2">
         <v>4.6</v>
@@ -7119,7 +7119,7 @@
         <v>50</v>
       </c>
       <c r="C3">
-        <v>-8.800000000000001</v>
+        <v>4.3</v>
       </c>
       <c r="D3">
         <v>6.1</v>
@@ -7139,7 +7139,7 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>-19.8</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>5.6</v>
@@ -7159,7 +7159,7 @@
         <v>50</v>
       </c>
       <c r="C5">
-        <v>-7.3</v>
+        <v>1.3</v>
       </c>
       <c r="D5">
         <v>6.8</v>
@@ -7179,7 +7179,7 @@
         <v>50</v>
       </c>
       <c r="C6">
-        <v>-8.800000000000001</v>
+        <v>-4.7</v>
       </c>
       <c r="D6">
         <v>3.8</v>
@@ -7199,7 +7199,7 @@
         <v>50</v>
       </c>
       <c r="C7">
-        <v>-9.1</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
         <v>7.4</v>
@@ -7219,7 +7219,7 @@
         <v>50</v>
       </c>
       <c r="C8">
-        <v>-9.9</v>
+        <v>-3</v>
       </c>
       <c r="D8">
         <v>6.5</v>
@@ -7239,7 +7239,7 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <v>-9.5</v>
+        <v>-4.6</v>
       </c>
       <c r="D9">
         <v>6.4</v>
@@ -7259,7 +7259,7 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>-11.2</v>
+        <v>-10.1</v>
       </c>
       <c r="D10">
         <v>4.7</v>
@@ -7279,7 +7279,7 @@
         <v>50</v>
       </c>
       <c r="C11">
-        <v>-11.5</v>
+        <v>-3.3</v>
       </c>
       <c r="D11">
         <v>6.1</v>
@@ -7338,7 +7338,7 @@
         <v>61</v>
       </c>
       <c r="C2">
-        <v>-12.2</v>
+        <v>4.3</v>
       </c>
       <c r="D2">
         <v>6.6</v>
@@ -7358,7 +7358,7 @@
         <v>61</v>
       </c>
       <c r="C3">
-        <v>-7.8</v>
+        <v>5.5</v>
       </c>
       <c r="D3">
         <v>6.7</v>
@@ -7378,7 +7378,7 @@
         <v>61</v>
       </c>
       <c r="C4">
-        <v>-4.5</v>
+        <v>12.1</v>
       </c>
       <c r="D4">
         <v>7.4</v>
@@ -7398,7 +7398,7 @@
         <v>61</v>
       </c>
       <c r="C5">
-        <v>-8.5</v>
+        <v>0.2</v>
       </c>
       <c r="D5">
         <v>8.1</v>
@@ -7418,7 +7418,7 @@
         <v>61</v>
       </c>
       <c r="C6">
-        <v>-10.9</v>
+        <v>-1.9</v>
       </c>
       <c r="D6">
         <v>6.1</v>
@@ -7438,7 +7438,7 @@
         <v>61</v>
       </c>
       <c r="C7">
-        <v>-9.6</v>
+        <v>-0.8</v>
       </c>
       <c r="D7">
         <v>7.1</v>
@@ -7495,7 +7495,7 @@
         <v>72</v>
       </c>
       <c r="C2">
-        <v>-8.300000000000001</v>
+        <v>-1.2</v>
       </c>
       <c r="D2">
         <v>8.1</v>
@@ -7515,7 +7515,7 @@
         <v>72</v>
       </c>
       <c r="C3">
-        <v>-7.4</v>
+        <v>-5.4</v>
       </c>
       <c r="D3">
         <v>7.1</v>
@@ -7535,7 +7535,7 @@
         <v>72</v>
       </c>
       <c r="C4">
-        <v>-6.5</v>
+        <v>-6.6</v>
       </c>
       <c r="D4">
         <v>4.7</v>
@@ -7555,7 +7555,7 @@
         <v>72</v>
       </c>
       <c r="C5">
-        <v>-6.5</v>
+        <v>-0.6</v>
       </c>
       <c r="D5">
         <v>9.300000000000001</v>
@@ -7575,7 +7575,7 @@
         <v>72</v>
       </c>
       <c r="C6">
-        <v>-10.3</v>
+        <v>-1</v>
       </c>
       <c r="D6">
         <v>5.1</v>
@@ -7595,7 +7595,7 @@
         <v>72</v>
       </c>
       <c r="C7">
-        <v>-5.7</v>
+        <v>5.1</v>
       </c>
       <c r="D7">
         <v>2.4</v>
@@ -7615,7 +7615,7 @@
         <v>72</v>
       </c>
       <c r="C8">
-        <v>-7.6</v>
+        <v>-1.6</v>
       </c>
       <c r="D8">
         <v>7.5</v>
@@ -7635,7 +7635,7 @@
         <v>72</v>
       </c>
       <c r="C9">
-        <v>-15.3</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -7692,7 +7692,7 @@
         <v>88</v>
       </c>
       <c r="C2">
-        <v>-8.300000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D2">
         <v>8.199999999999999</v>
@@ -7712,7 +7712,7 @@
         <v>88</v>
       </c>
       <c r="C3">
-        <v>-5.8</v>
+        <v>2.4</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -7732,7 +7732,7 @@
         <v>88</v>
       </c>
       <c r="C4">
-        <v>-11.7</v>
+        <v>1.4</v>
       </c>
       <c r="D4">
         <v>7.4</v>
@@ -7752,7 +7752,7 @@
         <v>88</v>
       </c>
       <c r="C5">
-        <v>-25.1</v>
+        <v>-5.9</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -7772,7 +7772,7 @@
         <v>88</v>
       </c>
       <c r="C6">
-        <v>-13.9</v>
+        <v>3.6</v>
       </c>
       <c r="D6">
         <v>7.8</v>
@@ -7792,7 +7792,7 @@
         <v>88</v>
       </c>
       <c r="C7">
-        <v>-5</v>
+        <v>1.6</v>
       </c>
       <c r="D7">
         <v>6.1</v>
@@ -7812,7 +7812,7 @@
         <v>88</v>
       </c>
       <c r="C8">
-        <v>-6.6</v>
+        <v>1.1</v>
       </c>
       <c r="D8">
         <v>7.8</v>
@@ -7832,7 +7832,7 @@
         <v>88</v>
       </c>
       <c r="C9">
-        <v>-8.800000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D9">
         <v>6.3</v>
@@ -7852,7 +7852,7 @@
         <v>88</v>
       </c>
       <c r="C10">
-        <v>-10.3</v>
+        <v>0.9</v>
       </c>
       <c r="D10">
         <v>6.4</v>
@@ -7872,7 +7872,7 @@
         <v>88</v>
       </c>
       <c r="C11">
-        <v>-6.7</v>
+        <v>-0.4</v>
       </c>
       <c r="D11">
         <v>7.1</v>
@@ -7892,7 +7892,7 @@
         <v>88</v>
       </c>
       <c r="C12">
-        <v>-7.9</v>
+        <v>0.3</v>
       </c>
       <c r="D12">
         <v>7.4</v>
@@ -7912,7 +7912,7 @@
         <v>88</v>
       </c>
       <c r="C13">
-        <v>-8.9</v>
+        <v>4.3</v>
       </c>
       <c r="D13">
         <v>6.4</v>
@@ -7932,7 +7932,7 @@
         <v>88</v>
       </c>
       <c r="C14">
-        <v>-8.5</v>
+        <v>0.7</v>
       </c>
       <c r="D14">
         <v>5.9</v>
@@ -7996,7 +7996,7 @@
         <v>110</v>
       </c>
       <c r="C2">
-        <v>-9.6</v>
+        <v>-3.7</v>
       </c>
       <c r="D2">
         <v>7.5</v>
@@ -8016,7 +8016,7 @@
         <v>110</v>
       </c>
       <c r="C3">
-        <v>-10.2</v>
+        <v>1.1</v>
       </c>
       <c r="D3">
         <v>5.3</v>
@@ -8036,7 +8036,7 @@
         <v>110</v>
       </c>
       <c r="C4">
-        <v>-9.9</v>
+        <v>4.1</v>
       </c>
       <c r="D4">
         <v>4.8</v>
@@ -8056,7 +8056,7 @@
         <v>110</v>
       </c>
       <c r="C5">
-        <v>-9.6</v>
+        <v>6.5</v>
       </c>
       <c r="D5">
         <v>4.8</v>
@@ -8076,7 +8076,7 @@
         <v>110</v>
       </c>
       <c r="C6">
-        <v>-9.199999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D6">
         <v>5.7</v>
@@ -8096,7 +8096,7 @@
         <v>110</v>
       </c>
       <c r="C7">
-        <v>-12.9</v>
+        <v>2.6</v>
       </c>
       <c r="D7">
         <v>6.5</v>
@@ -8116,7 +8116,7 @@
         <v>110</v>
       </c>
       <c r="C8">
-        <v>-6.9</v>
+        <v>1.5</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -8136,7 +8136,7 @@
         <v>110</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>7.7</v>
       </c>
       <c r="D9">
         <v>6.3</v>
@@ -8156,7 +8156,7 @@
         <v>110</v>
       </c>
       <c r="C10">
-        <v>-8.199999999999999</v>
+        <v>-4.4</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -8176,7 +8176,7 @@
         <v>110</v>
       </c>
       <c r="C11">
-        <v>-7.9</v>
+        <v>5.5</v>
       </c>
       <c r="D11">
         <v>6.2</v>
@@ -8196,7 +8196,7 @@
         <v>110</v>
       </c>
       <c r="C12">
-        <v>-13.4</v>
+        <v>2.8</v>
       </c>
       <c r="D12">
         <v>5.5</v>
@@ -8216,7 +8216,7 @@
         <v>110</v>
       </c>
       <c r="C13">
-        <v>-11.8</v>
+        <v>7.1</v>
       </c>
       <c r="D13">
         <v>5.8</v>
@@ -8274,7 +8274,7 @@
         <v>122</v>
       </c>
       <c r="C2">
-        <v>-10</v>
+        <v>0.4</v>
       </c>
       <c r="D2">
         <v>8.5</v>
@@ -8294,7 +8294,7 @@
         <v>122</v>
       </c>
       <c r="C3">
-        <v>-8.1</v>
+        <v>5.9</v>
       </c>
       <c r="D3">
         <v>7.9</v>
@@ -8314,7 +8314,7 @@
         <v>122</v>
       </c>
       <c r="C4">
-        <v>-6.4</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
         <v>5.9</v>
@@ -8334,7 +8334,7 @@
         <v>122</v>
       </c>
       <c r="C5">
-        <v>-7.3</v>
+        <v>-0.5</v>
       </c>
       <c r="D5">
         <v>6.6</v>
@@ -8354,7 +8354,7 @@
         <v>122</v>
       </c>
       <c r="C6">
-        <v>-8.6</v>
+        <v>1.4</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -8374,7 +8374,7 @@
         <v>122</v>
       </c>
       <c r="C7">
-        <v>-10.4</v>
+        <v>2.1</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -8394,7 +8394,7 @@
         <v>122</v>
       </c>
       <c r="C8">
-        <v>-19.8</v>
+        <v>-0.6</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -8414,7 +8414,7 @@
         <v>122</v>
       </c>
       <c r="C9">
-        <v>-9.800000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="D9">
         <v>7.1</v>

</xml_diff>

<commit_message>
update cement numbers for municipalities
</commit_message>
<xml_diff>
--- a/data/climate-data.xlsx
+++ b/data/climate-data.xlsx
@@ -5689,7 +5689,7 @@
         <v>397</v>
       </c>
       <c r="C32">
-        <v>427.3</v>
+        <v>21.8</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -7043,7 +7043,7 @@
         <v>38</v>
       </c>
       <c r="C2">
-        <v>790.1</v>
+        <v>-38.7</v>
       </c>
       <c r="D2">
         <v>6.6</v>

</xml_diff>

<commit_message>
Feat/update smhi data (#241)
* update smhi data and years

* update cement numbers

* update cement numbers for municipalities
</commit_message>
<xml_diff>
--- a/data/climate-data.xlsx
+++ b/data/climate-data.xlsx
@@ -42,7 +42,7 @@
     <t>Län</t>
   </si>
   <si>
-    <t>Utsläppsförändring 2019-2020 (%)</t>
+    <t>Utsläppsförändring 2020-2021 (%)</t>
   </si>
   <si>
     <t>KPI1: Förändringstakt andel laddbara bilar (%)</t>
@@ -1806,7 +1806,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1.7</v>
+        <v>85.09999999999999</v>
       </c>
       <c r="D2">
         <v>5.2</v>
@@ -1826,7 +1826,7 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>-7.9</v>
+        <v>-1.4</v>
       </c>
       <c r="D3">
         <v>7</v>
@@ -1846,7 +1846,7 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>-14</v>
+        <v>4.8</v>
       </c>
       <c r="D4">
         <v>4.8</v>
@@ -1866,7 +1866,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>-9.6</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>6.1</v>
@@ -1886,7 +1886,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>-19.6</v>
+        <v>5.4</v>
       </c>
       <c r="D6">
         <v>6.8</v>
@@ -1943,7 +1943,7 @@
         <v>143</v>
       </c>
       <c r="C2">
-        <v>-6.7</v>
+        <v>6.5</v>
       </c>
       <c r="D2">
         <v>6.4</v>
@@ -1963,7 +1963,7 @@
         <v>143</v>
       </c>
       <c r="C3">
-        <v>-10.7</v>
+        <v>2.2</v>
       </c>
       <c r="D3">
         <v>3.1</v>
@@ -1983,7 +1983,7 @@
         <v>143</v>
       </c>
       <c r="C4">
-        <v>-5.8</v>
+        <v>5.3</v>
       </c>
       <c r="D4">
         <v>6.1</v>
@@ -2003,7 +2003,7 @@
         <v>143</v>
       </c>
       <c r="C5">
-        <v>-11.1</v>
+        <v>-4.5</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -2023,7 +2023,7 @@
         <v>143</v>
       </c>
       <c r="C6">
-        <v>-4.6</v>
+        <v>-6.2</v>
       </c>
       <c r="D6">
         <v>3.9</v>
@@ -2043,7 +2043,7 @@
         <v>143</v>
       </c>
       <c r="C7">
-        <v>-6.8</v>
+        <v>5.6</v>
       </c>
       <c r="D7">
         <v>5.5</v>
@@ -2063,7 +2063,7 @@
         <v>143</v>
       </c>
       <c r="C8">
-        <v>-11.2</v>
+        <v>10.3</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -2083,7 +2083,7 @@
         <v>143</v>
       </c>
       <c r="C9">
-        <v>-1.4</v>
+        <v>-2.4</v>
       </c>
       <c r="D9">
         <v>3.9</v>
@@ -2103,7 +2103,7 @@
         <v>143</v>
       </c>
       <c r="C10">
-        <v>-3.1</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>7.6</v>
@@ -2123,7 +2123,7 @@
         <v>143</v>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>-1.3</v>
       </c>
       <c r="D11">
         <v>4.7</v>
@@ -2143,7 +2143,7 @@
         <v>143</v>
       </c>
       <c r="C12">
-        <v>-13.6</v>
+        <v>4.6</v>
       </c>
       <c r="D12">
         <v>8.4</v>
@@ -2163,7 +2163,7 @@
         <v>143</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>-8.1</v>
       </c>
       <c r="D13">
         <v>5.5</v>
@@ -2183,7 +2183,7 @@
         <v>143</v>
       </c>
       <c r="C14">
-        <v>-7.2</v>
+        <v>-0.7</v>
       </c>
       <c r="D14">
         <v>3.8</v>
@@ -2203,7 +2203,7 @@
         <v>143</v>
       </c>
       <c r="C15">
-        <v>-7.8</v>
+        <v>-3.2</v>
       </c>
       <c r="D15">
         <v>6.8</v>
@@ -2262,7 +2262,7 @@
         <v>182</v>
       </c>
       <c r="C2">
-        <v>-5.5</v>
+        <v>1.3</v>
       </c>
       <c r="D2">
         <v>4.6</v>
@@ -2282,7 +2282,7 @@
         <v>182</v>
       </c>
       <c r="C3">
-        <v>-23.8</v>
+        <v>6.7</v>
       </c>
       <c r="D3">
         <v>7.1</v>
@@ -2302,7 +2302,7 @@
         <v>182</v>
       </c>
       <c r="C4">
-        <v>-16.1</v>
+        <v>-11.6</v>
       </c>
       <c r="D4">
         <v>4.8</v>
@@ -2322,7 +2322,7 @@
         <v>182</v>
       </c>
       <c r="C5">
-        <v>-8.9</v>
+        <v>0.6</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -2342,7 +2342,7 @@
         <v>182</v>
       </c>
       <c r="C6">
-        <v>31.3</v>
+        <v>-2.4</v>
       </c>
       <c r="D6">
         <v>5.9</v>
@@ -2362,7 +2362,7 @@
         <v>182</v>
       </c>
       <c r="C7">
-        <v>-6.2</v>
+        <v>1.5</v>
       </c>
       <c r="D7">
         <v>6.3</v>
@@ -2382,7 +2382,7 @@
         <v>182</v>
       </c>
       <c r="C8">
-        <v>3.5</v>
+        <v>-11.6</v>
       </c>
       <c r="D8">
         <v>5.6</v>
@@ -2402,7 +2402,7 @@
         <v>182</v>
       </c>
       <c r="C9">
-        <v>-5.4</v>
+        <v>19.2</v>
       </c>
       <c r="D9">
         <v>7.3</v>
@@ -2422,7 +2422,7 @@
         <v>182</v>
       </c>
       <c r="C10">
-        <v>-8.800000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -2442,7 +2442,7 @@
         <v>182</v>
       </c>
       <c r="C11">
-        <v>-8.800000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D11">
         <v>6.3</v>
@@ -2462,7 +2462,7 @@
         <v>182</v>
       </c>
       <c r="C12">
-        <v>-2.9</v>
+        <v>1.1</v>
       </c>
       <c r="D12">
         <v>6.4</v>
@@ -2482,7 +2482,7 @@
         <v>182</v>
       </c>
       <c r="C13">
-        <v>-8.800000000000001</v>
+        <v>-1.7</v>
       </c>
       <c r="D13">
         <v>7.5</v>
@@ -2502,7 +2502,7 @@
         <v>182</v>
       </c>
       <c r="C14">
-        <v>-7.9</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
         <v>9.300000000000001</v>
@@ -2522,7 +2522,7 @@
         <v>182</v>
       </c>
       <c r="C15">
-        <v>-7.5</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>7.4</v>
@@ -2542,7 +2542,7 @@
         <v>182</v>
       </c>
       <c r="C16">
-        <v>-7.5</v>
+        <v>0.3</v>
       </c>
       <c r="D16">
         <v>9</v>
@@ -2562,7 +2562,7 @@
         <v>182</v>
       </c>
       <c r="C17">
-        <v>-9.300000000000001</v>
+        <v>-3.3</v>
       </c>
       <c r="D17">
         <v>10.4</v>
@@ -2582,7 +2582,7 @@
         <v>182</v>
       </c>
       <c r="C18">
-        <v>-16.6</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>6.4</v>
@@ -2602,7 +2602,7 @@
         <v>182</v>
       </c>
       <c r="C19">
-        <v>-11.5</v>
+        <v>-0.9</v>
       </c>
       <c r="D19">
         <v>5.4</v>
@@ -2622,7 +2622,7 @@
         <v>182</v>
       </c>
       <c r="C20">
-        <v>-0.8</v>
+        <v>1.1</v>
       </c>
       <c r="D20">
         <v>6.4</v>
@@ -2642,7 +2642,7 @@
         <v>182</v>
       </c>
       <c r="C21">
-        <v>-10.5</v>
+        <v>0.2</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -2662,7 +2662,7 @@
         <v>182</v>
       </c>
       <c r="C22">
-        <v>-7.8</v>
+        <v>0.4</v>
       </c>
       <c r="D22">
         <v>6.6</v>
@@ -2682,7 +2682,7 @@
         <v>182</v>
       </c>
       <c r="C23">
-        <v>-7.1</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>6.6</v>
@@ -2702,7 +2702,7 @@
         <v>182</v>
       </c>
       <c r="C24">
-        <v>-7.6</v>
+        <v>0.1</v>
       </c>
       <c r="D24">
         <v>8.199999999999999</v>
@@ -2722,7 +2722,7 @@
         <v>182</v>
       </c>
       <c r="C25">
-        <v>-10</v>
+        <v>2.6</v>
       </c>
       <c r="D25">
         <v>6.7</v>
@@ -2742,7 +2742,7 @@
         <v>182</v>
       </c>
       <c r="C26">
-        <v>-9.199999999999999</v>
+        <v>4.6</v>
       </c>
       <c r="D26">
         <v>7.5</v>
@@ -2762,7 +2762,7 @@
         <v>182</v>
       </c>
       <c r="C27">
-        <v>-7.2</v>
+        <v>-5.7</v>
       </c>
       <c r="D27">
         <v>2.9</v>
@@ -2782,7 +2782,7 @@
         <v>182</v>
       </c>
       <c r="C28">
-        <v>-9.800000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="D28">
         <v>7.3</v>
@@ -2802,7 +2802,7 @@
         <v>182</v>
       </c>
       <c r="C29">
-        <v>-6.5</v>
+        <v>-0.5</v>
       </c>
       <c r="D29">
         <v>8.4</v>
@@ -2822,7 +2822,7 @@
         <v>182</v>
       </c>
       <c r="C30">
-        <v>-7.3</v>
+        <v>0.3</v>
       </c>
       <c r="D30">
         <v>5.7</v>
@@ -2842,7 +2842,7 @@
         <v>182</v>
       </c>
       <c r="C31">
-        <v>-7.7</v>
+        <v>-2.3</v>
       </c>
       <c r="D31">
         <v>6.3</v>
@@ -2862,7 +2862,7 @@
         <v>182</v>
       </c>
       <c r="C32">
-        <v>-11</v>
+        <v>1.9</v>
       </c>
       <c r="D32">
         <v>7.2</v>
@@ -2882,7 +2882,7 @@
         <v>182</v>
       </c>
       <c r="C33">
-        <v>-7.8</v>
+        <v>1.1</v>
       </c>
       <c r="D33">
         <v>3.3</v>
@@ -2902,7 +2902,7 @@
         <v>182</v>
       </c>
       <c r="C34">
-        <v>-10</v>
+        <v>-0.8</v>
       </c>
       <c r="D34">
         <v>7.5</v>
@@ -2976,7 +2976,7 @@
         <v>228</v>
       </c>
       <c r="C2">
-        <v>-9.1</v>
+        <v>-0.3</v>
       </c>
       <c r="D2">
         <v>6.4</v>
@@ -2996,7 +2996,7 @@
         <v>228</v>
       </c>
       <c r="C3">
-        <v>-8.5</v>
+        <v>1.3</v>
       </c>
       <c r="D3">
         <v>10.5</v>
@@ -3016,7 +3016,7 @@
         <v>228</v>
       </c>
       <c r="C4">
-        <v>-11.1</v>
+        <v>7.4</v>
       </c>
       <c r="D4">
         <v>9.1</v>
@@ -3036,7 +3036,7 @@
         <v>228</v>
       </c>
       <c r="C5">
-        <v>-7</v>
+        <v>-3.1</v>
       </c>
       <c r="D5">
         <v>6.7</v>
@@ -3056,7 +3056,7 @@
         <v>228</v>
       </c>
       <c r="C6">
-        <v>-8.9</v>
+        <v>0.3</v>
       </c>
       <c r="D6">
         <v>6.9</v>
@@ -3076,7 +3076,7 @@
         <v>228</v>
       </c>
       <c r="C7">
-        <v>-9.4</v>
+        <v>0.3</v>
       </c>
       <c r="D7">
         <v>8.199999999999999</v>
@@ -3096,7 +3096,7 @@
         <v>228</v>
       </c>
       <c r="C8">
-        <v>7.3</v>
+        <v>9.6</v>
       </c>
       <c r="D8">
         <v>8.6</v>
@@ -3116,7 +3116,7 @@
         <v>228</v>
       </c>
       <c r="C9">
-        <v>-8.699999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D9">
         <v>9.4</v>
@@ -3136,7 +3136,7 @@
         <v>228</v>
       </c>
       <c r="C10">
-        <v>-8.9</v>
+        <v>2.7</v>
       </c>
       <c r="D10">
         <v>6.3</v>
@@ -3156,7 +3156,7 @@
         <v>228</v>
       </c>
       <c r="C11">
-        <v>-9.5</v>
+        <v>0.1</v>
       </c>
       <c r="D11">
         <v>6.5</v>
@@ -3176,7 +3176,7 @@
         <v>228</v>
       </c>
       <c r="C12">
-        <v>-8.4</v>
+        <v>-1.6</v>
       </c>
       <c r="D12">
         <v>7.3</v>
@@ -3196,7 +3196,7 @@
         <v>228</v>
       </c>
       <c r="C13">
-        <v>-8.199999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="D13">
         <v>7.1</v>
@@ -3216,7 +3216,7 @@
         <v>228</v>
       </c>
       <c r="C14">
-        <v>-8.800000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="D14">
         <v>8.199999999999999</v>
@@ -3236,7 +3236,7 @@
         <v>228</v>
       </c>
       <c r="C15">
-        <v>-8.6</v>
+        <v>0.5</v>
       </c>
       <c r="D15">
         <v>9.4</v>
@@ -3256,7 +3256,7 @@
         <v>228</v>
       </c>
       <c r="C16">
-        <v>-8.5</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>9.1</v>
@@ -3276,7 +3276,7 @@
         <v>228</v>
       </c>
       <c r="C17">
-        <v>-27.4</v>
+        <v>5.6</v>
       </c>
       <c r="D17">
         <v>9.1</v>
@@ -3296,7 +3296,7 @@
         <v>228</v>
       </c>
       <c r="C18">
-        <v>-8.9</v>
+        <v>-0</v>
       </c>
       <c r="D18">
         <v>11.3</v>
@@ -3316,7 +3316,7 @@
         <v>228</v>
       </c>
       <c r="C19">
-        <v>-41.6</v>
+        <v>-1.7</v>
       </c>
       <c r="D19">
         <v>7.7</v>
@@ -3336,7 +3336,7 @@
         <v>228</v>
       </c>
       <c r="C20">
-        <v>-8.6</v>
+        <v>0.7</v>
       </c>
       <c r="D20">
         <v>8.300000000000001</v>
@@ -3356,7 +3356,7 @@
         <v>228</v>
       </c>
       <c r="C21">
-        <v>-9.199999999999999</v>
+        <v>0.4</v>
       </c>
       <c r="D21">
         <v>8.699999999999999</v>
@@ -3376,7 +3376,7 @@
         <v>228</v>
       </c>
       <c r="C22">
-        <v>-13.4</v>
+        <v>0.6</v>
       </c>
       <c r="D22">
         <v>7.7</v>
@@ -3396,7 +3396,7 @@
         <v>228</v>
       </c>
       <c r="C23">
-        <v>109</v>
+        <v>2.6</v>
       </c>
       <c r="D23">
         <v>8.199999999999999</v>
@@ -3416,7 +3416,7 @@
         <v>228</v>
       </c>
       <c r="C24">
-        <v>-10</v>
+        <v>0.7</v>
       </c>
       <c r="D24">
         <v>8.9</v>
@@ -3436,7 +3436,7 @@
         <v>228</v>
       </c>
       <c r="C25">
-        <v>-4.9</v>
+        <v>12.3</v>
       </c>
       <c r="D25">
         <v>8.5</v>
@@ -3456,7 +3456,7 @@
         <v>228</v>
       </c>
       <c r="C26">
-        <v>-7.8</v>
+        <v>6.8</v>
       </c>
       <c r="D26">
         <v>9.699999999999999</v>
@@ -3476,7 +3476,7 @@
         <v>228</v>
       </c>
       <c r="C27">
-        <v>-9.300000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D27">
         <v>7.9</v>
@@ -3553,7 +3553,7 @@
         <v>260</v>
       </c>
       <c r="C2">
-        <v>-9.300000000000001</v>
+        <v>3.8</v>
       </c>
       <c r="D2">
         <v>7.4</v>
@@ -3573,7 +3573,7 @@
         <v>260</v>
       </c>
       <c r="C3">
-        <v>-9.300000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="D3">
         <v>6.6</v>
@@ -3593,7 +3593,7 @@
         <v>260</v>
       </c>
       <c r="C4">
-        <v>-12.6</v>
+        <v>3.3</v>
       </c>
       <c r="D4">
         <v>7.9</v>
@@ -3613,7 +3613,7 @@
         <v>260</v>
       </c>
       <c r="C5">
-        <v>-8.1</v>
+        <v>3.5</v>
       </c>
       <c r="D5">
         <v>6.8</v>
@@ -3633,7 +3633,7 @@
         <v>260</v>
       </c>
       <c r="C6">
-        <v>-7.9</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>6.7</v>
@@ -3653,7 +3653,7 @@
         <v>260</v>
       </c>
       <c r="C7">
-        <v>-27.4</v>
+        <v>8.9</v>
       </c>
       <c r="D7">
         <v>6.9</v>
@@ -3673,7 +3673,7 @@
         <v>260</v>
       </c>
       <c r="C8">
-        <v>-4</v>
+        <v>2.4</v>
       </c>
       <c r="D8">
         <v>6.1</v>
@@ -3693,7 +3693,7 @@
         <v>260</v>
       </c>
       <c r="C9">
-        <v>-10.3</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -3713,7 +3713,7 @@
         <v>260</v>
       </c>
       <c r="C10">
-        <v>-12.7</v>
+        <v>1.4</v>
       </c>
       <c r="D10">
         <v>6.4</v>
@@ -3773,7 +3773,7 @@
         <v>274</v>
       </c>
       <c r="C2">
-        <v>-9.1</v>
+        <v>-2.1</v>
       </c>
       <c r="D2">
         <v>7.3</v>
@@ -3793,7 +3793,7 @@
         <v>274</v>
       </c>
       <c r="C3">
-        <v>-6.9</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>7.3</v>
@@ -3813,7 +3813,7 @@
         <v>274</v>
       </c>
       <c r="C4">
-        <v>-8.5</v>
+        <v>5.6</v>
       </c>
       <c r="D4">
         <v>6.3</v>
@@ -3833,7 +3833,7 @@
         <v>274</v>
       </c>
       <c r="C5">
-        <v>-12.5</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>9.6</v>
@@ -3853,7 +3853,7 @@
         <v>274</v>
       </c>
       <c r="C6">
-        <v>-10.9</v>
+        <v>-1.3</v>
       </c>
       <c r="D6">
         <v>8.1</v>
@@ -3873,7 +3873,7 @@
         <v>274</v>
       </c>
       <c r="C7">
-        <v>-24.2</v>
+        <v>2.9</v>
       </c>
       <c r="D7">
         <v>7.6</v>
@@ -3893,7 +3893,7 @@
         <v>274</v>
       </c>
       <c r="C8">
-        <v>-8.6</v>
+        <v>1.8</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -3913,7 +3913,7 @@
         <v>274</v>
       </c>
       <c r="C9">
-        <v>-17.8</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>5.8</v>
@@ -3972,7 +3972,7 @@
         <v>295</v>
       </c>
       <c r="C2">
-        <v>-10.2</v>
+        <v>4.6</v>
       </c>
       <c r="D2">
         <v>6.3</v>
@@ -3992,7 +3992,7 @@
         <v>295</v>
       </c>
       <c r="C3">
-        <v>-5</v>
+        <v>7.9</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -4012,7 +4012,7 @@
         <v>295</v>
       </c>
       <c r="C4">
-        <v>-8.6</v>
+        <v>-1.3</v>
       </c>
       <c r="D4">
         <v>4.8</v>
@@ -4032,7 +4032,7 @@
         <v>295</v>
       </c>
       <c r="C5">
-        <v>-7.6</v>
+        <v>4.2</v>
       </c>
       <c r="D5">
         <v>7.1</v>
@@ -4052,7 +4052,7 @@
         <v>295</v>
       </c>
       <c r="C6">
-        <v>-13.7</v>
+        <v>-8.199999999999999</v>
       </c>
       <c r="D6">
         <v>7.6</v>
@@ -4072,7 +4072,7 @@
         <v>295</v>
       </c>
       <c r="C7">
-        <v>-7.7</v>
+        <v>16.7</v>
       </c>
       <c r="D7">
         <v>2.4</v>
@@ -4092,7 +4092,7 @@
         <v>295</v>
       </c>
       <c r="C8">
-        <v>-17.1</v>
+        <v>3.8</v>
       </c>
       <c r="D8">
         <v>7.1</v>
@@ -4112,7 +4112,7 @@
         <v>295</v>
       </c>
       <c r="C9">
-        <v>-6.6</v>
+        <v>1.5</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -4132,7 +4132,7 @@
         <v>295</v>
       </c>
       <c r="C10">
-        <v>-6.7</v>
+        <v>5.8</v>
       </c>
       <c r="D10">
         <v>6.4</v>
@@ -4152,7 +4152,7 @@
         <v>295</v>
       </c>
       <c r="C11">
-        <v>-4.1</v>
+        <v>0.3</v>
       </c>
       <c r="D11">
         <v>5.6</v>
@@ -4172,7 +4172,7 @@
         <v>295</v>
       </c>
       <c r="C12">
-        <v>-6.8</v>
+        <v>-2.6</v>
       </c>
       <c r="D12">
         <v>5.8</v>
@@ -4192,7 +4192,7 @@
         <v>295</v>
       </c>
       <c r="C13">
-        <v>-7.4</v>
+        <v>3.6</v>
       </c>
       <c r="D13">
         <v>6.2</v>
@@ -4212,7 +4212,7 @@
         <v>295</v>
       </c>
       <c r="C14">
-        <v>-11.2</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>5.3</v>
@@ -4232,7 +4232,7 @@
         <v>295</v>
       </c>
       <c r="C15">
-        <v>-6.5</v>
+        <v>10.7</v>
       </c>
       <c r="D15">
         <v>6.7</v>
@@ -4252,7 +4252,7 @@
         <v>295</v>
       </c>
       <c r="C16">
-        <v>-7.6</v>
+        <v>3.6</v>
       </c>
       <c r="D16">
         <v>4.9</v>
@@ -4272,7 +4272,7 @@
         <v>295</v>
       </c>
       <c r="C17">
-        <v>-8</v>
+        <v>1.8</v>
       </c>
       <c r="D17">
         <v>4.7</v>
@@ -4333,7 +4333,7 @@
         <v>317</v>
       </c>
       <c r="C2">
-        <v>-12.4</v>
+        <v>-5.4</v>
       </c>
       <c r="D2">
         <v>6.2</v>
@@ -4353,7 +4353,7 @@
         <v>317</v>
       </c>
       <c r="C3">
-        <v>-6.5</v>
+        <v>-4.8</v>
       </c>
       <c r="D3">
         <v>3.7</v>
@@ -4373,7 +4373,7 @@
         <v>317</v>
       </c>
       <c r="C4">
-        <v>-25</v>
+        <v>7.4</v>
       </c>
       <c r="D4">
         <v>6.3</v>
@@ -4393,7 +4393,7 @@
         <v>317</v>
       </c>
       <c r="C5">
-        <v>-8.800000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="D5">
         <v>3.9</v>
@@ -4413,7 +4413,7 @@
         <v>317</v>
       </c>
       <c r="C6">
-        <v>-11.6</v>
+        <v>1.1</v>
       </c>
       <c r="D6">
         <v>8.5</v>
@@ -4433,7 +4433,7 @@
         <v>317</v>
       </c>
       <c r="C7">
-        <v>-11.4</v>
+        <v>0.5</v>
       </c>
       <c r="D7">
         <v>10.2</v>
@@ -4453,7 +4453,7 @@
         <v>317</v>
       </c>
       <c r="C8">
-        <v>-14.3</v>
+        <v>-0.6</v>
       </c>
       <c r="D8">
         <v>10.1</v>
@@ -4473,7 +4473,7 @@
         <v>317</v>
       </c>
       <c r="C9">
-        <v>-4.7</v>
+        <v>3.3</v>
       </c>
       <c r="D9">
         <v>8.199999999999999</v>
@@ -4493,7 +4493,7 @@
         <v>317</v>
       </c>
       <c r="C10">
-        <v>-6.7</v>
+        <v>3.4</v>
       </c>
       <c r="D10">
         <v>1.8</v>
@@ -4513,7 +4513,7 @@
         <v>317</v>
       </c>
       <c r="C11">
-        <v>-8.1</v>
+        <v>0.8</v>
       </c>
       <c r="D11">
         <v>5.9</v>
@@ -4533,7 +4533,7 @@
         <v>317</v>
       </c>
       <c r="C12">
-        <v>-7.4</v>
+        <v>3.9</v>
       </c>
       <c r="D12">
         <v>7.3</v>
@@ -4553,7 +4553,7 @@
         <v>317</v>
       </c>
       <c r="C13">
-        <v>-7</v>
+        <v>-1.5</v>
       </c>
       <c r="D13">
         <v>5.7</v>
@@ -4573,7 +4573,7 @@
         <v>317</v>
       </c>
       <c r="C14">
-        <v>-9.6</v>
+        <v>-0.3</v>
       </c>
       <c r="D14">
         <v>8.199999999999999</v>
@@ -4593,7 +4593,7 @@
         <v>317</v>
       </c>
       <c r="C15">
-        <v>-11.2</v>
+        <v>2.1</v>
       </c>
       <c r="D15">
         <v>8.300000000000001</v>
@@ -4613,7 +4613,7 @@
         <v>317</v>
       </c>
       <c r="C16">
-        <v>-6.7</v>
+        <v>4.2</v>
       </c>
       <c r="D16">
         <v>8</v>
@@ -4672,7 +4672,7 @@
         <v>329</v>
       </c>
       <c r="C2">
-        <v>-11.9</v>
+        <v>0.9</v>
       </c>
       <c r="D2">
         <v>7.2</v>
@@ -4692,7 +4692,7 @@
         <v>329</v>
       </c>
       <c r="C3">
-        <v>-5.3</v>
+        <v>2.2</v>
       </c>
       <c r="D3">
         <v>8.1</v>
@@ -4712,7 +4712,7 @@
         <v>329</v>
       </c>
       <c r="C4">
-        <v>-6.7</v>
+        <v>-3.8</v>
       </c>
       <c r="D4">
         <v>6.2</v>
@@ -4732,7 +4732,7 @@
         <v>329</v>
       </c>
       <c r="C5">
-        <v>-7</v>
+        <v>-1.4</v>
       </c>
       <c r="D5">
         <v>6.6</v>
@@ -4752,7 +4752,7 @@
         <v>329</v>
       </c>
       <c r="C6">
-        <v>-9.699999999999999</v>
+        <v>-16.8</v>
       </c>
       <c r="D6">
         <v>7.5</v>
@@ -4772,7 +4772,7 @@
         <v>329</v>
       </c>
       <c r="C7">
-        <v>-9</v>
+        <v>7.5</v>
       </c>
       <c r="D7">
         <v>5.9</v>
@@ -4792,7 +4792,7 @@
         <v>329</v>
       </c>
       <c r="C8">
-        <v>-12.1</v>
+        <v>29.1</v>
       </c>
       <c r="D8">
         <v>6.1</v>
@@ -4850,7 +4850,7 @@
         <v>343</v>
       </c>
       <c r="C2">
-        <v>-8.6</v>
+        <v>-0.9</v>
       </c>
       <c r="D2">
         <v>7.7</v>
@@ -4870,7 +4870,7 @@
         <v>343</v>
       </c>
       <c r="C3">
-        <v>-10</v>
+        <v>2.6</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -4890,7 +4890,7 @@
         <v>343</v>
       </c>
       <c r="C4">
-        <v>-7.9</v>
+        <v>0.6</v>
       </c>
       <c r="D4">
         <v>8.1</v>
@@ -4910,7 +4910,7 @@
         <v>343</v>
       </c>
       <c r="C5">
-        <v>-9.199999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D5">
         <v>7.7</v>
@@ -4930,7 +4930,7 @@
         <v>343</v>
       </c>
       <c r="C6">
-        <v>-4.5</v>
+        <v>5.7</v>
       </c>
       <c r="D6">
         <v>6.7</v>
@@ -4950,7 +4950,7 @@
         <v>343</v>
       </c>
       <c r="C7">
-        <v>-8.699999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
         <v>8.199999999999999</v>
@@ -4970,7 +4970,7 @@
         <v>343</v>
       </c>
       <c r="C8">
-        <v>-9.300000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="D8">
         <v>6.9</v>
@@ -4990,7 +4990,7 @@
         <v>343</v>
       </c>
       <c r="C9">
-        <v>-7.3</v>
+        <v>-2.1</v>
       </c>
       <c r="D9">
         <v>8.5</v>
@@ -5010,7 +5010,7 @@
         <v>343</v>
       </c>
       <c r="C10">
-        <v>-10.2</v>
+        <v>2.1</v>
       </c>
       <c r="D10">
         <v>8.300000000000001</v>
@@ -5030,7 +5030,7 @@
         <v>343</v>
       </c>
       <c r="C11">
-        <v>-19.6</v>
+        <v>14.6</v>
       </c>
       <c r="D11">
         <v>7.6</v>
@@ -5089,7 +5089,7 @@
         <v>397</v>
       </c>
       <c r="C2">
-        <v>-16.8</v>
+        <v>5.5</v>
       </c>
       <c r="D2">
         <v>7.8</v>
@@ -5109,7 +5109,7 @@
         <v>397</v>
       </c>
       <c r="C3">
-        <v>-11.6</v>
+        <v>-4.9</v>
       </c>
       <c r="D3">
         <v>5.7</v>
@@ -5129,7 +5129,7 @@
         <v>397</v>
       </c>
       <c r="C4">
-        <v>-14</v>
+        <v>0.1</v>
       </c>
       <c r="D4">
         <v>5.5</v>
@@ -5149,7 +5149,7 @@
         <v>397</v>
       </c>
       <c r="C5">
-        <v>-9.300000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
         <v>7.5</v>
@@ -5169,7 +5169,7 @@
         <v>397</v>
       </c>
       <c r="C6">
-        <v>-7.6</v>
+        <v>0.2</v>
       </c>
       <c r="D6">
         <v>6.9</v>
@@ -5189,7 +5189,7 @@
         <v>397</v>
       </c>
       <c r="C7">
-        <v>-8.800000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -5209,7 +5209,7 @@
         <v>397</v>
       </c>
       <c r="C8">
-        <v>-11.8</v>
+        <v>-2.7</v>
       </c>
       <c r="D8">
         <v>5.5</v>
@@ -5229,7 +5229,7 @@
         <v>397</v>
       </c>
       <c r="C9">
-        <v>-11.6</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -5249,7 +5249,7 @@
         <v>397</v>
       </c>
       <c r="C10">
-        <v>-7.5</v>
+        <v>-2</v>
       </c>
       <c r="D10">
         <v>5.5</v>
@@ -5269,7 +5269,7 @@
         <v>397</v>
       </c>
       <c r="C11">
-        <v>-7.4</v>
+        <v>1.5</v>
       </c>
       <c r="D11">
         <v>6.3</v>
@@ -5289,7 +5289,7 @@
         <v>397</v>
       </c>
       <c r="C12">
-        <v>-8.699999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="D12">
         <v>4.7</v>
@@ -5309,7 +5309,7 @@
         <v>397</v>
       </c>
       <c r="C13">
-        <v>-10.6</v>
+        <v>1.7</v>
       </c>
       <c r="D13">
         <v>8.1</v>
@@ -5329,7 +5329,7 @@
         <v>397</v>
       </c>
       <c r="C14">
-        <v>-5.1</v>
+        <v>-1.3</v>
       </c>
       <c r="D14">
         <v>5.8</v>
@@ -5349,7 +5349,7 @@
         <v>397</v>
       </c>
       <c r="C15">
-        <v>-11.7</v>
+        <v>1.7</v>
       </c>
       <c r="D15">
         <v>7.4</v>
@@ -5369,7 +5369,7 @@
         <v>397</v>
       </c>
       <c r="C16">
-        <v>-9.300000000000001</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>7.4</v>
@@ -5389,7 +5389,7 @@
         <v>397</v>
       </c>
       <c r="C17">
-        <v>-8.5</v>
+        <v>0.6</v>
       </c>
       <c r="D17">
         <v>9</v>
@@ -5409,7 +5409,7 @@
         <v>397</v>
       </c>
       <c r="C18">
-        <v>-13.3</v>
+        <v>0.9</v>
       </c>
       <c r="D18">
         <v>6.6</v>
@@ -5429,7 +5429,7 @@
         <v>397</v>
       </c>
       <c r="C19">
-        <v>-7.5</v>
+        <v>-0.1</v>
       </c>
       <c r="D19">
         <v>6.5</v>
@@ -5449,7 +5449,7 @@
         <v>397</v>
       </c>
       <c r="C20">
-        <v>-10.1</v>
+        <v>3.1</v>
       </c>
       <c r="D20">
         <v>8.9</v>
@@ -5469,7 +5469,7 @@
         <v>397</v>
       </c>
       <c r="C21">
-        <v>-4.1</v>
+        <v>-5.9</v>
       </c>
       <c r="D21">
         <v>6.3</v>
@@ -5489,7 +5489,7 @@
         <v>397</v>
       </c>
       <c r="C22">
-        <v>-6.5</v>
+        <v>-0.7</v>
       </c>
       <c r="D22">
         <v>7.1</v>
@@ -5509,7 +5509,7 @@
         <v>397</v>
       </c>
       <c r="C23">
-        <v>-7.8</v>
+        <v>41.6</v>
       </c>
       <c r="D23">
         <v>6.8</v>
@@ -5529,7 +5529,7 @@
         <v>397</v>
       </c>
       <c r="C24">
-        <v>2.3</v>
+        <v>-2.2</v>
       </c>
       <c r="D24">
         <v>5.8</v>
@@ -5549,7 +5549,7 @@
         <v>397</v>
       </c>
       <c r="C25">
-        <v>-9.300000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D25">
         <v>5.9</v>
@@ -5569,7 +5569,7 @@
         <v>397</v>
       </c>
       <c r="C26">
-        <v>-7</v>
+        <v>0.6</v>
       </c>
       <c r="D26">
         <v>5.5</v>
@@ -5589,7 +5589,7 @@
         <v>397</v>
       </c>
       <c r="C27">
-        <v>-26.8</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <v>7.6</v>
@@ -5609,7 +5609,7 @@
         <v>397</v>
       </c>
       <c r="C28">
-        <v>-9.699999999999999</v>
+        <v>2.7</v>
       </c>
       <c r="D28">
         <v>8.300000000000001</v>
@@ -5629,7 +5629,7 @@
         <v>397</v>
       </c>
       <c r="C29">
-        <v>-7.6</v>
+        <v>5.1</v>
       </c>
       <c r="D29">
         <v>7.6</v>
@@ -5649,7 +5649,7 @@
         <v>397</v>
       </c>
       <c r="C30">
-        <v>-9.1</v>
+        <v>-0.2</v>
       </c>
       <c r="D30">
         <v>7.8</v>
@@ -5669,7 +5669,7 @@
         <v>397</v>
       </c>
       <c r="C31">
-        <v>-8.5</v>
+        <v>-0.2</v>
       </c>
       <c r="D31">
         <v>6.3</v>
@@ -5689,7 +5689,7 @@
         <v>397</v>
       </c>
       <c r="C32">
-        <v>-20</v>
+        <v>21.8</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -5709,7 +5709,7 @@
         <v>397</v>
       </c>
       <c r="C33">
-        <v>-11.8</v>
+        <v>-1.2</v>
       </c>
       <c r="D33">
         <v>8.300000000000001</v>
@@ -5729,7 +5729,7 @@
         <v>397</v>
       </c>
       <c r="C34">
-        <v>-32.1</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="D34">
         <v>8.199999999999999</v>
@@ -5749,7 +5749,7 @@
         <v>397</v>
       </c>
       <c r="C35">
-        <v>-11.8</v>
+        <v>7.4</v>
       </c>
       <c r="D35">
         <v>8</v>
@@ -5769,7 +5769,7 @@
         <v>397</v>
       </c>
       <c r="C36">
-        <v>-8.699999999999999</v>
+        <v>10.5</v>
       </c>
       <c r="D36">
         <v>7.1</v>
@@ -5789,7 +5789,7 @@
         <v>397</v>
       </c>
       <c r="C37">
-        <v>-7.9</v>
+        <v>3.3</v>
       </c>
       <c r="D37">
         <v>7.7</v>
@@ -5809,7 +5809,7 @@
         <v>397</v>
       </c>
       <c r="C38">
-        <v>-11.2</v>
+        <v>-0.9</v>
       </c>
       <c r="D38">
         <v>7.9</v>
@@ -5829,7 +5829,7 @@
         <v>397</v>
       </c>
       <c r="C39">
-        <v>10.5</v>
+        <v>13.2</v>
       </c>
       <c r="D39">
         <v>6.3</v>
@@ -5849,7 +5849,7 @@
         <v>397</v>
       </c>
       <c r="C40">
-        <v>-11.6</v>
+        <v>2.1</v>
       </c>
       <c r="D40">
         <v>8.199999999999999</v>
@@ -5869,7 +5869,7 @@
         <v>397</v>
       </c>
       <c r="C41">
-        <v>-4</v>
+        <v>0.7</v>
       </c>
       <c r="D41">
         <v>7</v>
@@ -5889,7 +5889,7 @@
         <v>397</v>
       </c>
       <c r="C42">
-        <v>-8.5</v>
+        <v>0.1</v>
       </c>
       <c r="D42">
         <v>7.7</v>
@@ -5909,7 +5909,7 @@
         <v>397</v>
       </c>
       <c r="C43">
-        <v>-11</v>
+        <v>1.4</v>
       </c>
       <c r="D43">
         <v>5.8</v>
@@ -5929,7 +5929,7 @@
         <v>397</v>
       </c>
       <c r="C44">
-        <v>-9.4</v>
+        <v>11.9</v>
       </c>
       <c r="D44">
         <v>8.4</v>
@@ -5949,7 +5949,7 @@
         <v>397</v>
       </c>
       <c r="C45">
-        <v>-8.5</v>
+        <v>1</v>
       </c>
       <c r="D45">
         <v>5.4</v>
@@ -5969,7 +5969,7 @@
         <v>397</v>
       </c>
       <c r="C46">
-        <v>-10.1</v>
+        <v>0.2</v>
       </c>
       <c r="D46">
         <v>8.1</v>
@@ -5989,7 +5989,7 @@
         <v>397</v>
       </c>
       <c r="C47">
-        <v>-12.6</v>
+        <v>3.8</v>
       </c>
       <c r="D47">
         <v>6.9</v>
@@ -6009,7 +6009,7 @@
         <v>397</v>
       </c>
       <c r="C48">
-        <v>-7.5</v>
+        <v>1.3</v>
       </c>
       <c r="D48">
         <v>7.4</v>
@@ -6029,7 +6029,7 @@
         <v>397</v>
       </c>
       <c r="C49">
-        <v>-8.300000000000001</v>
+        <v>-0.1</v>
       </c>
       <c r="D49">
         <v>4.7</v>
@@ -6049,7 +6049,7 @@
         <v>397</v>
       </c>
       <c r="C50">
-        <v>-5.6</v>
+        <v>-8.1</v>
       </c>
       <c r="D50">
         <v>7.7</v>
@@ -6126,7 +6126,7 @@
         <v>31</v>
       </c>
       <c r="C2">
-        <v>-9.300000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="D2">
         <v>6.4</v>
@@ -6146,7 +6146,7 @@
         <v>31</v>
       </c>
       <c r="C3">
-        <v>-7.6</v>
+        <v>6.1</v>
       </c>
       <c r="D3">
         <v>6.9</v>
@@ -6166,7 +6166,7 @@
         <v>31</v>
       </c>
       <c r="C4">
-        <v>-8.5</v>
+        <v>1.4</v>
       </c>
       <c r="D4">
         <v>7.3</v>
@@ -6186,7 +6186,7 @@
         <v>31</v>
       </c>
       <c r="C5">
-        <v>-9.699999999999999</v>
+        <v>-2.3</v>
       </c>
       <c r="D5">
         <v>7.9</v>
@@ -6206,7 +6206,7 @@
         <v>31</v>
       </c>
       <c r="C6">
-        <v>0.6</v>
+        <v>-2.6</v>
       </c>
       <c r="D6">
         <v>7.3</v>
@@ -6226,7 +6226,7 @@
         <v>31</v>
       </c>
       <c r="C7">
-        <v>-8</v>
+        <v>4.8</v>
       </c>
       <c r="D7">
         <v>7.4</v>
@@ -6246,7 +6246,7 @@
         <v>31</v>
       </c>
       <c r="C8">
-        <v>-23.3</v>
+        <v>-0.3</v>
       </c>
       <c r="D8">
         <v>6.3</v>
@@ -6266,7 +6266,7 @@
         <v>31</v>
       </c>
       <c r="C9">
-        <v>-6.4</v>
+        <v>1.8</v>
       </c>
       <c r="D9">
         <v>6.8</v>
@@ -6286,7 +6286,7 @@
         <v>31</v>
       </c>
       <c r="C10">
-        <v>-6.7</v>
+        <v>-2.1</v>
       </c>
       <c r="D10">
         <v>7.6</v>
@@ -6306,7 +6306,7 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>-6.5</v>
+        <v>-0</v>
       </c>
       <c r="D11">
         <v>6.6</v>
@@ -6326,7 +6326,7 @@
         <v>31</v>
       </c>
       <c r="C12">
-        <v>3.3</v>
+        <v>-0.4</v>
       </c>
       <c r="D12">
         <v>6.7</v>
@@ -6346,7 +6346,7 @@
         <v>31</v>
       </c>
       <c r="C13">
-        <v>-15</v>
+        <v>23.5</v>
       </c>
       <c r="D13">
         <v>7.1</v>
@@ -6366,7 +6366,7 @@
         <v>31</v>
       </c>
       <c r="C14">
-        <v>-8.4</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
         <v>8.6</v>
@@ -6386,7 +6386,7 @@
         <v>31</v>
       </c>
       <c r="C15">
-        <v>-7.8</v>
+        <v>0.3</v>
       </c>
       <c r="D15">
         <v>6.9</v>
@@ -6406,7 +6406,7 @@
         <v>31</v>
       </c>
       <c r="C16">
-        <v>-6.2</v>
+        <v>-1</v>
       </c>
       <c r="D16">
         <v>5.1</v>
@@ -6465,7 +6465,7 @@
         <v>432</v>
       </c>
       <c r="C2">
-        <v>-7</v>
+        <v>13.1</v>
       </c>
       <c r="D2">
         <v>8.199999999999999</v>
@@ -6485,7 +6485,7 @@
         <v>432</v>
       </c>
       <c r="C3">
-        <v>-13.1</v>
+        <v>2.9</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -6505,7 +6505,7 @@
         <v>432</v>
       </c>
       <c r="C4">
-        <v>-9.300000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -6525,7 +6525,7 @@
         <v>432</v>
       </c>
       <c r="C5">
-        <v>-12.4</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>2.3</v>
@@ -6545,7 +6545,7 @@
         <v>432</v>
       </c>
       <c r="C6">
-        <v>-8</v>
+        <v>-1</v>
       </c>
       <c r="D6">
         <v>6.7</v>
@@ -6565,7 +6565,7 @@
         <v>432</v>
       </c>
       <c r="C7">
-        <v>-5.5</v>
+        <v>8.4</v>
       </c>
       <c r="D7">
         <v>7.4</v>
@@ -6585,7 +6585,7 @@
         <v>432</v>
       </c>
       <c r="C8">
-        <v>-5.7</v>
+        <v>-3.1</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -6605,7 +6605,7 @@
         <v>432</v>
       </c>
       <c r="C9">
-        <v>-8</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
         <v>8.800000000000001</v>
@@ -6625,7 +6625,7 @@
         <v>432</v>
       </c>
       <c r="C10">
-        <v>-12.3</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D10">
         <v>6.3</v>
@@ -6645,7 +6645,7 @@
         <v>432</v>
       </c>
       <c r="C11">
-        <v>-0.3</v>
+        <v>-1.4</v>
       </c>
       <c r="D11">
         <v>6.2</v>
@@ -6665,7 +6665,7 @@
         <v>432</v>
       </c>
       <c r="C12">
-        <v>-8.6</v>
+        <v>1.1</v>
       </c>
       <c r="D12">
         <v>7.8</v>
@@ -6685,7 +6685,7 @@
         <v>432</v>
       </c>
       <c r="C13">
-        <v>-18.1</v>
+        <v>19.1</v>
       </c>
       <c r="D13">
         <v>6.8</v>
@@ -6745,7 +6745,7 @@
         <v>451</v>
       </c>
       <c r="C2">
-        <v>-12.2</v>
+        <v>16.2</v>
       </c>
       <c r="D2">
         <v>6.8</v>
@@ -6765,7 +6765,7 @@
         <v>451</v>
       </c>
       <c r="C3">
-        <v>-8.300000000000001</v>
+        <v>-0.4</v>
       </c>
       <c r="D3">
         <v>6.6</v>
@@ -6785,7 +6785,7 @@
         <v>451</v>
       </c>
       <c r="C4">
-        <v>-9.199999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="D4">
         <v>7.7</v>
@@ -6805,7 +6805,7 @@
         <v>451</v>
       </c>
       <c r="C5">
-        <v>-5</v>
+        <v>4.5</v>
       </c>
       <c r="D5">
         <v>7.8</v>
@@ -6825,7 +6825,7 @@
         <v>451</v>
       </c>
       <c r="C6">
-        <v>-9.199999999999999</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>8.300000000000001</v>
@@ -6845,7 +6845,7 @@
         <v>451</v>
       </c>
       <c r="C7">
-        <v>-9.4</v>
+        <v>3.3</v>
       </c>
       <c r="D7">
         <v>6.1</v>
@@ -6865,7 +6865,7 @@
         <v>451</v>
       </c>
       <c r="C8">
-        <v>-8.699999999999999</v>
+        <v>6.2</v>
       </c>
       <c r="D8">
         <v>6.9</v>
@@ -6885,7 +6885,7 @@
         <v>451</v>
       </c>
       <c r="C9">
-        <v>-12.4</v>
+        <v>1.2</v>
       </c>
       <c r="D9">
         <v>7.9</v>
@@ -6905,7 +6905,7 @@
         <v>451</v>
       </c>
       <c r="C10">
-        <v>-8.4</v>
+        <v>0.3</v>
       </c>
       <c r="D10">
         <v>8.300000000000001</v>
@@ -6925,7 +6925,7 @@
         <v>451</v>
       </c>
       <c r="C11">
-        <v>-12.3</v>
+        <v>4.5</v>
       </c>
       <c r="D11">
         <v>6.3</v>
@@ -6945,7 +6945,7 @@
         <v>451</v>
       </c>
       <c r="C12">
-        <v>-12.1</v>
+        <v>-1.1</v>
       </c>
       <c r="D12">
         <v>6.1</v>
@@ -6965,7 +6965,7 @@
         <v>451</v>
       </c>
       <c r="C13">
-        <v>-12.2</v>
+        <v>1.5</v>
       </c>
       <c r="D13">
         <v>7.8</v>
@@ -6985,7 +6985,7 @@
         <v>451</v>
       </c>
       <c r="C14">
-        <v>-10.9</v>
+        <v>0.1</v>
       </c>
       <c r="D14">
         <v>7.1</v>
@@ -7043,7 +7043,7 @@
         <v>38</v>
       </c>
       <c r="C2">
-        <v>-62.2</v>
+        <v>-38.7</v>
       </c>
       <c r="D2">
         <v>6.6</v>
@@ -7099,7 +7099,7 @@
         <v>50</v>
       </c>
       <c r="C2">
-        <v>-3.8</v>
+        <v>4.1</v>
       </c>
       <c r="D2">
         <v>4.6</v>
@@ -7119,7 +7119,7 @@
         <v>50</v>
       </c>
       <c r="C3">
-        <v>-8.800000000000001</v>
+        <v>4.3</v>
       </c>
       <c r="D3">
         <v>6.1</v>
@@ -7139,7 +7139,7 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>-19.8</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>5.6</v>
@@ -7159,7 +7159,7 @@
         <v>50</v>
       </c>
       <c r="C5">
-        <v>-7.3</v>
+        <v>1.3</v>
       </c>
       <c r="D5">
         <v>6.8</v>
@@ -7179,7 +7179,7 @@
         <v>50</v>
       </c>
       <c r="C6">
-        <v>-8.800000000000001</v>
+        <v>-4.7</v>
       </c>
       <c r="D6">
         <v>3.8</v>
@@ -7199,7 +7199,7 @@
         <v>50</v>
       </c>
       <c r="C7">
-        <v>-9.1</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
         <v>7.4</v>
@@ -7219,7 +7219,7 @@
         <v>50</v>
       </c>
       <c r="C8">
-        <v>-9.9</v>
+        <v>-3</v>
       </c>
       <c r="D8">
         <v>6.5</v>
@@ -7239,7 +7239,7 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <v>-9.5</v>
+        <v>-4.6</v>
       </c>
       <c r="D9">
         <v>6.4</v>
@@ -7259,7 +7259,7 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>-11.2</v>
+        <v>-10.1</v>
       </c>
       <c r="D10">
         <v>4.7</v>
@@ -7279,7 +7279,7 @@
         <v>50</v>
       </c>
       <c r="C11">
-        <v>-11.5</v>
+        <v>-3.3</v>
       </c>
       <c r="D11">
         <v>6.1</v>
@@ -7338,7 +7338,7 @@
         <v>61</v>
       </c>
       <c r="C2">
-        <v>-12.2</v>
+        <v>4.3</v>
       </c>
       <c r="D2">
         <v>6.6</v>
@@ -7358,7 +7358,7 @@
         <v>61</v>
       </c>
       <c r="C3">
-        <v>-7.8</v>
+        <v>5.5</v>
       </c>
       <c r="D3">
         <v>6.7</v>
@@ -7378,7 +7378,7 @@
         <v>61</v>
       </c>
       <c r="C4">
-        <v>-4.5</v>
+        <v>12.1</v>
       </c>
       <c r="D4">
         <v>7.4</v>
@@ -7398,7 +7398,7 @@
         <v>61</v>
       </c>
       <c r="C5">
-        <v>-8.5</v>
+        <v>0.2</v>
       </c>
       <c r="D5">
         <v>8.1</v>
@@ -7418,7 +7418,7 @@
         <v>61</v>
       </c>
       <c r="C6">
-        <v>-10.9</v>
+        <v>-1.9</v>
       </c>
       <c r="D6">
         <v>6.1</v>
@@ -7438,7 +7438,7 @@
         <v>61</v>
       </c>
       <c r="C7">
-        <v>-9.6</v>
+        <v>-0.8</v>
       </c>
       <c r="D7">
         <v>7.1</v>
@@ -7495,7 +7495,7 @@
         <v>72</v>
       </c>
       <c r="C2">
-        <v>-8.300000000000001</v>
+        <v>-1.2</v>
       </c>
       <c r="D2">
         <v>8.1</v>
@@ -7515,7 +7515,7 @@
         <v>72</v>
       </c>
       <c r="C3">
-        <v>-7.4</v>
+        <v>-5.4</v>
       </c>
       <c r="D3">
         <v>7.1</v>
@@ -7535,7 +7535,7 @@
         <v>72</v>
       </c>
       <c r="C4">
-        <v>-6.5</v>
+        <v>-6.6</v>
       </c>
       <c r="D4">
         <v>4.7</v>
@@ -7555,7 +7555,7 @@
         <v>72</v>
       </c>
       <c r="C5">
-        <v>-6.5</v>
+        <v>-0.6</v>
       </c>
       <c r="D5">
         <v>9.300000000000001</v>
@@ -7575,7 +7575,7 @@
         <v>72</v>
       </c>
       <c r="C6">
-        <v>-10.3</v>
+        <v>-1</v>
       </c>
       <c r="D6">
         <v>5.1</v>
@@ -7595,7 +7595,7 @@
         <v>72</v>
       </c>
       <c r="C7">
-        <v>-5.7</v>
+        <v>5.1</v>
       </c>
       <c r="D7">
         <v>2.4</v>
@@ -7615,7 +7615,7 @@
         <v>72</v>
       </c>
       <c r="C8">
-        <v>-7.6</v>
+        <v>-1.6</v>
       </c>
       <c r="D8">
         <v>7.5</v>
@@ -7635,7 +7635,7 @@
         <v>72</v>
       </c>
       <c r="C9">
-        <v>-15.3</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
         <v>6</v>
@@ -7692,7 +7692,7 @@
         <v>88</v>
       </c>
       <c r="C2">
-        <v>-8.300000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D2">
         <v>8.199999999999999</v>
@@ -7712,7 +7712,7 @@
         <v>88</v>
       </c>
       <c r="C3">
-        <v>-5.8</v>
+        <v>2.4</v>
       </c>
       <c r="D3">
         <v>6</v>
@@ -7732,7 +7732,7 @@
         <v>88</v>
       </c>
       <c r="C4">
-        <v>-11.7</v>
+        <v>1.4</v>
       </c>
       <c r="D4">
         <v>7.4</v>
@@ -7752,7 +7752,7 @@
         <v>88</v>
       </c>
       <c r="C5">
-        <v>-25.1</v>
+        <v>-5.9</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -7772,7 +7772,7 @@
         <v>88</v>
       </c>
       <c r="C6">
-        <v>-13.9</v>
+        <v>3.6</v>
       </c>
       <c r="D6">
         <v>7.8</v>
@@ -7792,7 +7792,7 @@
         <v>88</v>
       </c>
       <c r="C7">
-        <v>-5</v>
+        <v>1.6</v>
       </c>
       <c r="D7">
         <v>6.1</v>
@@ -7812,7 +7812,7 @@
         <v>88</v>
       </c>
       <c r="C8">
-        <v>-6.6</v>
+        <v>1.1</v>
       </c>
       <c r="D8">
         <v>7.8</v>
@@ -7832,7 +7832,7 @@
         <v>88</v>
       </c>
       <c r="C9">
-        <v>-8.800000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="D9">
         <v>6.3</v>
@@ -7852,7 +7852,7 @@
         <v>88</v>
       </c>
       <c r="C10">
-        <v>-10.3</v>
+        <v>0.9</v>
       </c>
       <c r="D10">
         <v>6.4</v>
@@ -7872,7 +7872,7 @@
         <v>88</v>
       </c>
       <c r="C11">
-        <v>-6.7</v>
+        <v>-0.4</v>
       </c>
       <c r="D11">
         <v>7.1</v>
@@ -7892,7 +7892,7 @@
         <v>88</v>
       </c>
       <c r="C12">
-        <v>-7.9</v>
+        <v>0.3</v>
       </c>
       <c r="D12">
         <v>7.4</v>
@@ -7912,7 +7912,7 @@
         <v>88</v>
       </c>
       <c r="C13">
-        <v>-8.9</v>
+        <v>4.3</v>
       </c>
       <c r="D13">
         <v>6.4</v>
@@ -7932,7 +7932,7 @@
         <v>88</v>
       </c>
       <c r="C14">
-        <v>-8.5</v>
+        <v>0.7</v>
       </c>
       <c r="D14">
         <v>5.9</v>
@@ -7996,7 +7996,7 @@
         <v>110</v>
       </c>
       <c r="C2">
-        <v>-9.6</v>
+        <v>-3.7</v>
       </c>
       <c r="D2">
         <v>7.5</v>
@@ -8016,7 +8016,7 @@
         <v>110</v>
       </c>
       <c r="C3">
-        <v>-10.2</v>
+        <v>1.1</v>
       </c>
       <c r="D3">
         <v>5.3</v>
@@ -8036,7 +8036,7 @@
         <v>110</v>
       </c>
       <c r="C4">
-        <v>-9.9</v>
+        <v>4.1</v>
       </c>
       <c r="D4">
         <v>4.8</v>
@@ -8056,7 +8056,7 @@
         <v>110</v>
       </c>
       <c r="C5">
-        <v>-9.6</v>
+        <v>6.5</v>
       </c>
       <c r="D5">
         <v>4.8</v>
@@ -8076,7 +8076,7 @@
         <v>110</v>
       </c>
       <c r="C6">
-        <v>-9.199999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D6">
         <v>5.7</v>
@@ -8096,7 +8096,7 @@
         <v>110</v>
       </c>
       <c r="C7">
-        <v>-12.9</v>
+        <v>2.6</v>
       </c>
       <c r="D7">
         <v>6.5</v>
@@ -8116,7 +8116,7 @@
         <v>110</v>
       </c>
       <c r="C8">
-        <v>-6.9</v>
+        <v>1.5</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -8136,7 +8136,7 @@
         <v>110</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>7.7</v>
       </c>
       <c r="D9">
         <v>6.3</v>
@@ -8156,7 +8156,7 @@
         <v>110</v>
       </c>
       <c r="C10">
-        <v>-8.199999999999999</v>
+        <v>-4.4</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -8176,7 +8176,7 @@
         <v>110</v>
       </c>
       <c r="C11">
-        <v>-7.9</v>
+        <v>5.5</v>
       </c>
       <c r="D11">
         <v>6.2</v>
@@ -8196,7 +8196,7 @@
         <v>110</v>
       </c>
       <c r="C12">
-        <v>-13.4</v>
+        <v>2.8</v>
       </c>
       <c r="D12">
         <v>5.5</v>
@@ -8216,7 +8216,7 @@
         <v>110</v>
       </c>
       <c r="C13">
-        <v>-11.8</v>
+        <v>7.1</v>
       </c>
       <c r="D13">
         <v>5.8</v>
@@ -8274,7 +8274,7 @@
         <v>122</v>
       </c>
       <c r="C2">
-        <v>-10</v>
+        <v>0.4</v>
       </c>
       <c r="D2">
         <v>8.5</v>
@@ -8294,7 +8294,7 @@
         <v>122</v>
       </c>
       <c r="C3">
-        <v>-8.1</v>
+        <v>5.9</v>
       </c>
       <c r="D3">
         <v>7.9</v>
@@ -8314,7 +8314,7 @@
         <v>122</v>
       </c>
       <c r="C4">
-        <v>-6.4</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
         <v>5.9</v>
@@ -8334,7 +8334,7 @@
         <v>122</v>
       </c>
       <c r="C5">
-        <v>-7.3</v>
+        <v>-0.5</v>
       </c>
       <c r="D5">
         <v>6.6</v>
@@ -8354,7 +8354,7 @@
         <v>122</v>
       </c>
       <c r="C6">
-        <v>-8.6</v>
+        <v>1.4</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -8374,7 +8374,7 @@
         <v>122</v>
       </c>
       <c r="C7">
-        <v>-10.4</v>
+        <v>2.1</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -8394,7 +8394,7 @@
         <v>122</v>
       </c>
       <c r="C8">
-        <v>-19.8</v>
+        <v>-0.6</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -8414,7 +8414,7 @@
         <v>122</v>
       </c>
       <c r="C9">
-        <v>-9.800000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="D9">
         <v>7.1</v>

</xml_diff>